<commit_message>
Latest action item status.
</commit_message>
<xml_diff>
--- a/project_management/caArray_caIntegrator_Action_Items.xlsx
+++ b/project_management/caArray_caIntegrator_Action_Items.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-20" yWindow="-20" windowWidth="29600" windowHeight="19000" tabRatio="500"/>
+    <workbookView xWindow="8200" yWindow="-100" windowWidth="25880" windowHeight="19100" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Action_Items" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,21 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="35">
+  <si>
+    <t>In Progress (Need to reschedule caArray demo)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Complete</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Follow up with Doug Hosier on BDA-Lite and AntHill Pro 3.0 requirement.</t>
+  </si>
+  <si>
+    <t>Follow up on CIT Security policy change re: resolution of Medium vulnerabilities of app scan.</t>
+  </si>
   <si>
     <t>Rashmi Srinivasa</t>
   </si>
@@ -72,18 +86,12 @@
     <t>Rashmi Srinivasa and Shine Jacob</t>
   </si>
   <si>
-    <t>In Progress (Meeting with TRANSCEND team on September 14)</t>
-  </si>
-  <si>
     <t>Shine and Rashmi to provide latest product roadmaps to Zhong for the MAT-KC.</t>
   </si>
   <si>
     <t>Shine Jacob and Rashmi Srinivasa</t>
   </si>
   <si>
-    <t>In Progress (caArray roadmap sent)</t>
-  </si>
-  <si>
     <t>Provide TRANSCEND requirements document to JJ.</t>
   </si>
   <si>
@@ -93,9 +101,6 @@
     <t>Talk to the UPT team re: dissuading caArray users from creating groups within UPT.</t>
   </si>
   <si>
-    <t>In Progress (Meeting scheduled for September 14)</t>
-  </si>
-  <si>
     <t>Item #</t>
   </si>
   <si>
@@ -112,12 +117,28 @@
   </si>
   <si>
     <t>Set up a meeting to discuss alternative short-term solutions to the large data set import problem.</t>
+  </si>
+  <si>
+    <t>Eve Shalley</t>
+  </si>
+  <si>
+    <t>In Progress (Eve will send out notes)</t>
+  </si>
+  <si>
+    <t>Complete</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+  </numFmts>
   <fonts count="6">
     <font>
       <sz val="10"/>
@@ -251,7 +272,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -285,6 +306,15 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="5" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -616,10 +646,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
-  <dimension ref="A1:E15"/>
+  <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+      <selection activeCell="D16" sqref="D16:D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -634,19 +664,19 @@
   <sheetData>
     <row r="1" spans="1:5" s="2" customFormat="1" ht="16" thickBot="1">
       <c r="A1" s="5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:5" s="3" customFormat="1" ht="31" thickBot="1">
@@ -654,16 +684,16 @@
         <v>1</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D2" s="9">
         <v>39297</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:5" s="3" customFormat="1" ht="16" thickBot="1">
@@ -671,16 +701,16 @@
         <v>2</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D3" s="9">
         <v>39297</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:5" s="4" customFormat="1" ht="31" thickBot="1">
@@ -688,16 +718,16 @@
         <v>3</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="D4" s="9">
         <v>39297</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="46" thickBot="1">
@@ -705,16 +735,16 @@
         <v>4</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="D5" s="9">
         <v>39297</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="16" thickBot="1">
@@ -722,16 +752,16 @@
         <v>5</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="D6" s="12">
         <v>39297</v>
       </c>
       <c r="E6" s="11" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="31" thickBot="1">
@@ -739,16 +769,16 @@
         <v>6</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="D7" s="9">
         <v>39309</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="31" thickBot="1">
@@ -756,16 +786,16 @@
         <v>7</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D8" s="9">
         <v>39309</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="31" thickBot="1">
@@ -773,16 +803,16 @@
         <v>8</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D9" s="9">
         <v>39309</v>
       </c>
       <c r="E9" s="8" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="31" thickBot="1">
@@ -790,16 +820,16 @@
         <v>9</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="D10" s="9">
         <v>39309</v>
       </c>
       <c r="E10" s="8" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="16" thickBot="1">
@@ -807,16 +837,16 @@
         <v>10</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="C11" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="D11" s="12">
+        <v>19</v>
+      </c>
+      <c r="C11" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="D11" s="14">
         <v>39309</v>
       </c>
-      <c r="E11" s="11" t="s">
-        <v>17</v>
+      <c r="E11" s="15" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="31" thickBot="1">
@@ -824,16 +854,16 @@
         <v>11</v>
       </c>
       <c r="B12" s="11" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C12" s="11" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="D12" s="12">
         <v>39316</v>
       </c>
       <c r="E12" s="11" t="s">
-        <v>20</v>
+        <v>34</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="16" thickBot="1">
@@ -841,16 +871,16 @@
         <v>12</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="D13" s="9">
         <v>39323</v>
       </c>
       <c r="E13" s="8" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="16" thickBot="1">
@@ -858,16 +888,16 @@
         <v>13</v>
       </c>
       <c r="B14" s="11" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C14" s="11" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="D14" s="12">
         <v>39330</v>
       </c>
       <c r="E14" s="11" t="s">
-        <v>8</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="31" thickBot="1">
@@ -875,16 +905,50 @@
         <v>14</v>
       </c>
       <c r="B15" s="11" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C15" s="11" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="D15" s="12">
         <v>39330</v>
       </c>
       <c r="E15" s="11" t="s">
-        <v>24</v>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="16" thickBot="1">
+      <c r="A16" s="10">
+        <v>15</v>
+      </c>
+      <c r="B16" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="C16" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="D16" s="12">
+        <v>39344</v>
+      </c>
+      <c r="E16" s="15" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="16" thickBot="1">
+      <c r="A17" s="10">
+        <v>16</v>
+      </c>
+      <c r="B17" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="C17" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="D17" s="12">
+        <v>39344</v>
+      </c>
+      <c r="E17" s="15" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -895,6 +959,7 @@
   </sortState>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
Latest status of action items.
</commit_message>
<xml_diff>
--- a/project_management/caArray_caIntegrator_Action_Items.xlsx
+++ b/project_management/caArray_caIntegrator_Action_Items.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="8200" yWindow="-100" windowWidth="25880" windowHeight="19100" tabRatio="500"/>
+    <workbookView xWindow="-20" yWindow="-20" windowWidth="29600" windowHeight="19000" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Action_Items" sheetId="1" r:id="rId1"/>
@@ -19,13 +19,17 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="36">
+  <si>
+    <t>Complete (UPT team to prioritize and schedule the 2-3 week effort.)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Complete</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
   <si>
     <t>In Progress (Need to reschedule caArray demo)</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Complete</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
@@ -133,12 +137,6 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-  </numFmts>
   <fonts count="6">
     <font>
       <sz val="10"/>
@@ -649,7 +647,7 @@
   <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16:D17"/>
+      <selection activeCell="A16" sqref="A16:XFD17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -664,19 +662,19 @@
   <sheetData>
     <row r="1" spans="1:5" s="2" customFormat="1" ht="16" thickBot="1">
       <c r="A1" s="5" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:5" s="3" customFormat="1" ht="31" thickBot="1">
@@ -684,16 +682,16 @@
         <v>1</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D2" s="9">
         <v>39297</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:5" s="3" customFormat="1" ht="16" thickBot="1">
@@ -701,16 +699,16 @@
         <v>2</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D3" s="9">
         <v>39297</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:5" s="4" customFormat="1" ht="31" thickBot="1">
@@ -718,16 +716,16 @@
         <v>3</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D4" s="9">
         <v>39297</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="46" thickBot="1">
@@ -735,16 +733,16 @@
         <v>4</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D5" s="9">
         <v>39297</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="16" thickBot="1">
@@ -752,16 +750,16 @@
         <v>5</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D6" s="12">
         <v>39297</v>
       </c>
       <c r="E6" s="11" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="31" thickBot="1">
@@ -769,16 +767,16 @@
         <v>6</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D7" s="9">
         <v>39309</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="31" thickBot="1">
@@ -786,16 +784,16 @@
         <v>7</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D8" s="9">
         <v>39309</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="31" thickBot="1">
@@ -803,16 +801,16 @@
         <v>8</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D9" s="9">
         <v>39309</v>
       </c>
       <c r="E9" s="8" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="31" thickBot="1">
@@ -820,16 +818,16 @@
         <v>9</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D10" s="9">
         <v>39309</v>
       </c>
       <c r="E10" s="8" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="16" thickBot="1">
@@ -837,33 +835,33 @@
         <v>10</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C11" s="13" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D11" s="14">
         <v>39309</v>
       </c>
       <c r="E11" s="15" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="31" thickBot="1">
-      <c r="A12" s="10">
+      <c r="A12" s="7">
         <v>11</v>
       </c>
-      <c r="B12" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="C12" s="11" t="s">
+      <c r="B12" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="D12" s="12">
+      <c r="C12" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D12" s="9">
         <v>39316</v>
       </c>
-      <c r="E12" s="11" t="s">
-        <v>34</v>
+      <c r="E12" s="8" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="16" thickBot="1">
@@ -871,16 +869,16 @@
         <v>12</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D13" s="9">
         <v>39323</v>
       </c>
       <c r="E13" s="8" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="16" thickBot="1">
@@ -888,16 +886,16 @@
         <v>13</v>
       </c>
       <c r="B14" s="11" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C14" s="11" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D14" s="12">
         <v>39330</v>
       </c>
       <c r="E14" s="11" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="31" thickBot="1">
@@ -905,53 +903,54 @@
         <v>14</v>
       </c>
       <c r="B15" s="11" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C15" s="11" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D15" s="12">
         <v>39330</v>
       </c>
       <c r="E15" s="11" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="31" thickBot="1">
+      <c r="A16" s="7">
+        <v>15</v>
+      </c>
+      <c r="B16" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="C16" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D16" s="9">
+        <v>39344</v>
+      </c>
+      <c r="E16" s="8" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="16" thickBot="1">
-      <c r="A16" s="10">
+    <row r="17" spans="1:5" ht="31" thickBot="1">
+      <c r="A17" s="7">
+        <v>16</v>
+      </c>
+      <c r="B17" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C17" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="B16" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="C16" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="D16" s="12">
+      <c r="D17" s="9">
         <v>39344</v>
       </c>
-      <c r="E16" s="15" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" ht="16" thickBot="1">
-      <c r="A17" s="10">
-        <v>16</v>
-      </c>
-      <c r="B17" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="C17" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="D17" s="12">
-        <v>39344</v>
-      </c>
-      <c r="E17" s="15" t="s">
-        <v>12</v>
+      <c r="E17" s="8" t="s">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
+  <sheetCalcPr fullCalcOnLoad="1"/>
   <sortState ref="A2:H13">
     <sortCondition ref="D3:D13"/>
     <sortCondition ref="E3:E13"/>
@@ -959,7 +958,6 @@
   </sortState>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
New action items from Oct 18 meeting.
</commit_message>
<xml_diff>
--- a/project_management/caArray_caIntegrator_Action_Items.xlsx
+++ b/project_management/caArray_caIntegrator_Action_Items.xlsx
@@ -19,7 +19,66 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="43">
+  <si>
+    <t>Talk to the UPT team re: dissuading caArray users from creating groups within UPT.</t>
+  </si>
+  <si>
+    <t>Item #</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Responsible Party</t>
+  </si>
+  <si>
+    <t>Date Identified</t>
+  </si>
+  <si>
+    <t>Disposition</t>
+  </si>
+  <si>
+    <t>Set up a meeting to discuss alternative short-term solutions to the large data set import problem.</t>
+  </si>
+  <si>
+    <t>Upgrade Training tier to caArray 2.4.1.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Upgrade Curation tier to caArray 2.4.1.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Don Swan</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Quy Phung</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Eve Shalley</t>
+  </si>
+  <si>
+    <t>In Progress (Eve will send out notes)</t>
+  </si>
+  <si>
+    <t>Complete</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Create wireframes to depict how permissions will work across caIntegrator and caArray.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Andy Evans and Will Fitzhugh</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Not Started</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
   <si>
     <t>Complete (UPT team to prioritize and schedule the 2-3 week effort.)</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -100,43 +159,18 @@
   </si>
   <si>
     <t>caArray and caIntegrator demos for JJ</t>
-  </si>
-  <si>
-    <t>Talk to the UPT team re: dissuading caArray users from creating groups within UPT.</t>
-  </si>
-  <si>
-    <t>Item #</t>
-  </si>
-  <si>
-    <t>Description</t>
-  </si>
-  <si>
-    <t>Responsible Party</t>
-  </si>
-  <si>
-    <t>Date Identified</t>
-  </si>
-  <si>
-    <t>Disposition</t>
-  </si>
-  <si>
-    <t>Set up a meeting to discuss alternative short-term solutions to the large data set import problem.</t>
-  </si>
-  <si>
-    <t>Eve Shalley</t>
-  </si>
-  <si>
-    <t>In Progress (Eve will send out notes)</t>
-  </si>
-  <si>
-    <t>Complete</t>
-    <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+  </numFmts>
   <fonts count="6">
     <font>
       <sz val="10"/>
@@ -644,10 +678,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
-  <dimension ref="A1:E17"/>
+  <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16:XFD17"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -662,19 +696,19 @@
   <sheetData>
     <row r="1" spans="1:5" s="2" customFormat="1" ht="16" thickBot="1">
       <c r="A1" s="5" t="s">
-        <v>27</v>
+        <v>1</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>28</v>
+        <v>2</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>29</v>
+        <v>3</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>30</v>
+        <v>4</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>31</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:5" s="3" customFormat="1" ht="31" thickBot="1">
@@ -682,16 +716,16 @@
         <v>1</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>32</v>
+        <v>6</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="D2" s="9">
         <v>39297</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>6</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:5" s="3" customFormat="1" ht="16" thickBot="1">
@@ -699,16 +733,16 @@
         <v>2</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>7</v>
+        <v>24</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="D3" s="9">
         <v>39297</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>6</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:5" s="4" customFormat="1" ht="31" thickBot="1">
@@ -716,16 +750,16 @@
         <v>3</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>8</v>
+        <v>25</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>9</v>
+        <v>26</v>
       </c>
       <c r="D4" s="9">
         <v>39297</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>6</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="46" thickBot="1">
@@ -733,16 +767,16 @@
         <v>4</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>10</v>
+        <v>27</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>11</v>
+        <v>28</v>
       </c>
       <c r="D5" s="9">
         <v>39297</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>6</v>
+        <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="16" thickBot="1">
@@ -750,16 +784,16 @@
         <v>5</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>12</v>
+        <v>29</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>9</v>
+        <v>26</v>
       </c>
       <c r="D6" s="12">
         <v>39297</v>
       </c>
       <c r="E6" s="11" t="s">
-        <v>13</v>
+        <v>30</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="31" thickBot="1">
@@ -767,16 +801,16 @@
         <v>6</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>14</v>
+        <v>31</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>15</v>
+        <v>32</v>
       </c>
       <c r="D7" s="9">
         <v>39309</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>6</v>
+        <v>23</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="31" thickBot="1">
@@ -784,16 +818,16 @@
         <v>7</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>16</v>
+        <v>33</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="D8" s="9">
         <v>39309</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>6</v>
+        <v>23</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="31" thickBot="1">
@@ -801,16 +835,16 @@
         <v>8</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>17</v>
+        <v>34</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="D9" s="9">
         <v>39309</v>
       </c>
       <c r="E9" s="8" t="s">
-        <v>6</v>
+        <v>23</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="31" thickBot="1">
@@ -818,16 +852,16 @@
         <v>9</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>18</v>
+        <v>35</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>19</v>
+        <v>36</v>
       </c>
       <c r="D10" s="9">
         <v>39309</v>
       </c>
       <c r="E10" s="8" t="s">
-        <v>6</v>
+        <v>23</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="16" thickBot="1">
@@ -835,16 +869,16 @@
         <v>10</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>20</v>
+        <v>37</v>
       </c>
       <c r="C11" s="13" t="s">
-        <v>33</v>
+        <v>11</v>
       </c>
       <c r="D11" s="14">
         <v>39309</v>
       </c>
       <c r="E11" s="15" t="s">
-        <v>34</v>
+        <v>12</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="31" thickBot="1">
@@ -852,16 +886,16 @@
         <v>11</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>22</v>
+        <v>39</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>23</v>
+        <v>40</v>
       </c>
       <c r="D12" s="9">
         <v>39316</v>
       </c>
       <c r="E12" s="8" t="s">
-        <v>35</v>
+        <v>13</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="16" thickBot="1">
@@ -869,16 +903,16 @@
         <v>12</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>24</v>
+        <v>41</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>9</v>
+        <v>26</v>
       </c>
       <c r="D13" s="9">
         <v>39323</v>
       </c>
       <c r="E13" s="8" t="s">
-        <v>6</v>
+        <v>23</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="16" thickBot="1">
@@ -886,16 +920,16 @@
         <v>13</v>
       </c>
       <c r="B14" s="11" t="s">
-        <v>25</v>
+        <v>42</v>
       </c>
       <c r="C14" s="11" t="s">
-        <v>21</v>
+        <v>38</v>
       </c>
       <c r="D14" s="12">
         <v>39330</v>
       </c>
       <c r="E14" s="11" t="s">
-        <v>2</v>
+        <v>19</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="31" thickBot="1">
@@ -903,16 +937,16 @@
         <v>14</v>
       </c>
       <c r="B15" s="11" t="s">
-        <v>26</v>
+        <v>0</v>
       </c>
       <c r="C15" s="11" t="s">
-        <v>15</v>
+        <v>32</v>
       </c>
       <c r="D15" s="12">
         <v>39330</v>
       </c>
       <c r="E15" s="11" t="s">
-        <v>0</v>
+        <v>17</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="31" thickBot="1">
@@ -920,16 +954,16 @@
         <v>15</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>3</v>
+        <v>20</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>15</v>
+        <v>32</v>
       </c>
       <c r="D16" s="9">
         <v>39344</v>
       </c>
       <c r="E16" s="8" t="s">
-        <v>1</v>
+        <v>18</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="31" thickBot="1">
@@ -937,20 +971,70 @@
         <v>16</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>4</v>
+        <v>21</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>15</v>
+        <v>32</v>
       </c>
       <c r="D17" s="9">
         <v>39344</v>
       </c>
       <c r="E17" s="8" t="s">
-        <v>1</v>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="16" thickBot="1">
+      <c r="A18" s="10">
+        <v>17</v>
+      </c>
+      <c r="B18" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="C18" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="D18" s="12">
+        <v>39372</v>
+      </c>
+      <c r="E18" s="11" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="16" thickBot="1">
+      <c r="A19" s="10">
+        <v>18</v>
+      </c>
+      <c r="B19" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="C19" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="D19" s="12">
+        <v>39372</v>
+      </c>
+      <c r="E19" s="11" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="31" thickBot="1">
+      <c r="A20" s="10">
+        <v>19</v>
+      </c>
+      <c r="B20" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="C20" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="D20" s="12">
+        <v>39372</v>
+      </c>
+      <c r="E20" s="11" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <sortState ref="A2:H13">
     <sortCondition ref="D3:D13"/>
     <sortCondition ref="E3:E13"/>
@@ -958,6 +1042,7 @@
   </sortState>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
Updated after weekly status meeting.
</commit_message>
<xml_diff>
--- a/project_management/caArray_caIntegrator_Action_Items.xlsx
+++ b/project_management/caArray_caIntegrator_Action_Items.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-20" yWindow="-20" windowWidth="29600" windowHeight="19000" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="33440" windowHeight="18920" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Action_Items" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,71 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="55">
+  <si>
+    <t>Mervi Heiskanen</t>
+  </si>
+  <si>
+    <t>Set up a meeting to discuss caGrid 1.2 upgrade</t>
+  </si>
+  <si>
+    <t>Not Started</t>
+  </si>
+  <si>
+    <t>Set up a meeting to discuss access needs to run caArrayImporter client to load data onto caArray on NCI Production server.</t>
+  </si>
+  <si>
+    <t>JJ Pan</t>
+  </si>
+  <si>
+    <t>Write up a short capability description of caArrayImporter client and QTP for loading large data sets.  Quy and Andrew to support.</t>
+  </si>
+  <si>
+    <t>Write up a requirement for autoloader – short term solution using caArrayImporter or QTP.  Xiaopang to provide input.</t>
+  </si>
+  <si>
+    <t>Complete</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>In Progress (UPT team working on it.)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Work with Eve to schedule a meeting with UCSF.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Juli Klemm</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Not Started</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Links to the caArray User’s Guide on the Download Center -&gt; Download page are incorrect</t>
+  </si>
+  <si>
+    <t>Rashmi Srinivasa</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Maureen Colbert</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Create sample experiments in caArray to represent TRANSCEND use cases.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Andy Evans</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Update permissions wireframes for TRANSCEND to reflect the latest understanding of the data.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
   <si>
     <t>Follow up with Rashmi to see if she can help resolve the problem of running the 508 compliance testing tool against caIntegrator.</t>
   </si>
@@ -49,10 +113,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>In Progress (UPT team to prioritize and schedule the 2-3 week effort.)</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>Complete</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -105,9 +165,6 @@
     <t>Eve Shalley</t>
   </si>
   <si>
-    <t>In Progress (Eve will send out notes)</t>
-  </si>
-  <si>
     <t>Complete</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -150,33 +207,18 @@
   </si>
   <si>
     <t>Set up a meeting to discuss which TCGA data types need to be loaded into caIntegrator. Attendees: Tanya Davidson, Xiaopeng, Juli, Mervi, Shine, JP. (Mervi, Shine and JP all have vacation plans during August.)</t>
-  </si>
-  <si>
-    <t>Mervi Heiskanen</t>
-  </si>
-  <si>
-    <t>Set up a meeting to discuss caGrid 1.2 upgrade</t>
-  </si>
-  <si>
-    <t>Not Started</t>
-  </si>
-  <si>
-    <t>Set up a meeting to discuss access needs to run caArrayImporter client to load data onto caArray on NCI Production server.</t>
-  </si>
-  <si>
-    <t>JJ Pan</t>
-  </si>
-  <si>
-    <t>Write up a short capability description of caArrayImporter client and QTP for loading large data sets.  Quy and Andrew to support.</t>
-  </si>
-  <si>
-    <t>Write up a requirement for autoloader – short term solution using caArrayImporter or QTP.  Xiaopang to provide input.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+  </numFmts>
   <fonts count="6">
     <font>
       <sz val="10"/>
@@ -310,7 +352,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -344,15 +386,6 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="5" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="5" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -684,10 +717,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
-  <dimension ref="A1:E20"/>
+  <dimension ref="A1:E24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -702,19 +735,19 @@
   <sheetData>
     <row r="1" spans="1:5" s="2" customFormat="1" ht="16" thickBot="1">
       <c r="A1" s="5" t="s">
-        <v>14</v>
+        <v>31</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>15</v>
+        <v>32</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>16</v>
+        <v>33</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>17</v>
+        <v>34</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>18</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:5" s="3" customFormat="1" ht="31" thickBot="1">
@@ -722,16 +755,16 @@
         <v>1</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>19</v>
+        <v>36</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>33</v>
+        <v>49</v>
       </c>
       <c r="D2" s="9">
         <v>39297</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>34</v>
+        <v>50</v>
       </c>
     </row>
     <row r="3" spans="1:5" s="3" customFormat="1" ht="16" thickBot="1">
@@ -739,16 +772,16 @@
         <v>2</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>35</v>
+        <v>51</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>33</v>
+        <v>49</v>
       </c>
       <c r="D3" s="9">
         <v>39297</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>34</v>
+        <v>50</v>
       </c>
     </row>
     <row r="4" spans="1:5" s="4" customFormat="1" ht="31" thickBot="1">
@@ -756,16 +789,16 @@
         <v>3</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>36</v>
+        <v>52</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>37</v>
+        <v>53</v>
       </c>
       <c r="D4" s="9">
         <v>39297</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>34</v>
+        <v>50</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="46" thickBot="1">
@@ -773,16 +806,16 @@
         <v>4</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>38</v>
+        <v>54</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>39</v>
+        <v>0</v>
       </c>
       <c r="D5" s="9">
         <v>39297</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>34</v>
+        <v>50</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="16" thickBot="1">
@@ -790,16 +823,16 @@
         <v>5</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>40</v>
+        <v>1</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>37</v>
+        <v>53</v>
       </c>
       <c r="D6" s="12">
         <v>39297</v>
       </c>
       <c r="E6" s="11" t="s">
-        <v>41</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="31" thickBot="1">
@@ -807,16 +840,16 @@
         <v>6</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>42</v>
+        <v>3</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>43</v>
+        <v>4</v>
       </c>
       <c r="D7" s="9">
         <v>39309</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>34</v>
+        <v>50</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="31" thickBot="1">
@@ -824,16 +857,16 @@
         <v>7</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>44</v>
+        <v>5</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>33</v>
+        <v>49</v>
       </c>
       <c r="D8" s="9">
         <v>39309</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>34</v>
+        <v>50</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="31" thickBot="1">
@@ -841,16 +874,16 @@
         <v>8</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>45</v>
+        <v>6</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>33</v>
+        <v>49</v>
       </c>
       <c r="D9" s="9">
         <v>39309</v>
       </c>
       <c r="E9" s="8" t="s">
-        <v>34</v>
+        <v>50</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="31" thickBot="1">
@@ -858,33 +891,33 @@
         <v>9</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>1</v>
+        <v>19</v>
       </c>
       <c r="D10" s="9">
         <v>39309</v>
       </c>
       <c r="E10" s="8" t="s">
-        <v>34</v>
+        <v>50</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="16" thickBot="1">
-      <c r="A11" s="10">
+      <c r="A11" s="7">
         <v>10</v>
       </c>
-      <c r="B11" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="C11" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="D11" s="14">
+      <c r="B11" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="D11" s="9">
         <v>39309</v>
       </c>
-      <c r="E11" s="15" t="s">
-        <v>25</v>
+      <c r="E11" s="8" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="31" thickBot="1">
@@ -892,16 +925,16 @@
         <v>11</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>4</v>
+        <v>22</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>5</v>
+        <v>23</v>
       </c>
       <c r="D12" s="9">
         <v>39316</v>
       </c>
       <c r="E12" s="8" t="s">
-        <v>26</v>
+        <v>42</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="16" thickBot="1">
@@ -909,16 +942,16 @@
         <v>12</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>6</v>
+        <v>24</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>37</v>
+        <v>53</v>
       </c>
       <c r="D13" s="9">
         <v>39323</v>
       </c>
       <c r="E13" s="8" t="s">
-        <v>34</v>
+        <v>50</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="16" thickBot="1">
@@ -926,16 +959,16 @@
         <v>13</v>
       </c>
       <c r="B14" s="11" t="s">
-        <v>7</v>
+        <v>25</v>
       </c>
       <c r="C14" s="11" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="D14" s="12">
         <v>39330</v>
       </c>
       <c r="E14" s="11" t="s">
-        <v>30</v>
+        <v>46</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="31" thickBot="1">
@@ -943,16 +976,16 @@
         <v>14</v>
       </c>
       <c r="B15" s="11" t="s">
-        <v>13</v>
+        <v>30</v>
       </c>
       <c r="C15" s="11" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="D15" s="12">
         <v>39330</v>
       </c>
       <c r="E15" s="11" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="31" thickBot="1">
@@ -960,16 +993,16 @@
         <v>15</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>31</v>
+        <v>47</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>43</v>
+        <v>4</v>
       </c>
       <c r="D16" s="9">
         <v>39344</v>
       </c>
       <c r="E16" s="8" t="s">
-        <v>29</v>
+        <v>45</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="31" thickBot="1">
@@ -977,16 +1010,16 @@
         <v>16</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>32</v>
+        <v>48</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>43</v>
+        <v>4</v>
       </c>
       <c r="D17" s="9">
         <v>39344</v>
       </c>
       <c r="E17" s="8" t="s">
-        <v>29</v>
+        <v>45</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="16" thickBot="1">
@@ -994,16 +1027,16 @@
         <v>17</v>
       </c>
       <c r="B18" s="11" t="s">
-        <v>20</v>
+        <v>37</v>
       </c>
       <c r="C18" s="11" t="s">
-        <v>22</v>
+        <v>39</v>
       </c>
       <c r="D18" s="12">
         <v>39372</v>
       </c>
       <c r="E18" s="11" t="s">
-        <v>10</v>
+        <v>27</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="16" thickBot="1">
@@ -1011,16 +1044,16 @@
         <v>18</v>
       </c>
       <c r="B19" s="11" t="s">
-        <v>21</v>
+        <v>38</v>
       </c>
       <c r="C19" s="11" t="s">
-        <v>23</v>
+        <v>40</v>
       </c>
       <c r="D19" s="12">
         <v>39372</v>
       </c>
       <c r="E19" s="11" t="s">
-        <v>11</v>
+        <v>28</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="31" thickBot="1">
@@ -1028,16 +1061,84 @@
         <v>19</v>
       </c>
       <c r="B20" s="11" t="s">
-        <v>27</v>
+        <v>43</v>
       </c>
       <c r="C20" s="11" t="s">
-        <v>28</v>
+        <v>44</v>
       </c>
       <c r="D20" s="12">
         <v>39372</v>
       </c>
       <c r="E20" s="11" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="16" thickBot="1">
+      <c r="A21" s="10">
+        <v>20</v>
+      </c>
+      <c r="B21" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C21" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="D21" s="12">
+        <v>39400</v>
+      </c>
+      <c r="E21" s="11" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="31" thickBot="1">
+      <c r="A22" s="10">
+        <v>21</v>
+      </c>
+      <c r="B22" s="11" t="s">
         <v>12</v>
+      </c>
+      <c r="C22" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="D22" s="12">
+        <v>39400</v>
+      </c>
+      <c r="E22" s="11" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="31" thickBot="1">
+      <c r="A23" s="10">
+        <v>22</v>
+      </c>
+      <c r="B23" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="C23" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="D23" s="12">
+        <v>39400</v>
+      </c>
+      <c r="E23" s="11" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="31" thickBot="1">
+      <c r="A24" s="10">
+        <v>23</v>
+      </c>
+      <c r="B24" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="C24" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="D24" s="12">
+        <v>39400</v>
+      </c>
+      <c r="E24" s="11" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -1048,6 +1149,7 @@
   </sortState>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
Updated Action Items after weekly status meeting.
</commit_message>
<xml_diff>
--- a/project_management/caArray_caIntegrator_Action_Items.xlsx
+++ b/project_management/caArray_caIntegrator_Action_Items.xlsx
@@ -19,7 +19,77 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="58">
+  <si>
+    <t>Update permissions wireframes for TRANSCEND to reflect the latest understanding of the data.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Follow up with Rashmi to see if she can help resolve the problem of running the 508 compliance testing tool against caIntegrator.</t>
+  </si>
+  <si>
+    <t>Quy Phung</t>
+  </si>
+  <si>
+    <t>Tony Kervalage needs list of TRANSCEND requirements and LOE.</t>
+  </si>
+  <si>
+    <t>Rashmi Srinivasa and Shine Jacob</t>
+  </si>
+  <si>
+    <t>Shine and Rashmi to provide latest product roadmaps to Zhong for the MAT-KC.</t>
+  </si>
+  <si>
+    <t>Shine Jacob and Rashmi Srinivasa</t>
+  </si>
+  <si>
+    <t>Provide TRANSCEND requirements document to JJ.</t>
+  </si>
+  <si>
+    <t>caArray and caIntegrator demos for JJ</t>
+  </si>
+  <si>
+    <t>JJ Pan and Larry Brem</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Complete</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Talk to the UPT team re: dissuading caArray users from creating groups within UPT.</t>
+  </si>
+  <si>
+    <t>Item #</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Responsible Party</t>
+  </si>
+  <si>
+    <t>Date Identified</t>
+  </si>
+  <si>
+    <t>Disposition</t>
+  </si>
+  <si>
+    <t>Set up a meeting to discuss alternative short-term solutions to the large data set import problem.</t>
+  </si>
+  <si>
+    <t>Upgrade Training tier to caArray 2.4.1.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Set up regular once-in-2-weeks meetings with TRANSCEND</t>
+  </si>
+  <si>
+    <t>Set up a meeting with the caDSR team to discuss permissible values.</t>
+  </si>
+  <si>
+    <t>Set up an internal meeting to evaluate alternative approaches to setting permissions (common UI versus changes to individual apps)</t>
+  </si>
   <si>
     <t>Upgrade Curation tier to caArray 2.4.1.</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -145,67 +215,6 @@
   </si>
   <si>
     <t>Andy Evans</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Update permissions wireframes for TRANSCEND to reflect the latest understanding of the data.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Follow up with Rashmi to see if she can help resolve the problem of running the 508 compliance testing tool against caIntegrator.</t>
-  </si>
-  <si>
-    <t>Quy Phung</t>
-  </si>
-  <si>
-    <t>Tony Kervalage needs list of TRANSCEND requirements and LOE.</t>
-  </si>
-  <si>
-    <t>Rashmi Srinivasa and Shine Jacob</t>
-  </si>
-  <si>
-    <t>Shine and Rashmi to provide latest product roadmaps to Zhong for the MAT-KC.</t>
-  </si>
-  <si>
-    <t>Shine Jacob and Rashmi Srinivasa</t>
-  </si>
-  <si>
-    <t>Provide TRANSCEND requirements document to JJ.</t>
-  </si>
-  <si>
-    <t>caArray and caIntegrator demos for JJ</t>
-  </si>
-  <si>
-    <t>JJ Pan and Larry Brem</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Complete</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Talk to the UPT team re: dissuading caArray users from creating groups within UPT.</t>
-  </si>
-  <si>
-    <t>Item #</t>
-  </si>
-  <si>
-    <t>Description</t>
-  </si>
-  <si>
-    <t>Responsible Party</t>
-  </si>
-  <si>
-    <t>Date Identified</t>
-  </si>
-  <si>
-    <t>Disposition</t>
-  </si>
-  <si>
-    <t>Set up a meeting to discuss alternative short-term solutions to the large data set import problem.</t>
-  </si>
-  <si>
-    <t>Upgrade Training tier to caArray 2.4.1.</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -346,7 +355,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -380,6 +389,15 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="5" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -711,10 +729,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
-  <dimension ref="A1:E24"/>
+  <dimension ref="A1:E27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+      <selection activeCell="A25" sqref="A25:E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -729,19 +747,19 @@
   <sheetData>
     <row r="1" spans="1:5" s="2" customFormat="1" ht="16" thickBot="1">
       <c r="A1" s="5" t="s">
-        <v>48</v>
+        <v>12</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>49</v>
+        <v>13</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>50</v>
+        <v>14</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>51</v>
+        <v>15</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>52</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:5" s="3" customFormat="1" ht="31" thickBot="1">
@@ -749,16 +767,16 @@
         <v>1</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>53</v>
+        <v>17</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>11</v>
+        <v>33</v>
       </c>
       <c r="D2" s="9">
         <v>39297</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>12</v>
+        <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:5" s="3" customFormat="1" ht="16" thickBot="1">
@@ -766,16 +784,16 @@
         <v>2</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>13</v>
+        <v>35</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>11</v>
+        <v>33</v>
       </c>
       <c r="D3" s="9">
         <v>39297</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>12</v>
+        <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:5" s="4" customFormat="1" ht="31" thickBot="1">
@@ -783,16 +801,16 @@
         <v>3</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>14</v>
+        <v>36</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>15</v>
+        <v>37</v>
       </c>
       <c r="D4" s="9">
         <v>39297</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>12</v>
+        <v>34</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="46" thickBot="1">
@@ -800,16 +818,16 @@
         <v>4</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>16</v>
+        <v>38</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>19</v>
+        <v>41</v>
       </c>
       <c r="D5" s="9">
         <v>39297</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>12</v>
+        <v>34</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="16" thickBot="1">
@@ -817,16 +835,16 @@
         <v>5</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>20</v>
+        <v>42</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>15</v>
+        <v>37</v>
       </c>
       <c r="D6" s="12">
         <v>39297</v>
       </c>
       <c r="E6" s="11" t="s">
-        <v>21</v>
+        <v>43</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="31" thickBot="1">
@@ -834,16 +852,16 @@
         <v>6</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>22</v>
+        <v>44</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>23</v>
+        <v>45</v>
       </c>
       <c r="D7" s="9">
         <v>39309</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>12</v>
+        <v>34</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="31" thickBot="1">
@@ -851,16 +869,16 @@
         <v>7</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>24</v>
+        <v>46</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>11</v>
+        <v>33</v>
       </c>
       <c r="D8" s="9">
         <v>39309</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>12</v>
+        <v>34</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="31" thickBot="1">
@@ -868,16 +886,16 @@
         <v>8</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>25</v>
+        <v>47</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>11</v>
+        <v>33</v>
       </c>
       <c r="D9" s="9">
         <v>39309</v>
       </c>
       <c r="E9" s="8" t="s">
-        <v>12</v>
+        <v>34</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="31" thickBot="1">
@@ -885,16 +903,16 @@
         <v>9</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>37</v>
+        <v>1</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>38</v>
+        <v>2</v>
       </c>
       <c r="D10" s="9">
         <v>39309</v>
       </c>
       <c r="E10" s="8" t="s">
-        <v>12</v>
+        <v>34</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="16" thickBot="1">
@@ -902,16 +920,16 @@
         <v>10</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>39</v>
+        <v>3</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>3</v>
+        <v>25</v>
       </c>
       <c r="D11" s="9">
         <v>39309</v>
       </c>
       <c r="E11" s="8" t="s">
-        <v>26</v>
+        <v>48</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="31" thickBot="1">
@@ -919,16 +937,16 @@
         <v>11</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>41</v>
+        <v>5</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>42</v>
+        <v>6</v>
       </c>
       <c r="D12" s="9">
         <v>39316</v>
       </c>
       <c r="E12" s="8" t="s">
-        <v>4</v>
+        <v>26</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="16" thickBot="1">
@@ -936,16 +954,16 @@
         <v>12</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>43</v>
+        <v>7</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>15</v>
+        <v>37</v>
       </c>
       <c r="D13" s="9">
         <v>39323</v>
       </c>
       <c r="E13" s="8" t="s">
-        <v>12</v>
+        <v>34</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="16" thickBot="1">
@@ -953,16 +971,16 @@
         <v>13</v>
       </c>
       <c r="B14" s="11" t="s">
-        <v>44</v>
+        <v>8</v>
       </c>
       <c r="C14" s="11" t="s">
-        <v>40</v>
+        <v>4</v>
       </c>
       <c r="D14" s="12">
         <v>39330</v>
       </c>
       <c r="E14" s="11" t="s">
-        <v>8</v>
+        <v>30</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="31" thickBot="1">
@@ -970,16 +988,16 @@
         <v>14</v>
       </c>
       <c r="B15" s="11" t="s">
-        <v>47</v>
+        <v>11</v>
       </c>
       <c r="C15" s="11" t="s">
-        <v>45</v>
+        <v>9</v>
       </c>
       <c r="D15" s="12">
         <v>39330</v>
       </c>
       <c r="E15" s="11" t="s">
-        <v>27</v>
+        <v>49</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="31" thickBot="1">
@@ -987,16 +1005,16 @@
         <v>15</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>9</v>
+        <v>31</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>23</v>
+        <v>45</v>
       </c>
       <c r="D16" s="9">
         <v>39344</v>
       </c>
       <c r="E16" s="8" t="s">
-        <v>7</v>
+        <v>29</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="31" thickBot="1">
@@ -1004,16 +1022,16 @@
         <v>16</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>10</v>
+        <v>32</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>23</v>
+        <v>45</v>
       </c>
       <c r="D17" s="9">
         <v>39344</v>
       </c>
       <c r="E17" s="8" t="s">
-        <v>7</v>
+        <v>29</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="16" thickBot="1">
@@ -1021,16 +1039,16 @@
         <v>17</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>54</v>
+        <v>18</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>1</v>
+        <v>23</v>
       </c>
       <c r="D18" s="9">
         <v>39372</v>
       </c>
       <c r="E18" s="8" t="s">
-        <v>46</v>
+        <v>10</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="16" thickBot="1">
@@ -1038,16 +1056,16 @@
         <v>18</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="C19" s="8" t="s">
-        <v>2</v>
+        <v>24</v>
       </c>
       <c r="D19" s="9">
         <v>39372</v>
       </c>
       <c r="E19" s="8" t="s">
-        <v>17</v>
+        <v>39</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="31" thickBot="1">
@@ -1055,16 +1073,16 @@
         <v>19</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>5</v>
+        <v>27</v>
       </c>
       <c r="C20" s="8" t="s">
-        <v>6</v>
+        <v>28</v>
       </c>
       <c r="D20" s="9">
         <v>39372</v>
       </c>
       <c r="E20" s="8" t="s">
-        <v>17</v>
+        <v>39</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="16" thickBot="1">
@@ -1072,16 +1090,16 @@
         <v>20</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>28</v>
+        <v>50</v>
       </c>
       <c r="C21" s="8" t="s">
-        <v>29</v>
+        <v>51</v>
       </c>
       <c r="D21" s="9">
         <v>39400</v>
       </c>
       <c r="E21" s="8" t="s">
-        <v>18</v>
+        <v>40</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="31" thickBot="1">
@@ -1089,16 +1107,16 @@
         <v>21</v>
       </c>
       <c r="B22" s="8" t="s">
-        <v>31</v>
+        <v>53</v>
       </c>
       <c r="C22" s="8" t="s">
-        <v>32</v>
+        <v>54</v>
       </c>
       <c r="D22" s="9">
         <v>39400</v>
       </c>
       <c r="E22" s="8" t="s">
-        <v>18</v>
+        <v>40</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="31" thickBot="1">
@@ -1106,16 +1124,16 @@
         <v>22</v>
       </c>
       <c r="B23" s="8" t="s">
-        <v>34</v>
+        <v>56</v>
       </c>
       <c r="C23" s="8" t="s">
-        <v>33</v>
+        <v>55</v>
       </c>
       <c r="D23" s="9">
         <v>39400</v>
       </c>
       <c r="E23" s="8" t="s">
-        <v>18</v>
+        <v>40</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="31" thickBot="1">
@@ -1123,16 +1141,67 @@
         <v>23</v>
       </c>
       <c r="B24" s="11" t="s">
-        <v>36</v>
+        <v>0</v>
       </c>
       <c r="C24" s="11" t="s">
-        <v>35</v>
+        <v>57</v>
       </c>
       <c r="D24" s="12">
         <v>39400</v>
       </c>
       <c r="E24" s="11" t="s">
-        <v>30</v>
+        <v>52</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="14" thickBot="1">
+      <c r="A25" s="13">
+        <v>24</v>
+      </c>
+      <c r="B25" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="C25" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="D25" s="15">
+        <v>39415</v>
+      </c>
+      <c r="E25" s="14" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="14" thickBot="1">
+      <c r="A26" s="10">
+        <v>25</v>
+      </c>
+      <c r="B26" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="C26" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="D26" s="12">
+        <v>39421</v>
+      </c>
+      <c r="E26" s="11" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="14" thickBot="1">
+      <c r="A27" s="10">
+        <v>26</v>
+      </c>
+      <c r="B27" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="C27" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="D27" s="12">
+        <v>39421</v>
+      </c>
+      <c r="E27" s="11" t="s">
+        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
closed action items marked as complete
</commit_message>
<xml_diff>
--- a/project_management/caArray_caIntegrator_Action_Items.xlsx
+++ b/project_management/caArray_caIntegrator_Action_Items.xlsx
@@ -9,7 +9,7 @@
   <sheets>
     <sheet name="Action_Items" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="130407"/>
+  <calcPr calcId="130407" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:ArchID Flags="2"/>
@@ -19,7 +19,82 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="59">
+  <si>
+    <t>Set up a meeting to discuss which TCGA data types need to be loaded into caIntegrator. Attendees: Tanya Davidson, Xiaopeng, Juli, Mervi, Shine, JP. (Mervi, Shine and JP all have vacation plans during August.)</t>
+  </si>
+  <si>
+    <t>Complete</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Complete</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Mervi Heiskanen</t>
+  </si>
+  <si>
+    <t>Set up a meeting to discuss caGrid 1.2 upgrade</t>
+  </si>
+  <si>
+    <t>Not Started</t>
+  </si>
+  <si>
+    <t>Set up a meeting to discuss access needs to run caArrayImporter client to load data onto caArray on NCI Production server.</t>
+  </si>
+  <si>
+    <t>JJ Pan</t>
+  </si>
+  <si>
+    <t>Write up a short capability description of caArrayImporter client and QTP for loading large data sets.  Quy and Andrew to support.</t>
+  </si>
+  <si>
+    <t>Write up a requirement for autoloader – short term solution using caArrayImporter or QTP.  Xiaopang to provide input.</t>
+  </si>
+  <si>
+    <t>Complete</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>In Progress (UPT team working on it.)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Work with Eve to schedule a meeting with UCSF.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Juli Klemm</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Links to the caArray User’s Guide on the Download Center -&gt; Download page are incorrect</t>
+  </si>
+  <si>
+    <t>Rashmi Srinivasa</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Maureen Colbert</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Create sample experiments in caArray to represent TRANSCEND use cases.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Andy Evans</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Complete</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Complete</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
   <si>
     <t>Update permissions wireframes for TRANSCEND to reflect the latest understanding of the data.</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -145,83 +220,20 @@
   </si>
   <si>
     <t>Shine Jacob</t>
-  </si>
-  <si>
-    <t>Set up a meeting to discuss which TCGA data types need to be loaded into caIntegrator. Attendees: Tanya Davidson, Xiaopeng, Juli, Mervi, Shine, JP. (Mervi, Shine and JP all have vacation plans during August.)</t>
-  </si>
-  <si>
-    <t>Complete</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Complete</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Mervi Heiskanen</t>
-  </si>
-  <si>
-    <t>Set up a meeting to discuss caGrid 1.2 upgrade</t>
-  </si>
-  <si>
-    <t>Not Started</t>
-  </si>
-  <si>
-    <t>Set up a meeting to discuss access needs to run caArrayImporter client to load data onto caArray on NCI Production server.</t>
-  </si>
-  <si>
-    <t>JJ Pan</t>
-  </si>
-  <si>
-    <t>Write up a short capability description of caArrayImporter client and QTP for loading large data sets.  Quy and Andrew to support.</t>
-  </si>
-  <si>
-    <t>Write up a requirement for autoloader – short term solution using caArrayImporter or QTP.  Xiaopang to provide input.</t>
-  </si>
-  <si>
-    <t>Complete</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>In Progress (UPT team working on it.)</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Work with Eve to schedule a meeting with UCSF.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Juli Klemm</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Not Started</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Links to the caArray User’s Guide on the Download Center -&gt; Download page are incorrect</t>
-  </si>
-  <si>
-    <t>Rashmi Srinivasa</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Maureen Colbert</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Create sample experiments in caArray to represent TRANSCEND use cases.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Andy Evans</t>
-    <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="6">
+    <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
+    <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+  </numFmts>
   <fonts count="6">
     <font>
       <sz val="10"/>
@@ -391,13 +403,13 @@
     <xf numFmtId="14" fontId="5" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="5" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="5" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -732,7 +744,7 @@
   <dimension ref="A1:E27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25:E27"/>
+      <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -747,19 +759,19 @@
   <sheetData>
     <row r="1" spans="1:5" s="2" customFormat="1" ht="16" thickBot="1">
       <c r="A1" s="5" t="s">
-        <v>12</v>
+        <v>33</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>13</v>
+        <v>34</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>14</v>
+        <v>35</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>15</v>
+        <v>36</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>16</v>
+        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:5" s="3" customFormat="1" ht="31" thickBot="1">
@@ -767,16 +779,16 @@
         <v>1</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>17</v>
+        <v>38</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>33</v>
+        <v>54</v>
       </c>
       <c r="D2" s="9">
         <v>39297</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>34</v>
+        <v>55</v>
       </c>
     </row>
     <row r="3" spans="1:5" s="3" customFormat="1" ht="16" thickBot="1">
@@ -784,16 +796,16 @@
         <v>2</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>35</v>
+        <v>56</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>33</v>
+        <v>54</v>
       </c>
       <c r="D3" s="9">
         <v>39297</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>34</v>
+        <v>55</v>
       </c>
     </row>
     <row r="4" spans="1:5" s="4" customFormat="1" ht="31" thickBot="1">
@@ -801,16 +813,16 @@
         <v>3</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>36</v>
+        <v>57</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>37</v>
+        <v>58</v>
       </c>
       <c r="D4" s="9">
         <v>39297</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>34</v>
+        <v>55</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="46" thickBot="1">
@@ -818,16 +830,16 @@
         <v>4</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>38</v>
+        <v>0</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>41</v>
+        <v>3</v>
       </c>
       <c r="D5" s="9">
         <v>39297</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>34</v>
+        <v>55</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="16" thickBot="1">
@@ -835,16 +847,16 @@
         <v>5</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>42</v>
+        <v>4</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>37</v>
+        <v>58</v>
       </c>
       <c r="D6" s="12">
         <v>39297</v>
       </c>
       <c r="E6" s="11" t="s">
-        <v>43</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="31" thickBot="1">
@@ -852,16 +864,16 @@
         <v>6</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>44</v>
+        <v>6</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>45</v>
+        <v>7</v>
       </c>
       <c r="D7" s="9">
         <v>39309</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>34</v>
+        <v>55</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="31" thickBot="1">
@@ -869,16 +881,16 @@
         <v>7</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>46</v>
+        <v>8</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>33</v>
+        <v>54</v>
       </c>
       <c r="D8" s="9">
         <v>39309</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>34</v>
+        <v>55</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="31" thickBot="1">
@@ -886,16 +898,16 @@
         <v>8</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>47</v>
+        <v>9</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>33</v>
+        <v>54</v>
       </c>
       <c r="D9" s="9">
         <v>39309</v>
       </c>
       <c r="E9" s="8" t="s">
-        <v>34</v>
+        <v>55</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="31" thickBot="1">
@@ -903,16 +915,16 @@
         <v>9</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>1</v>
+        <v>22</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>2</v>
+        <v>23</v>
       </c>
       <c r="D10" s="9">
         <v>39309</v>
       </c>
       <c r="E10" s="8" t="s">
-        <v>34</v>
+        <v>55</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="16" thickBot="1">
@@ -920,16 +932,16 @@
         <v>10</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>3</v>
+        <v>24</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>25</v>
+        <v>46</v>
       </c>
       <c r="D11" s="9">
         <v>39309</v>
       </c>
       <c r="E11" s="8" t="s">
-        <v>48</v>
+        <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="31" thickBot="1">
@@ -937,16 +949,16 @@
         <v>11</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>5</v>
+        <v>26</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>6</v>
+        <v>27</v>
       </c>
       <c r="D12" s="9">
         <v>39316</v>
       </c>
       <c r="E12" s="8" t="s">
-        <v>26</v>
+        <v>47</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="16" thickBot="1">
@@ -954,16 +966,16 @@
         <v>12</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>7</v>
+        <v>28</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>37</v>
+        <v>58</v>
       </c>
       <c r="D13" s="9">
         <v>39323</v>
       </c>
       <c r="E13" s="8" t="s">
-        <v>34</v>
+        <v>55</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="16" thickBot="1">
@@ -971,16 +983,16 @@
         <v>13</v>
       </c>
       <c r="B14" s="11" t="s">
-        <v>8</v>
+        <v>29</v>
       </c>
       <c r="C14" s="11" t="s">
-        <v>4</v>
+        <v>25</v>
       </c>
       <c r="D14" s="12">
         <v>39330</v>
       </c>
       <c r="E14" s="11" t="s">
-        <v>30</v>
+        <v>51</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="31" thickBot="1">
@@ -988,16 +1000,16 @@
         <v>14</v>
       </c>
       <c r="B15" s="11" t="s">
-        <v>11</v>
+        <v>32</v>
       </c>
       <c r="C15" s="11" t="s">
-        <v>9</v>
+        <v>30</v>
       </c>
       <c r="D15" s="12">
         <v>39330</v>
       </c>
       <c r="E15" s="11" t="s">
-        <v>49</v>
+        <v>11</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="31" thickBot="1">
@@ -1005,16 +1017,16 @@
         <v>15</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>31</v>
+        <v>52</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>45</v>
+        <v>7</v>
       </c>
       <c r="D16" s="9">
         <v>39344</v>
       </c>
       <c r="E16" s="8" t="s">
-        <v>29</v>
+        <v>50</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="31" thickBot="1">
@@ -1022,16 +1034,16 @@
         <v>16</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>32</v>
+        <v>53</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>45</v>
+        <v>7</v>
       </c>
       <c r="D17" s="9">
         <v>39344</v>
       </c>
       <c r="E17" s="8" t="s">
-        <v>29</v>
+        <v>50</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="16" thickBot="1">
@@ -1039,16 +1051,16 @@
         <v>17</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>18</v>
+        <v>39</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>23</v>
+        <v>44</v>
       </c>
       <c r="D18" s="9">
         <v>39372</v>
       </c>
       <c r="E18" s="8" t="s">
-        <v>10</v>
+        <v>31</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="16" thickBot="1">
@@ -1056,16 +1068,16 @@
         <v>18</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>22</v>
+        <v>43</v>
       </c>
       <c r="C19" s="8" t="s">
-        <v>24</v>
+        <v>45</v>
       </c>
       <c r="D19" s="9">
         <v>39372</v>
       </c>
       <c r="E19" s="8" t="s">
-        <v>39</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="31" thickBot="1">
@@ -1073,16 +1085,16 @@
         <v>19</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>27</v>
+        <v>48</v>
       </c>
       <c r="C20" s="8" t="s">
-        <v>28</v>
+        <v>49</v>
       </c>
       <c r="D20" s="9">
         <v>39372</v>
       </c>
       <c r="E20" s="8" t="s">
-        <v>39</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="16" thickBot="1">
@@ -1090,16 +1102,16 @@
         <v>20</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>50</v>
+        <v>12</v>
       </c>
       <c r="C21" s="8" t="s">
-        <v>51</v>
+        <v>13</v>
       </c>
       <c r="D21" s="9">
         <v>39400</v>
       </c>
       <c r="E21" s="8" t="s">
-        <v>40</v>
+        <v>2</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="31" thickBot="1">
@@ -1107,16 +1119,16 @@
         <v>21</v>
       </c>
       <c r="B22" s="8" t="s">
-        <v>53</v>
+        <v>14</v>
       </c>
       <c r="C22" s="8" t="s">
-        <v>54</v>
+        <v>15</v>
       </c>
       <c r="D22" s="9">
         <v>39400</v>
       </c>
       <c r="E22" s="8" t="s">
-        <v>40</v>
+        <v>2</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="31" thickBot="1">
@@ -1124,84 +1136,84 @@
         <v>22</v>
       </c>
       <c r="B23" s="8" t="s">
-        <v>56</v>
+        <v>17</v>
       </c>
       <c r="C23" s="8" t="s">
-        <v>55</v>
+        <v>16</v>
       </c>
       <c r="D23" s="9">
         <v>39400</v>
       </c>
       <c r="E23" s="8" t="s">
-        <v>40</v>
+        <v>2</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="31" thickBot="1">
-      <c r="A24" s="10">
+      <c r="A24" s="7">
         <v>23</v>
       </c>
-      <c r="B24" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="C24" s="11" t="s">
-        <v>57</v>
-      </c>
-      <c r="D24" s="12">
+      <c r="B24" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="C24" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="D24" s="9">
         <v>39400</v>
       </c>
-      <c r="E24" s="11" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" ht="14" thickBot="1">
+      <c r="E24" s="8" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="16" thickBot="1">
       <c r="A25" s="13">
         <v>24</v>
       </c>
       <c r="B25" s="14" t="s">
-        <v>19</v>
+        <v>40</v>
       </c>
       <c r="C25" s="14" t="s">
-        <v>25</v>
+        <v>46</v>
       </c>
       <c r="D25" s="15">
         <v>39415</v>
       </c>
       <c r="E25" s="14" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" ht="14" thickBot="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="16" thickBot="1">
       <c r="A26" s="10">
         <v>25</v>
       </c>
       <c r="B26" s="11" t="s">
-        <v>20</v>
+        <v>41</v>
       </c>
       <c r="C26" s="11" t="s">
-        <v>41</v>
+        <v>3</v>
       </c>
       <c r="D26" s="12">
         <v>39421</v>
       </c>
       <c r="E26" s="11" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" ht="14" thickBot="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="31" thickBot="1">
       <c r="A27" s="10">
         <v>26</v>
       </c>
       <c r="B27" s="11" t="s">
-        <v>21</v>
+        <v>42</v>
       </c>
       <c r="C27" s="11" t="s">
-        <v>33</v>
+        <v>54</v>
       </c>
       <c r="D27" s="12">
         <v>39421</v>
       </c>
       <c r="E27" s="11" t="s">
-        <v>43</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added Agilent custom array design action item.
</commit_message>
<xml_diff>
--- a/project_management/caArray_caIntegrator_Action_Items.xlsx
+++ b/project_management/caArray_caIntegrator_Action_Items.xlsx
@@ -19,7 +19,165 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="74">
+  <si>
+    <t>Mervi Heiskanen</t>
+  </si>
+  <si>
+    <t>On Hold (I-SPY2 data not yet available)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Complete</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>On Hold</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Send the Agilent 415K ADF custom array design to Zhong.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Henry Schaefer</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Not Started</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Shine and Rashmi to provide latest product roadmaps to Zhong for the MAT-KC.</t>
+  </si>
+  <si>
+    <t>Shine Jacob and Rashmi Srinivasa</t>
+  </si>
+  <si>
+    <t>Provide TRANSCEND requirements document to JJ.</t>
+  </si>
+  <si>
+    <t>caArray and caIntegrator demos for JJ</t>
+  </si>
+  <si>
+    <t>JJ Pan and Larry Brem</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Complete</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Talk to the UPT team re: dissuading caArray users from creating groups within UPT.</t>
+  </si>
+  <si>
+    <t>Item #</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Responsible Party</t>
+  </si>
+  <si>
+    <t>Date Identified</t>
+  </si>
+  <si>
+    <t>Disposition</t>
+  </si>
+  <si>
+    <t>Set up a meeting to discuss alternative short-term solutions to the large data set import problem.</t>
+  </si>
+  <si>
+    <t>Upgrade Training tier to caArray 2.4.1.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Set up regular once-in-2-weeks meetings with TRANSCEND</t>
+  </si>
+  <si>
+    <t>Set up a meeting with the caDSR team to discuss permissible values.</t>
+  </si>
+  <si>
+    <t>Set up an internal meeting to evaluate alternative approaches to setting permissions (common UI versus changes to individual apps)</t>
+  </si>
+  <si>
+    <t>Upgrade Curation tier to caArray 2.4.1.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Don Swan</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Quy Phung</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Eve Shalley</t>
+  </si>
+  <si>
+    <t>Complete</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Create wireframes to depict how permissions will work across caIntegrator and caArray.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Andy Evans and Will Fitzhugh</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Complete</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Follow up with Doug Hosier on BDA-Lite and AntHill Pro 3.0 requirement.</t>
+  </si>
+  <si>
+    <t>Follow up on CIT Security policy change re: resolution of Medium vulnerabilities of app scan.</t>
+  </si>
+  <si>
+    <t>Rashmi Srinivasa</t>
+  </si>
+  <si>
+    <t>Complete</t>
+  </si>
+  <si>
+    <t>Send requirements process to JJ and schedule follow-up meeting.</t>
+  </si>
+  <si>
+    <t>Provide a list of TCGA data - loadable/not loadable/unknowns and some options</t>
+  </si>
+  <si>
+    <t>Shine Jacob</t>
+  </si>
+  <si>
+    <t>Complete</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Complete</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Get sample data files from Sarah Davis/TRANSCEND team.</t>
+  </si>
+  <si>
+    <t>Deb Hope to ping Eve Shalley</t>
+  </si>
+  <si>
+    <t>Set up a meeting to discuss which TCGA data types need to be loaded into caIntegrator. Attendees: Tanya Davidson, Xiaopeng, Juli, Mervi, Shine, JP. (Mervi, Shine and JP all have vacation plans during August.)</t>
+  </si>
+  <si>
+    <t>Complete</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Complete</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
   <si>
     <t>Schedule meeting to discuss TRANSCEND architecture recommendations and effect on caArray and caIntegrator project plans.</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -52,10 +210,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>Not Started</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>Complete</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -63,9 +217,6 @@
     <t>Set up a meeting to discuss caGrid 1.2 upgrade</t>
   </si>
   <si>
-    <t>Not Started</t>
-  </si>
-  <si>
     <t>Set up a meeting to discuss access needs to run caArrayImporter client to load data onto caArray on NCI Production server.</t>
   </si>
   <si>
@@ -131,144 +282,6 @@
   </si>
   <si>
     <t>Rashmi Srinivasa and Shine Jacob</t>
-  </si>
-  <si>
-    <t>Shine and Rashmi to provide latest product roadmaps to Zhong for the MAT-KC.</t>
-  </si>
-  <si>
-    <t>Shine Jacob and Rashmi Srinivasa</t>
-  </si>
-  <si>
-    <t>Provide TRANSCEND requirements document to JJ.</t>
-  </si>
-  <si>
-    <t>caArray and caIntegrator demos for JJ</t>
-  </si>
-  <si>
-    <t>JJ Pan and Larry Brem</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Complete</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Talk to the UPT team re: dissuading caArray users from creating groups within UPT.</t>
-  </si>
-  <si>
-    <t>Item #</t>
-  </si>
-  <si>
-    <t>Description</t>
-  </si>
-  <si>
-    <t>Responsible Party</t>
-  </si>
-  <si>
-    <t>In Progress</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Date Identified</t>
-  </si>
-  <si>
-    <t>Disposition</t>
-  </si>
-  <si>
-    <t>Set up a meeting to discuss alternative short-term solutions to the large data set import problem.</t>
-  </si>
-  <si>
-    <t>Upgrade Training tier to caArray 2.4.1.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Set up regular once-in-2-weeks meetings with TRANSCEND</t>
-  </si>
-  <si>
-    <t>Set up a meeting with the caDSR team to discuss permissible values.</t>
-  </si>
-  <si>
-    <t>Set up an internal meeting to evaluate alternative approaches to setting permissions (common UI versus changes to individual apps)</t>
-  </si>
-  <si>
-    <t>Upgrade Curation tier to caArray 2.4.1.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Don Swan</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Quy Phung</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Eve Shalley</t>
-  </si>
-  <si>
-    <t>Complete</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Create wireframes to depict how permissions will work across caIntegrator and caArray.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Andy Evans and Will Fitzhugh</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Complete</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Follow up with Doug Hosier on BDA-Lite and AntHill Pro 3.0 requirement.</t>
-  </si>
-  <si>
-    <t>Follow up on CIT Security policy change re: resolution of Medium vulnerabilities of app scan.</t>
-  </si>
-  <si>
-    <t>Rashmi Srinivasa</t>
-  </si>
-  <si>
-    <t>Complete</t>
-  </si>
-  <si>
-    <t>Send requirements process to JJ and schedule follow-up meeting.</t>
-  </si>
-  <si>
-    <t>Provide a list of TCGA data - loadable/not loadable/unknowns and some options</t>
-  </si>
-  <si>
-    <t>Shine Jacob</t>
-  </si>
-  <si>
-    <t>Complete</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Complete</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Get sample data files from Sarah Davis/TRANSCEND team.</t>
-  </si>
-  <si>
-    <t>Deb Hope to ping Eve Shalley</t>
-  </si>
-  <si>
-    <t>Set up a meeting to discuss which TCGA data types need to be loaded into caIntegrator. Attendees: Tanya Davidson, Xiaopeng, Juli, Mervi, Shine, JP. (Mervi, Shine and JP all have vacation plans during August.)</t>
-  </si>
-  <si>
-    <t>Complete</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Complete</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Mervi Heiskanen</t>
   </si>
 </sst>
 </file>
@@ -335,7 +348,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -408,50 +421,6 @@
       <bottom style="medium">
         <color indexed="62"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="62"/>
-      </left>
-      <right style="medium">
-        <color indexed="62"/>
-      </right>
-      <top style="medium">
-        <color indexed="62"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="62"/>
-      </right>
-      <top style="medium">
-        <color indexed="62"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="62"/>
-      </left>
-      <right style="medium">
-        <color indexed="62"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="62"/>
-      </right>
-      <top/>
-      <bottom/>
       <diagonal/>
     </border>
   </borders>
@@ -844,10 +813,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
-  <dimension ref="A1:E31"/>
+  <dimension ref="A1:E32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -862,19 +831,19 @@
   <sheetData>
     <row r="1" spans="1:5" s="2" customFormat="1" ht="16" thickBot="1">
       <c r="A1" s="5" t="s">
-        <v>37</v>
+        <v>14</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>38</v>
+        <v>15</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>39</v>
+        <v>16</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>41</v>
+        <v>17</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>42</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:5" s="3" customFormat="1" ht="31" thickBot="1">
@@ -882,16 +851,16 @@
         <v>1</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>43</v>
+        <v>19</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>58</v>
+        <v>34</v>
       </c>
       <c r="D2" s="9">
         <v>39297</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>59</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:5" s="3" customFormat="1" ht="16" thickBot="1">
@@ -899,16 +868,16 @@
         <v>2</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>60</v>
+        <v>36</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>58</v>
+        <v>34</v>
       </c>
       <c r="D3" s="9">
         <v>39297</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>59</v>
+        <v>35</v>
       </c>
     </row>
     <row r="4" spans="1:5" s="4" customFormat="1" ht="31" thickBot="1">
@@ -916,16 +885,16 @@
         <v>3</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>61</v>
+        <v>37</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>62</v>
+        <v>38</v>
       </c>
       <c r="D4" s="9">
         <v>39297</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>59</v>
+        <v>35</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="46" thickBot="1">
@@ -933,16 +902,16 @@
         <v>4</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>67</v>
+        <v>43</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>70</v>
+        <v>0</v>
       </c>
       <c r="D5" s="9">
         <v>39297</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>59</v>
+        <v>35</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="16" thickBot="1">
@@ -950,16 +919,16 @@
         <v>5</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>9</v>
+        <v>54</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>62</v>
+        <v>38</v>
       </c>
       <c r="D6" s="12">
         <v>39297</v>
       </c>
       <c r="E6" s="11" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="31" thickBot="1">
@@ -967,16 +936,16 @@
         <v>6</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>11</v>
+        <v>55</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>12</v>
+        <v>56</v>
       </c>
       <c r="D7" s="9">
         <v>39309</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>59</v>
+        <v>35</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="31" thickBot="1">
@@ -984,16 +953,16 @@
         <v>7</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>13</v>
+        <v>57</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>58</v>
+        <v>34</v>
       </c>
       <c r="D8" s="9">
         <v>39309</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>59</v>
+        <v>35</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="31" thickBot="1">
@@ -1001,16 +970,16 @@
         <v>8</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>14</v>
+        <v>58</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>58</v>
+        <v>34</v>
       </c>
       <c r="D9" s="9">
         <v>39309</v>
       </c>
       <c r="E9" s="8" t="s">
-        <v>59</v>
+        <v>35</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="31" thickBot="1">
@@ -1018,16 +987,16 @@
         <v>9</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>26</v>
+        <v>70</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>27</v>
+        <v>71</v>
       </c>
       <c r="D10" s="9">
         <v>39309</v>
       </c>
       <c r="E10" s="8" t="s">
-        <v>59</v>
+        <v>35</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="16" thickBot="1">
@@ -1035,16 +1004,16 @@
         <v>10</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>28</v>
+        <v>72</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>51</v>
+        <v>27</v>
       </c>
       <c r="D11" s="9">
         <v>39309</v>
       </c>
       <c r="E11" s="8" t="s">
-        <v>15</v>
+        <v>59</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="31" thickBot="1">
@@ -1052,16 +1021,16 @@
         <v>11</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>30</v>
+        <v>7</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>31</v>
+        <v>8</v>
       </c>
       <c r="D12" s="9">
         <v>39316</v>
       </c>
       <c r="E12" s="8" t="s">
-        <v>52</v>
+        <v>28</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="16" thickBot="1">
@@ -1069,16 +1038,16 @@
         <v>12</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>32</v>
+        <v>9</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>62</v>
+        <v>38</v>
       </c>
       <c r="D13" s="9">
         <v>39323</v>
       </c>
       <c r="E13" s="8" t="s">
-        <v>59</v>
+        <v>35</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="16" thickBot="1">
@@ -1086,16 +1055,16 @@
         <v>13</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>33</v>
+        <v>10</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>29</v>
+        <v>73</v>
       </c>
       <c r="D14" s="9">
         <v>39330</v>
       </c>
       <c r="E14" s="8" t="s">
-        <v>63</v>
+        <v>39</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="31" thickBot="1">
@@ -1103,16 +1072,16 @@
         <v>14</v>
       </c>
       <c r="B15" s="14" t="s">
-        <v>36</v>
+        <v>13</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>34</v>
+        <v>11</v>
       </c>
       <c r="D15" s="15">
         <v>39330</v>
       </c>
       <c r="E15" s="14" t="s">
-        <v>8</v>
+        <v>53</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="31" thickBot="1">
@@ -1120,16 +1089,16 @@
         <v>15</v>
       </c>
       <c r="B16" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="C16" s="8" t="s">
         <v>56</v>
-      </c>
-      <c r="C16" s="8" t="s">
-        <v>12</v>
       </c>
       <c r="D16" s="9">
         <v>39344</v>
       </c>
       <c r="E16" s="8" t="s">
-        <v>55</v>
+        <v>31</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="31" thickBot="1">
@@ -1137,16 +1106,16 @@
         <v>16</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>57</v>
+        <v>33</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>12</v>
+        <v>56</v>
       </c>
       <c r="D17" s="9">
         <v>39344</v>
       </c>
       <c r="E17" s="8" t="s">
-        <v>55</v>
+        <v>31</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="16" thickBot="1">
@@ -1154,16 +1123,16 @@
         <v>17</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>44</v>
+        <v>20</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>49</v>
+        <v>25</v>
       </c>
       <c r="D18" s="9">
         <v>39372</v>
       </c>
       <c r="E18" s="8" t="s">
-        <v>35</v>
+        <v>12</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="16" thickBot="1">
@@ -1171,16 +1140,16 @@
         <v>18</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>48</v>
+        <v>24</v>
       </c>
       <c r="C19" s="8" t="s">
-        <v>50</v>
+        <v>26</v>
       </c>
       <c r="D19" s="9">
         <v>39372</v>
       </c>
       <c r="E19" s="8" t="s">
-        <v>68</v>
+        <v>44</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="31" thickBot="1">
@@ -1188,16 +1157,16 @@
         <v>19</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>53</v>
+        <v>29</v>
       </c>
       <c r="C20" s="8" t="s">
-        <v>54</v>
+        <v>30</v>
       </c>
       <c r="D20" s="9">
         <v>39372</v>
       </c>
       <c r="E20" s="8" t="s">
-        <v>68</v>
+        <v>44</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="16" thickBot="1">
@@ -1205,16 +1174,16 @@
         <v>20</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>16</v>
+        <v>60</v>
       </c>
       <c r="C21" s="8" t="s">
-        <v>17</v>
+        <v>61</v>
       </c>
       <c r="D21" s="9">
         <v>39400</v>
       </c>
       <c r="E21" s="8" t="s">
-        <v>69</v>
+        <v>45</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="31" thickBot="1">
@@ -1222,16 +1191,16 @@
         <v>21</v>
       </c>
       <c r="B22" s="8" t="s">
-        <v>18</v>
+        <v>62</v>
       </c>
       <c r="C22" s="8" t="s">
-        <v>19</v>
+        <v>63</v>
       </c>
       <c r="D22" s="9">
         <v>39400</v>
       </c>
       <c r="E22" s="8" t="s">
-        <v>69</v>
+        <v>45</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="31" thickBot="1">
@@ -1239,16 +1208,16 @@
         <v>22</v>
       </c>
       <c r="B23" s="8" t="s">
-        <v>21</v>
+        <v>65</v>
       </c>
       <c r="C23" s="8" t="s">
-        <v>20</v>
+        <v>64</v>
       </c>
       <c r="D23" s="9">
         <v>39400</v>
       </c>
       <c r="E23" s="8" t="s">
-        <v>69</v>
+        <v>45</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="31" thickBot="1">
@@ -1256,16 +1225,16 @@
         <v>23</v>
       </c>
       <c r="B24" s="8" t="s">
-        <v>25</v>
+        <v>69</v>
       </c>
       <c r="C24" s="8" t="s">
-        <v>22</v>
+        <v>66</v>
       </c>
       <c r="D24" s="9">
         <v>39400</v>
       </c>
       <c r="E24" s="8" t="s">
-        <v>23</v>
+        <v>67</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="16" thickBot="1">
@@ -1273,16 +1242,16 @@
         <v>24</v>
       </c>
       <c r="B25" s="14" t="s">
-        <v>45</v>
+        <v>21</v>
       </c>
       <c r="C25" s="14" t="s">
-        <v>51</v>
+        <v>27</v>
       </c>
       <c r="D25" s="15">
         <v>39415</v>
       </c>
       <c r="E25" s="14" t="s">
-        <v>24</v>
+        <v>68</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="16" thickBot="1">
@@ -1290,16 +1259,16 @@
         <v>25</v>
       </c>
       <c r="B26" s="14" t="s">
-        <v>46</v>
+        <v>22</v>
       </c>
       <c r="C26" s="14" t="s">
-        <v>70</v>
+        <v>0</v>
       </c>
       <c r="D26" s="15">
         <v>39421</v>
       </c>
       <c r="E26" s="14" t="s">
-        <v>64</v>
+        <v>40</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="31" thickBot="1">
@@ -1307,16 +1276,16 @@
         <v>26</v>
       </c>
       <c r="B27" s="14" t="s">
-        <v>47</v>
+        <v>23</v>
       </c>
       <c r="C27" s="14" t="s">
-        <v>58</v>
+        <v>34</v>
       </c>
       <c r="D27" s="15">
         <v>39421</v>
       </c>
       <c r="E27" s="14" t="s">
-        <v>64</v>
+        <v>40</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="16" thickBot="1">
@@ -1324,16 +1293,16 @@
         <v>27</v>
       </c>
       <c r="B28" s="16" t="s">
-        <v>65</v>
+        <v>41</v>
       </c>
       <c r="C28" s="17" t="s">
-        <v>66</v>
+        <v>42</v>
       </c>
       <c r="D28" s="18">
         <v>39470</v>
       </c>
       <c r="E28" s="17" t="s">
-        <v>40</v>
+        <v>1</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="91" thickBot="1">
@@ -1341,50 +1310,67 @@
         <v>28</v>
       </c>
       <c r="B29" s="14" t="s">
-        <v>2</v>
+        <v>48</v>
       </c>
       <c r="C29" s="14" t="s">
-        <v>3</v>
+        <v>49</v>
       </c>
       <c r="D29" s="15">
         <v>39470</v>
       </c>
       <c r="E29" s="14" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="31" thickBot="1">
+      <c r="A30" s="13">
+        <v>29</v>
+      </c>
+      <c r="B30" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="C30" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="D30" s="15">
+        <v>39477</v>
+      </c>
+      <c r="E30" s="14" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="46" thickBot="1">
+      <c r="A31" s="13">
+        <v>30</v>
+      </c>
+      <c r="B31" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="C31" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="D31" s="15">
+        <v>39477</v>
+      </c>
+      <c r="E31" s="14" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="16" thickBot="1">
+      <c r="A32" s="19">
+        <v>31</v>
+      </c>
+      <c r="B32" s="16" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" ht="31" thickBot="1">
-      <c r="A30" s="19">
-        <v>29</v>
-      </c>
-      <c r="B30" s="16" t="s">
+      <c r="C32" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="C30" s="17" t="s">
+      <c r="D32" s="18">
+        <v>39491</v>
+      </c>
+      <c r="E32" s="17" t="s">
         <v>6</v>
-      </c>
-      <c r="D30" s="18">
-        <v>39477</v>
-      </c>
-      <c r="E30" s="17" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" ht="46" thickBot="1">
-      <c r="A31" s="19">
-        <v>30</v>
-      </c>
-      <c r="B31" s="16" t="s">
-        <v>0</v>
-      </c>
-      <c r="C31" s="17" t="s">
-        <v>1</v>
-      </c>
-      <c r="D31" s="18">
-        <v>39477</v>
-      </c>
-      <c r="E31" s="17" t="s">
-        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated Action Items list with new TODOs.
</commit_message>
<xml_diff>
--- a/project_management/caArray_caIntegrator_Action_Items.xlsx
+++ b/project_management/caArray_caIntegrator_Action_Items.xlsx
@@ -19,157 +19,39 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="74">
-  <si>
-    <t>Provide a list of TCGA data - loadable/not loadable/unknowns and some options</t>
-  </si>
-  <si>
-    <t>Shine Jacob</t>
-  </si>
-  <si>
-    <t>Complete</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Complete</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Get sample data files from Sarah Davis/TRANSCEND team.</t>
-  </si>
-  <si>
-    <t>Deb Hope to ping Eve Shalley</t>
-  </si>
-  <si>
-    <t>Create sample experiments in caArray to represent TRANSCEND use cases.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Andy Evans</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Complete</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Complete</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Update permissions wireframes for TRANSCEND to reflect the latest understanding of the data.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Mervi Heiskanen</t>
-  </si>
-  <si>
-    <t>On Hold (I-SPY2 data not yet available)</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Complete</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>On Hold</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Send the Agilent 415K ADF custom array design to Zhong.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Henry Schaefer</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Shine and Rashmi to provide latest product roadmaps to Zhong for the MAT-KC.</t>
-  </si>
-  <si>
-    <t>Shine Jacob and Rashmi Srinivasa</t>
-  </si>
-  <si>
-    <t>Provide TRANSCEND requirements document to JJ.</t>
-  </si>
-  <si>
-    <t>caArray and caIntegrator demos for JJ</t>
-  </si>
-  <si>
-    <t>JJ Pan and Larry Brem</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Complete</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Talk to the UPT team re: dissuading caArray users from creating groups within UPT.</t>
-  </si>
-  <si>
-    <t>Item #</t>
-  </si>
-  <si>
-    <t>Description</t>
-  </si>
-  <si>
-    <t>Responsible Party</t>
-  </si>
-  <si>
-    <t>Date Identified</t>
-  </si>
-  <si>
-    <t>Disposition</t>
-  </si>
-  <si>
-    <t>Set up a meeting to discuss alternative short-term solutions to the large data set import problem.</t>
-  </si>
-  <si>
-    <t>Upgrade Training tier to caArray 2.4.1.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Set up regular once-in-2-weeks meetings with TRANSCEND</t>
-  </si>
-  <si>
-    <t>Set up a meeting with the caDSR team to discuss permissible values.</t>
-  </si>
-  <si>
-    <t>Set up an internal meeting to evaluate alternative approaches to setting permissions (common UI versus changes to individual apps)</t>
-  </si>
-  <si>
-    <t>Upgrade Curation tier to caArray 2.4.1.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Don Swan</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Quy Phung</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Eve Shalley</t>
-  </si>
-  <si>
-    <t>Complete</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Create wireframes to depict how permissions will work across caIntegrator and caArray.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Andy Evans and Will Fitzhugh</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Complete</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Follow up with Doug Hosier on BDA-Lite and AntHill Pro 3.0 requirement.</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="80">
+  <si>
+    <t>Juli Klemm</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Links to the caArray User’s Guide on the Download Center -&gt; Download page are incorrect</t>
+  </si>
+  <si>
+    <t>Rashmi Srinivasa</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Maureen Colbert</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Send triaged bug list to Juli, JJ, Deb and Larry and schedule a second Bug Triage meeting.</t>
+  </si>
+  <si>
+    <t>Submit ticket for BDALite configuration on the new STAGE tier</t>
+  </si>
+  <si>
+    <t>Discuss need for disaster recovery / backup server solution</t>
+  </si>
+  <si>
+    <t>Juli Klemm and JJ Pan</t>
+  </si>
+  <si>
+    <t>Not Started</t>
+  </si>
+  <si>
+    <t>Forward information re: dependency on EVS</t>
   </si>
   <si>
     <t>Follow up on CIT Security policy change re: resolution of Medium vulnerabilities of app scan.</t>
@@ -269,19 +151,155 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>Juli Klemm</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Links to the caArray User’s Guide on the Download Center -&gt; Download page are incorrect</t>
-  </si>
-  <si>
-    <t>Rashmi Srinivasa</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Maureen Colbert</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <t>Provide a list of TCGA data - loadable/not loadable/unknowns and some options</t>
+  </si>
+  <si>
+    <t>Shine Jacob</t>
+  </si>
+  <si>
+    <t>Complete</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Complete</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Get sample data files from Sarah Davis/TRANSCEND team.</t>
+  </si>
+  <si>
+    <t>Deb Hope to ping Eve Shalley</t>
+  </si>
+  <si>
+    <t>Create sample experiments in caArray to represent TRANSCEND use cases.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Andy Evans</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Complete</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Complete</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Update permissions wireframes for TRANSCEND to reflect the latest understanding of the data.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Mervi Heiskanen</t>
+  </si>
+  <si>
+    <t>On Hold (I-SPY2 data not yet available)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Complete</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>On Hold</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Send the Agilent 415K ADF custom array design to Zhong.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Henry Schaefer</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Shine and Rashmi to provide latest product roadmaps to Zhong for the MAT-KC.</t>
+  </si>
+  <si>
+    <t>Shine Jacob and Rashmi Srinivasa</t>
+  </si>
+  <si>
+    <t>Provide TRANSCEND requirements document to JJ.</t>
+  </si>
+  <si>
+    <t>caArray and caIntegrator demos for JJ</t>
+  </si>
+  <si>
+    <t>JJ Pan and Larry Brem</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Complete</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Talk to the UPT team re: dissuading caArray users from creating groups within UPT.</t>
+  </si>
+  <si>
+    <t>Item #</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Responsible Party</t>
+  </si>
+  <si>
+    <t>Date Identified</t>
+  </si>
+  <si>
+    <t>Disposition</t>
+  </si>
+  <si>
+    <t>Set up a meeting to discuss alternative short-term solutions to the large data set import problem.</t>
+  </si>
+  <si>
+    <t>Upgrade Training tier to caArray 2.4.1.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Set up regular once-in-2-weeks meetings with TRANSCEND</t>
+  </si>
+  <si>
+    <t>Set up a meeting with the caDSR team to discuss permissible values.</t>
+  </si>
+  <si>
+    <t>Set up an internal meeting to evaluate alternative approaches to setting permissions (common UI versus changes to individual apps)</t>
+  </si>
+  <si>
+    <t>Upgrade Curation tier to caArray 2.4.1.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Don Swan</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Quy Phung</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Eve Shalley</t>
+  </si>
+  <si>
+    <t>Complete</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Create wireframes to depict how permissions will work across caIntegrator and caArray.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Andy Evans and Will Fitzhugh</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Complete</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Follow up with Doug Hosier on BDA-Lite and AntHill Pro 3.0 requirement.</t>
   </si>
 </sst>
 </file>
@@ -779,10 +797,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
-  <dimension ref="A1:E32"/>
+  <dimension ref="A1:E36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="A36" sqref="A36:XFD36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -797,19 +815,19 @@
   <sheetData>
     <row r="1" spans="1:5" s="2" customFormat="1" ht="16" thickBot="1">
       <c r="A1" s="3" t="s">
-        <v>24</v>
+        <v>61</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>25</v>
+        <v>62</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>26</v>
+        <v>63</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>27</v>
+        <v>64</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>28</v>
+        <v>65</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="31" thickBot="1">
@@ -817,16 +835,16 @@
         <v>1</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>29</v>
+        <v>66</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>44</v>
+        <v>11</v>
       </c>
       <c r="D2" s="7">
         <v>39297</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>45</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="16" thickBot="1">
@@ -834,16 +852,16 @@
         <v>2</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>46</v>
+        <v>13</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>44</v>
+        <v>11</v>
       </c>
       <c r="D3" s="7">
         <v>39297</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>45</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="31" thickBot="1">
@@ -851,16 +869,16 @@
         <v>3</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>0</v>
+        <v>37</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>1</v>
+        <v>38</v>
       </c>
       <c r="D4" s="7">
         <v>39297</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>45</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="46" thickBot="1">
@@ -868,16 +886,16 @@
         <v>4</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>52</v>
+        <v>19</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>11</v>
+        <v>48</v>
       </c>
       <c r="D5" s="7">
         <v>39297</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>45</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="16" thickBot="1">
@@ -885,16 +903,16 @@
         <v>5</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>63</v>
+        <v>30</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>1</v>
+        <v>38</v>
       </c>
       <c r="D6" s="10">
         <v>39297</v>
       </c>
       <c r="E6" s="9" t="s">
-        <v>14</v>
+        <v>51</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="31" thickBot="1">
@@ -902,16 +920,16 @@
         <v>6</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>64</v>
+        <v>31</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>65</v>
+        <v>32</v>
       </c>
       <c r="D7" s="7">
         <v>39309</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>45</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="31" thickBot="1">
@@ -919,16 +937,16 @@
         <v>7</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>66</v>
+        <v>33</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>44</v>
+        <v>11</v>
       </c>
       <c r="D8" s="7">
         <v>39309</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>45</v>
+        <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="31" thickBot="1">
@@ -936,16 +954,16 @@
         <v>8</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>67</v>
+        <v>34</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>44</v>
+        <v>11</v>
       </c>
       <c r="D9" s="7">
         <v>39309</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>45</v>
+        <v>12</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="31" thickBot="1">
@@ -953,16 +971,16 @@
         <v>9</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>47</v>
+        <v>14</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>48</v>
+        <v>15</v>
       </c>
       <c r="D10" s="7">
         <v>39309</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>45</v>
+        <v>12</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="16" thickBot="1">
@@ -970,16 +988,16 @@
         <v>10</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>49</v>
+        <v>16</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>37</v>
+        <v>74</v>
       </c>
       <c r="D11" s="7">
         <v>39309</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>68</v>
+        <v>35</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="31" thickBot="1">
@@ -987,16 +1005,16 @@
         <v>11</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>17</v>
+        <v>54</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>18</v>
+        <v>55</v>
       </c>
       <c r="D12" s="7">
         <v>39316</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>38</v>
+        <v>75</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="16" thickBot="1">
@@ -1004,16 +1022,16 @@
         <v>12</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>19</v>
+        <v>56</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>1</v>
+        <v>38</v>
       </c>
       <c r="D13" s="7">
         <v>39323</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>45</v>
+        <v>12</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="16" thickBot="1">
@@ -1021,16 +1039,16 @@
         <v>13</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>20</v>
+        <v>57</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>50</v>
+        <v>17</v>
       </c>
       <c r="D14" s="7">
         <v>39330</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>2</v>
+        <v>39</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="31" thickBot="1">
@@ -1038,16 +1056,16 @@
         <v>14</v>
       </c>
       <c r="B15" s="12" t="s">
-        <v>23</v>
+        <v>60</v>
       </c>
       <c r="C15" s="12" t="s">
-        <v>21</v>
+        <v>58</v>
       </c>
       <c r="D15" s="13">
         <v>39330</v>
       </c>
       <c r="E15" s="12" t="s">
-        <v>62</v>
+        <v>29</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="31" thickBot="1">
@@ -1055,16 +1073,16 @@
         <v>15</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>42</v>
+        <v>79</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>65</v>
+        <v>32</v>
       </c>
       <c r="D16" s="7">
         <v>39344</v>
       </c>
       <c r="E16" s="6" t="s">
-        <v>41</v>
+        <v>78</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="31" thickBot="1">
@@ -1072,16 +1090,16 @@
         <v>16</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>43</v>
+        <v>10</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>65</v>
+        <v>32</v>
       </c>
       <c r="D17" s="7">
         <v>39344</v>
       </c>
       <c r="E17" s="6" t="s">
-        <v>41</v>
+        <v>78</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="16" thickBot="1">
@@ -1089,16 +1107,16 @@
         <v>17</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>30</v>
+        <v>67</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>35</v>
+        <v>72</v>
       </c>
       <c r="D18" s="7">
         <v>39372</v>
       </c>
       <c r="E18" s="6" t="s">
-        <v>22</v>
+        <v>59</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="16" thickBot="1">
@@ -1106,16 +1124,16 @@
         <v>18</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>34</v>
+        <v>71</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>36</v>
+        <v>73</v>
       </c>
       <c r="D19" s="7">
         <v>39372</v>
       </c>
       <c r="E19" s="6" t="s">
-        <v>53</v>
+        <v>20</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="31" thickBot="1">
@@ -1123,16 +1141,16 @@
         <v>19</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>39</v>
+        <v>76</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="D20" s="7">
         <v>39372</v>
       </c>
       <c r="E20" s="6" t="s">
-        <v>53</v>
+        <v>20</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="16" thickBot="1">
@@ -1140,16 +1158,16 @@
         <v>20</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>69</v>
+        <v>36</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>70</v>
+        <v>0</v>
       </c>
       <c r="D21" s="7">
         <v>39400</v>
       </c>
       <c r="E21" s="6" t="s">
-        <v>54</v>
+        <v>21</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="31" thickBot="1">
@@ -1157,16 +1175,16 @@
         <v>21</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>71</v>
+        <v>1</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>72</v>
+        <v>2</v>
       </c>
       <c r="D22" s="7">
         <v>39400</v>
       </c>
       <c r="E22" s="6" t="s">
-        <v>54</v>
+        <v>21</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="31" thickBot="1">
@@ -1174,16 +1192,16 @@
         <v>22</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>6</v>
+        <v>43</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>73</v>
+        <v>3</v>
       </c>
       <c r="D23" s="7">
         <v>39400</v>
       </c>
       <c r="E23" s="6" t="s">
-        <v>54</v>
+        <v>21</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="31" thickBot="1">
@@ -1191,16 +1209,16 @@
         <v>23</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>10</v>
+        <v>47</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>7</v>
+        <v>44</v>
       </c>
       <c r="D24" s="7">
         <v>39400</v>
       </c>
       <c r="E24" s="6" t="s">
-        <v>8</v>
+        <v>45</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="16" thickBot="1">
@@ -1208,16 +1226,16 @@
         <v>24</v>
       </c>
       <c r="B25" s="12" t="s">
-        <v>31</v>
+        <v>68</v>
       </c>
       <c r="C25" s="12" t="s">
-        <v>37</v>
+        <v>74</v>
       </c>
       <c r="D25" s="13">
         <v>39415</v>
       </c>
       <c r="E25" s="12" t="s">
-        <v>9</v>
+        <v>46</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="16" thickBot="1">
@@ -1225,16 +1243,16 @@
         <v>25</v>
       </c>
       <c r="B26" s="12" t="s">
-        <v>32</v>
+        <v>69</v>
       </c>
       <c r="C26" s="12" t="s">
-        <v>11</v>
+        <v>48</v>
       </c>
       <c r="D26" s="13">
         <v>39421</v>
       </c>
       <c r="E26" s="12" t="s">
-        <v>3</v>
+        <v>40</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="31" thickBot="1">
@@ -1242,16 +1260,16 @@
         <v>26</v>
       </c>
       <c r="B27" s="12" t="s">
-        <v>33</v>
+        <v>70</v>
       </c>
       <c r="C27" s="12" t="s">
-        <v>44</v>
+        <v>11</v>
       </c>
       <c r="D27" s="13">
         <v>39421</v>
       </c>
       <c r="E27" s="12" t="s">
-        <v>3</v>
+        <v>40</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="16" thickBot="1">
@@ -1259,16 +1277,16 @@
         <v>27</v>
       </c>
       <c r="B28" s="14" t="s">
-        <v>4</v>
+        <v>41</v>
       </c>
       <c r="C28" s="15" t="s">
-        <v>5</v>
+        <v>42</v>
       </c>
       <c r="D28" s="16">
         <v>39470</v>
       </c>
       <c r="E28" s="15" t="s">
-        <v>12</v>
+        <v>49</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="91" thickBot="1">
@@ -1276,16 +1294,16 @@
         <v>28</v>
       </c>
       <c r="B29" s="12" t="s">
-        <v>57</v>
+        <v>24</v>
       </c>
       <c r="C29" s="12" t="s">
-        <v>58</v>
+        <v>25</v>
       </c>
       <c r="D29" s="13">
         <v>39470</v>
       </c>
       <c r="E29" s="12" t="s">
-        <v>59</v>
+        <v>26</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="31" thickBot="1">
@@ -1293,16 +1311,16 @@
         <v>29</v>
       </c>
       <c r="B30" s="12" t="s">
-        <v>60</v>
+        <v>27</v>
       </c>
       <c r="C30" s="12" t="s">
-        <v>61</v>
+        <v>28</v>
       </c>
       <c r="D30" s="13">
         <v>39477</v>
       </c>
       <c r="E30" s="12" t="s">
-        <v>13</v>
+        <v>50</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="46" thickBot="1">
@@ -1310,16 +1328,16 @@
         <v>30</v>
       </c>
       <c r="B31" s="12" t="s">
-        <v>55</v>
+        <v>22</v>
       </c>
       <c r="C31" s="12" t="s">
-        <v>56</v>
+        <v>23</v>
       </c>
       <c r="D31" s="13">
         <v>39477</v>
       </c>
       <c r="E31" s="12" t="s">
-        <v>13</v>
+        <v>50</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="16" thickBot="1">
@@ -1327,16 +1345,84 @@
         <v>31</v>
       </c>
       <c r="B32" s="12" t="s">
-        <v>15</v>
+        <v>52</v>
       </c>
       <c r="C32" s="12" t="s">
-        <v>16</v>
+        <v>53</v>
       </c>
       <c r="D32" s="13">
         <v>39491</v>
       </c>
       <c r="E32" s="12" t="s">
-        <v>51</v>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" ht="31" thickBot="1">
+      <c r="A33" s="11">
+        <v>32</v>
+      </c>
+      <c r="B33" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="C33" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="D33" s="13">
+        <v>39498</v>
+      </c>
+      <c r="E33" s="12" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" ht="16" thickBot="1">
+      <c r="A34" s="11">
+        <v>33</v>
+      </c>
+      <c r="B34" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="C34" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="D34" s="13">
+        <v>39498</v>
+      </c>
+      <c r="E34" s="12" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" ht="14" thickBot="1">
+      <c r="A35" s="8">
+        <v>34</v>
+      </c>
+      <c r="B35" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C35" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="D35" s="10">
+        <v>39505</v>
+      </c>
+      <c r="E35" s="9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" ht="16" thickBot="1">
+      <c r="A36" s="11">
+        <v>35</v>
+      </c>
+      <c r="B36" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="C36" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="D36" s="13">
+        <v>39505</v>
+      </c>
+      <c r="E36" s="12" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added action item re: MAGE-TAB export.
</commit_message>
<xml_diff>
--- a/project_management/caArray_caIntegrator_Action_Items.xlsx
+++ b/project_management/caArray_caIntegrator_Action_Items.xlsx
@@ -19,266 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="85">
-  <si>
-    <t>Set up an internal meeting to evaluate alternative approaches to setting permissions (common UI versus changes to individual apps)</t>
-  </si>
-  <si>
-    <t>Upgrade Curation tier to caArray 2.4.1.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Don Swan</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Quy Phung</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Eve Shalley</t>
-  </si>
-  <si>
-    <t>Complete</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Create wireframes to depict how permissions will work across caIntegrator and caArray.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Andy Evans and Will Fitzhugh</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Complete</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Follow up with Doug Hosier on BDA-Lite and AntHill Pro 3.0 requirement.</t>
-  </si>
-  <si>
-    <t>Warn caArray community re: planned down time of &lt;1 hour on Thursday at 8am.</t>
-  </si>
-  <si>
-    <t>Juli Klemm and Zhong Li</t>
-  </si>
-  <si>
-    <t>In Progress</t>
-  </si>
-  <si>
-    <t>Get modify access to Jira for Jill.</t>
-  </si>
-  <si>
-    <t>Complete</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Set up a meeting to discuss access needs to run caArrayImporter client to load data onto caArray on NCI Production server.</t>
-  </si>
-  <si>
-    <t>JJ Pan</t>
-  </si>
-  <si>
-    <t>Write up a short capability description of caArrayImporter client and QTP for loading large data sets.  Quy and Andrew to support.</t>
-  </si>
-  <si>
-    <t>Write up a requirement for autoloader – short term solution using caArrayImporter or QTP.  Xiaopang to provide input.</t>
-  </si>
-  <si>
-    <t>Complete</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Work with Eve to schedule a meeting with UCSF.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Provide a list of TCGA data - loadable/not loadable/unknowns and some options</t>
-  </si>
-  <si>
-    <t>Shine Jacob</t>
-  </si>
-  <si>
-    <t>Complete</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Complete</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Get sample data files from Sarah Davis/TRANSCEND team.</t>
-  </si>
-  <si>
-    <t>Deb Hope to ping Eve Shalley</t>
-  </si>
-  <si>
-    <t>Create sample experiments in caArray to represent TRANSCEND use cases.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Andy Evans</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Complete</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Complete</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Update permissions wireframes for TRANSCEND to reflect the latest understanding of the data.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Mervi Heiskanen</t>
-  </si>
-  <si>
-    <t>On Hold (I-SPY2 data not yet available)</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Complete</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>On Hold</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Send the Agilent 415K ADF custom array design to Zhong.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Henry Schaefer</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Shine and Rashmi to provide latest product roadmaps to Zhong for the MAT-KC.</t>
-  </si>
-  <si>
-    <t>Shine Jacob and Rashmi Srinivasa</t>
-  </si>
-  <si>
-    <t>Provide TRANSCEND requirements document to JJ.</t>
-  </si>
-  <si>
-    <t>caArray and caIntegrator demos for JJ</t>
-  </si>
-  <si>
-    <t>JJ Pan and Larry Brem</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Complete</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Talk to the UPT team re: dissuading caArray users from creating groups within UPT.</t>
-  </si>
-  <si>
-    <t>Item #</t>
-  </si>
-  <si>
-    <t>Description</t>
-  </si>
-  <si>
-    <t>Responsible Party</t>
-  </si>
-  <si>
-    <t>Date Identified</t>
-  </si>
-  <si>
-    <t>Disposition</t>
-  </si>
-  <si>
-    <t>Set up a meeting to discuss alternative short-term solutions to the large data set import problem.</t>
-  </si>
-  <si>
-    <t>Upgrade Training tier to caArray 2.4.1.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Set up regular once-in-2-weeks meetings with TRANSCEND</t>
-  </si>
-  <si>
-    <t>Set up a meeting with the caDSR team to discuss permissible values.</t>
-  </si>
-  <si>
-    <t>Juli Klemm</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Links to the caArray User’s Guide on the Download Center -&gt; Download page are incorrect</t>
-  </si>
-  <si>
-    <t>Rashmi Srinivasa</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Maureen Colbert</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Send triaged bug list to Juli, JJ, Deb and Larry and schedule a second Bug Triage meeting.</t>
-  </si>
-  <si>
-    <t>Submit ticket for BDALite configuration on the new STAGE tier</t>
-  </si>
-  <si>
-    <t>Discuss need for disaster recovery / backup server solution</t>
-  </si>
-  <si>
-    <t>Juli Klemm and JJ Pan</t>
-  </si>
-  <si>
-    <t>Not Started</t>
-  </si>
-  <si>
-    <t>Forward information re: dependency on EVS</t>
-  </si>
-  <si>
-    <t>Follow up on CIT Security policy change re: resolution of Medium vulnerabilities of app scan.</t>
-  </si>
-  <si>
-    <t>Rashmi Srinivasa</t>
-  </si>
-  <si>
-    <t>Complete</t>
-  </si>
-  <si>
-    <t>Send requirements process to JJ and schedule follow-up meeting.</t>
-  </si>
-  <si>
-    <t>Follow up with Rashmi to see if she can help resolve the problem of running the 508 compliance testing tool against caIntegrator.</t>
-  </si>
-  <si>
-    <t>Quy Phung</t>
-  </si>
-  <si>
-    <t>Tony Kervalage needs list of TRANSCEND requirements and LOE.</t>
-  </si>
-  <si>
-    <t>Rashmi Srinivasa and Shine Jacob</t>
-  </si>
-  <si>
-    <t>Complete</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Set up a meeting to discuss which TCGA data types need to be loaded into caIntegrator. Attendees: Tanya Davidson, Xiaopeng, Juli, Mervi, Shine, JP. (Mervi, Shine and JP all have vacation plans during August.)</t>
-  </si>
-  <si>
-    <t>Complete</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Complete</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="86">
   <si>
     <t>Schedule meeting to discuss TRANSCEND architecture recommendations and effect on caArray and caIntegrator project plans.</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -316,12 +57,284 @@
   </si>
   <si>
     <t>Set up a meeting to discuss caGrid 1.2 upgrade</t>
+  </si>
+  <si>
+    <t>Eve Shalley</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Rashmi Srinivasa</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Not Started</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Answer MAGE-TAB export question sent to App Support</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Shine Jacob and Rashmi Srinivasa</t>
+  </si>
+  <si>
+    <t>Provide TRANSCEND requirements document to JJ.</t>
+  </si>
+  <si>
+    <t>caArray and caIntegrator demos for JJ</t>
+  </si>
+  <si>
+    <t>JJ Pan and Larry Brem</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Complete</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Talk to the UPT team re: dissuading caArray users from creating groups within UPT.</t>
+  </si>
+  <si>
+    <t>Item #</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Responsible Party</t>
+  </si>
+  <si>
+    <t>Date Identified</t>
+  </si>
+  <si>
+    <t>Disposition</t>
+  </si>
+  <si>
+    <t>Set up a meeting to discuss alternative short-term solutions to the large data set import problem.</t>
+  </si>
+  <si>
+    <t>Upgrade Training tier to caArray 2.4.1.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Set up regular once-in-2-weeks meetings with TRANSCEND</t>
+  </si>
+  <si>
+    <t>Set up a meeting with the caDSR team to discuss permissible values.</t>
+  </si>
+  <si>
+    <t>Juli Klemm</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Links to the caArray User’s Guide on the Download Center -&gt; Download page are incorrect</t>
+  </si>
+  <si>
+    <t>Rashmi Srinivasa</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Maureen Colbert</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Send triaged bug list to Juli, JJ, Deb and Larry and schedule a second Bug Triage meeting.</t>
+  </si>
+  <si>
+    <t>Submit ticket for BDALite configuration on the new STAGE tier</t>
+  </si>
+  <si>
+    <t>Discuss need for disaster recovery / backup server solution</t>
+  </si>
+  <si>
+    <t>Juli Klemm and JJ Pan</t>
+  </si>
+  <si>
+    <t>Forward information re: dependency on EVS</t>
+  </si>
+  <si>
+    <t>Follow up on CIT Security policy change re: resolution of Medium vulnerabilities of app scan.</t>
+  </si>
+  <si>
+    <t>Rashmi Srinivasa</t>
+  </si>
+  <si>
+    <t>Complete</t>
+  </si>
+  <si>
+    <t>Send requirements process to JJ and schedule follow-up meeting.</t>
+  </si>
+  <si>
+    <t>Follow up with Rashmi to see if she can help resolve the problem of running the 508 compliance testing tool against caIntegrator.</t>
+  </si>
+  <si>
+    <t>Quy Phung</t>
+  </si>
+  <si>
+    <t>Tony Kervalage needs list of TRANSCEND requirements and LOE.</t>
+  </si>
+  <si>
+    <t>Rashmi Srinivasa and Shine Jacob</t>
+  </si>
+  <si>
+    <t>Complete</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Set up a meeting to discuss which TCGA data types need to be loaded into caIntegrator. Attendees: Tanya Davidson, Xiaopeng, Juli, Mervi, Shine, JP. (Mervi, Shine and JP all have vacation plans during August.)</t>
+  </si>
+  <si>
+    <t>Complete</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Complete</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Set up an internal meeting to evaluate alternative approaches to setting permissions (common UI versus changes to individual apps)</t>
+  </si>
+  <si>
+    <t>Upgrade Curation tier to caArray 2.4.1.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Don Swan</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Quy Phung</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Eve Shalley</t>
+  </si>
+  <si>
+    <t>Complete</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Create wireframes to depict how permissions will work across caIntegrator and caArray.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Andy Evans and Will Fitzhugh</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Complete</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Follow up with Doug Hosier on BDA-Lite and AntHill Pro 3.0 requirement.</t>
+  </si>
+  <si>
+    <t>Warn caArray community re: planned down time of &lt;1 hour on Thursday at 8am.</t>
+  </si>
+  <si>
+    <t>Juli Klemm and Zhong Li</t>
+  </si>
+  <si>
+    <t>Get modify access to Jira for Jill.</t>
+  </si>
+  <si>
+    <t>Complete</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Set up a meeting to discuss access needs to run caArrayImporter client to load data onto caArray on NCI Production server.</t>
+  </si>
+  <si>
+    <t>JJ Pan</t>
+  </si>
+  <si>
+    <t>Write up a short capability description of caArrayImporter client and QTP for loading large data sets.  Quy and Andrew to support.</t>
+  </si>
+  <si>
+    <t>Write up a requirement for autoloader – short term solution using caArrayImporter or QTP.  Xiaopang to provide input.</t>
+  </si>
+  <si>
+    <t>Complete</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Work with Eve to schedule a meeting with UCSF.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Provide a list of TCGA data - loadable/not loadable/unknowns and some options</t>
+  </si>
+  <si>
+    <t>Shine Jacob</t>
+  </si>
+  <si>
+    <t>Complete</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Complete</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Get sample data files from Sarah Davis/TRANSCEND team.</t>
+  </si>
+  <si>
+    <t>Create sample experiments in caArray to represent TRANSCEND use cases.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Andy Evans</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Complete</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Complete</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Update permissions wireframes for TRANSCEND to reflect the latest understanding of the data.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Mervi Heiskanen</t>
+  </si>
+  <si>
+    <t>On Hold (I-SPY2 data not yet available)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Complete</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>On Hold</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Send the Agilent 415K ADF custom array design to Zhong.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Henry Schaefer</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Shine and Rashmi to provide latest product roadmaps to Zhong for the MAT-KC.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+  </numFmts>
   <fonts count="6">
     <font>
       <sz val="10"/>
@@ -816,10 +829,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
-  <dimension ref="A1:E38"/>
+  <dimension ref="A1:E39"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="E36" sqref="E36"/>
+      <selection activeCell="C40" sqref="C40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -834,19 +847,19 @@
   <sheetData>
     <row r="1" spans="1:5" s="2" customFormat="1" ht="16" thickBot="1">
       <c r="A1" s="3" t="s">
-        <v>45</v>
+        <v>19</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>46</v>
+        <v>20</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>47</v>
+        <v>21</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>48</v>
+        <v>22</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>49</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="31" thickBot="1">
@@ -854,16 +867,16 @@
         <v>1</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>50</v>
+        <v>24</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>65</v>
+        <v>38</v>
       </c>
       <c r="D2" s="7">
         <v>39297</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>66</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="16" thickBot="1">
@@ -871,16 +884,16 @@
         <v>2</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>67</v>
+        <v>40</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>65</v>
+        <v>38</v>
       </c>
       <c r="D3" s="7">
         <v>39297</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>66</v>
+        <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="31" thickBot="1">
@@ -888,16 +901,16 @@
         <v>3</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>21</v>
+        <v>69</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>22</v>
+        <v>70</v>
       </c>
       <c r="D4" s="7">
         <v>39297</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>66</v>
+        <v>39</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="46" thickBot="1">
@@ -905,16 +918,16 @@
         <v>4</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>73</v>
+        <v>46</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>32</v>
+        <v>79</v>
       </c>
       <c r="D5" s="7">
         <v>39297</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>66</v>
+        <v>39</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="16" thickBot="1">
@@ -922,16 +935,16 @@
         <v>5</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>84</v>
+        <v>8</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>22</v>
+        <v>70</v>
       </c>
       <c r="D6" s="10">
         <v>39297</v>
       </c>
       <c r="E6" s="9" t="s">
-        <v>35</v>
+        <v>82</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="31" thickBot="1">
@@ -939,16 +952,16 @@
         <v>6</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>15</v>
+        <v>63</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>16</v>
+        <v>64</v>
       </c>
       <c r="D7" s="7">
         <v>39309</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>66</v>
+        <v>39</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="31" thickBot="1">
@@ -956,16 +969,16 @@
         <v>7</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>17</v>
+        <v>65</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>65</v>
+        <v>38</v>
       </c>
       <c r="D8" s="7">
         <v>39309</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>66</v>
+        <v>39</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="31" thickBot="1">
@@ -973,16 +986,16 @@
         <v>8</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>18</v>
+        <v>66</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>65</v>
+        <v>38</v>
       </c>
       <c r="D9" s="7">
         <v>39309</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>66</v>
+        <v>39</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="31" thickBot="1">
@@ -990,16 +1003,16 @@
         <v>9</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>68</v>
+        <v>41</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>69</v>
+        <v>42</v>
       </c>
       <c r="D10" s="7">
         <v>39309</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>66</v>
+        <v>39</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="16" thickBot="1">
@@ -1007,16 +1020,16 @@
         <v>10</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>70</v>
+        <v>43</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>4</v>
+        <v>53</v>
       </c>
       <c r="D11" s="7">
         <v>39309</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>19</v>
+        <v>67</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="31" thickBot="1">
@@ -1024,16 +1037,16 @@
         <v>11</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>38</v>
+        <v>85</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>39</v>
+        <v>13</v>
       </c>
       <c r="D12" s="7">
         <v>39316</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>5</v>
+        <v>54</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="16" thickBot="1">
@@ -1041,16 +1054,16 @@
         <v>12</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>40</v>
+        <v>14</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>22</v>
+        <v>70</v>
       </c>
       <c r="D13" s="7">
         <v>39323</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>66</v>
+        <v>39</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="16" thickBot="1">
@@ -1058,16 +1071,16 @@
         <v>13</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>41</v>
+        <v>15</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>71</v>
+        <v>44</v>
       </c>
       <c r="D14" s="7">
         <v>39330</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>23</v>
+        <v>71</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="31" thickBot="1">
@@ -1075,16 +1088,16 @@
         <v>14</v>
       </c>
       <c r="B15" s="12" t="s">
-        <v>44</v>
+        <v>18</v>
       </c>
       <c r="C15" s="12" t="s">
-        <v>42</v>
+        <v>16</v>
       </c>
       <c r="D15" s="13">
         <v>39330</v>
       </c>
       <c r="E15" s="12" t="s">
-        <v>83</v>
+        <v>7</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="31" thickBot="1">
@@ -1092,16 +1105,16 @@
         <v>15</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>9</v>
+        <v>58</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>16</v>
+        <v>64</v>
       </c>
       <c r="D16" s="7">
         <v>39344</v>
       </c>
       <c r="E16" s="6" t="s">
-        <v>8</v>
+        <v>57</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="31" thickBot="1">
@@ -1109,16 +1122,16 @@
         <v>16</v>
       </c>
       <c r="B17" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="C17" s="6" t="s">
         <v>64</v>
-      </c>
-      <c r="C17" s="6" t="s">
-        <v>16</v>
       </c>
       <c r="D17" s="7">
         <v>39344</v>
       </c>
       <c r="E17" s="6" t="s">
-        <v>8</v>
+        <v>57</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="16" thickBot="1">
@@ -1126,16 +1139,16 @@
         <v>17</v>
       </c>
       <c r="B18" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C18" s="6" t="s">
         <v>51</v>
-      </c>
-      <c r="C18" s="6" t="s">
-        <v>2</v>
       </c>
       <c r="D18" s="7">
         <v>39372</v>
       </c>
       <c r="E18" s="6" t="s">
-        <v>43</v>
+        <v>17</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="16" thickBot="1">
@@ -1143,16 +1156,16 @@
         <v>18</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>1</v>
+        <v>50</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>3</v>
+        <v>52</v>
       </c>
       <c r="D19" s="7">
         <v>39372</v>
       </c>
       <c r="E19" s="6" t="s">
-        <v>74</v>
+        <v>47</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="31" thickBot="1">
@@ -1160,16 +1173,16 @@
         <v>19</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>6</v>
+        <v>55</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>7</v>
+        <v>56</v>
       </c>
       <c r="D20" s="7">
         <v>39372</v>
       </c>
       <c r="E20" s="6" t="s">
-        <v>74</v>
+        <v>47</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="16" thickBot="1">
@@ -1177,16 +1190,16 @@
         <v>20</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>20</v>
+        <v>68</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>54</v>
+        <v>28</v>
       </c>
       <c r="D21" s="7">
         <v>39400</v>
       </c>
       <c r="E21" s="6" t="s">
-        <v>75</v>
+        <v>48</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="31" thickBot="1">
@@ -1194,16 +1207,16 @@
         <v>21</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>55</v>
+        <v>29</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>56</v>
+        <v>30</v>
       </c>
       <c r="D22" s="7">
         <v>39400</v>
       </c>
       <c r="E22" s="6" t="s">
-        <v>75</v>
+        <v>48</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="31" thickBot="1">
@@ -1211,16 +1224,16 @@
         <v>22</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>27</v>
+        <v>74</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>57</v>
+        <v>31</v>
       </c>
       <c r="D23" s="7">
         <v>39400</v>
       </c>
       <c r="E23" s="6" t="s">
-        <v>75</v>
+        <v>48</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="31" thickBot="1">
@@ -1228,16 +1241,16 @@
         <v>23</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>31</v>
+        <v>78</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>28</v>
+        <v>75</v>
       </c>
       <c r="D24" s="7">
         <v>39400</v>
       </c>
       <c r="E24" s="6" t="s">
-        <v>29</v>
+        <v>76</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="16" thickBot="1">
@@ -1245,16 +1258,16 @@
         <v>24</v>
       </c>
       <c r="B25" s="12" t="s">
-        <v>52</v>
+        <v>26</v>
       </c>
       <c r="C25" s="12" t="s">
-        <v>4</v>
+        <v>53</v>
       </c>
       <c r="D25" s="13">
         <v>39415</v>
       </c>
       <c r="E25" s="12" t="s">
-        <v>30</v>
+        <v>77</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="16" thickBot="1">
@@ -1262,16 +1275,16 @@
         <v>25</v>
       </c>
       <c r="B26" s="12" t="s">
-        <v>53</v>
+        <v>27</v>
       </c>
       <c r="C26" s="12" t="s">
-        <v>32</v>
+        <v>79</v>
       </c>
       <c r="D26" s="13">
         <v>39421</v>
       </c>
       <c r="E26" s="12" t="s">
-        <v>24</v>
+        <v>72</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="31" thickBot="1">
@@ -1279,16 +1292,16 @@
         <v>26</v>
       </c>
       <c r="B27" s="12" t="s">
-        <v>0</v>
+        <v>49</v>
       </c>
       <c r="C27" s="12" t="s">
-        <v>65</v>
+        <v>38</v>
       </c>
       <c r="D27" s="13">
         <v>39421</v>
       </c>
       <c r="E27" s="12" t="s">
-        <v>24</v>
+        <v>72</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="16" thickBot="1">
@@ -1296,16 +1309,16 @@
         <v>27</v>
       </c>
       <c r="B28" s="14" t="s">
-        <v>25</v>
+        <v>73</v>
       </c>
       <c r="C28" s="15" t="s">
-        <v>26</v>
+        <v>9</v>
       </c>
       <c r="D28" s="16">
         <v>39470</v>
       </c>
       <c r="E28" s="15" t="s">
-        <v>33</v>
+        <v>80</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="91" thickBot="1">
@@ -1313,16 +1326,16 @@
         <v>28</v>
       </c>
       <c r="B29" s="12" t="s">
-        <v>78</v>
+        <v>2</v>
       </c>
       <c r="C29" s="12" t="s">
-        <v>79</v>
+        <v>3</v>
       </c>
       <c r="D29" s="13">
         <v>39470</v>
       </c>
       <c r="E29" s="12" t="s">
-        <v>80</v>
+        <v>4</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="31" thickBot="1">
@@ -1330,16 +1343,16 @@
         <v>29</v>
       </c>
       <c r="B30" s="12" t="s">
-        <v>81</v>
+        <v>5</v>
       </c>
       <c r="C30" s="12" t="s">
-        <v>82</v>
+        <v>6</v>
       </c>
       <c r="D30" s="13">
         <v>39477</v>
       </c>
       <c r="E30" s="12" t="s">
-        <v>34</v>
+        <v>81</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="46" thickBot="1">
@@ -1347,16 +1360,16 @@
         <v>30</v>
       </c>
       <c r="B31" s="12" t="s">
-        <v>76</v>
+        <v>0</v>
       </c>
       <c r="C31" s="12" t="s">
-        <v>77</v>
+        <v>1</v>
       </c>
       <c r="D31" s="13">
         <v>39477</v>
       </c>
       <c r="E31" s="12" t="s">
-        <v>34</v>
+        <v>81</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="16" thickBot="1">
@@ -1364,16 +1377,16 @@
         <v>31</v>
       </c>
       <c r="B32" s="12" t="s">
-        <v>36</v>
+        <v>83</v>
       </c>
       <c r="C32" s="12" t="s">
-        <v>37</v>
+        <v>84</v>
       </c>
       <c r="D32" s="13">
         <v>39491</v>
       </c>
       <c r="E32" s="12" t="s">
-        <v>72</v>
+        <v>45</v>
       </c>
     </row>
     <row r="33" spans="1:5" ht="31" thickBot="1">
@@ -1381,16 +1394,16 @@
         <v>32</v>
       </c>
       <c r="B33" s="12" t="s">
-        <v>58</v>
+        <v>32</v>
       </c>
       <c r="C33" s="12" t="s">
-        <v>65</v>
+        <v>38</v>
       </c>
       <c r="D33" s="13">
         <v>39498</v>
       </c>
       <c r="E33" s="12" t="s">
-        <v>66</v>
+        <v>39</v>
       </c>
     </row>
     <row r="34" spans="1:5" ht="16" thickBot="1">
@@ -1398,16 +1411,16 @@
         <v>33</v>
       </c>
       <c r="B34" s="12" t="s">
-        <v>59</v>
+        <v>33</v>
       </c>
       <c r="C34" s="12" t="s">
-        <v>65</v>
+        <v>38</v>
       </c>
       <c r="D34" s="13">
         <v>39498</v>
       </c>
       <c r="E34" s="12" t="s">
-        <v>66</v>
+        <v>39</v>
       </c>
     </row>
     <row r="35" spans="1:5" ht="16" thickBot="1">
@@ -1415,16 +1428,16 @@
         <v>34</v>
       </c>
       <c r="B35" s="12" t="s">
-        <v>60</v>
+        <v>34</v>
       </c>
       <c r="C35" s="12" t="s">
-        <v>61</v>
+        <v>35</v>
       </c>
       <c r="D35" s="13">
         <v>39505</v>
       </c>
       <c r="E35" s="12" t="s">
-        <v>14</v>
+        <v>62</v>
       </c>
     </row>
     <row r="36" spans="1:5" ht="16" thickBot="1">
@@ -1432,50 +1445,67 @@
         <v>35</v>
       </c>
       <c r="B36" s="12" t="s">
-        <v>63</v>
+        <v>36</v>
       </c>
       <c r="C36" s="12" t="s">
-        <v>32</v>
+        <v>79</v>
       </c>
       <c r="D36" s="13">
         <v>39505</v>
       </c>
       <c r="E36" s="12" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" ht="26">
-      <c r="A37" s="1">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" ht="31" thickBot="1">
+      <c r="A37" s="11">
         <v>36</v>
       </c>
-      <c r="B37" s="1" t="s">
+      <c r="B37" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="C37" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="D37" s="13">
+        <v>39512</v>
+      </c>
+      <c r="E37" s="12" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" ht="16" thickBot="1">
+      <c r="A38" s="11">
+        <v>37</v>
+      </c>
+      <c r="B38" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="C38" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="D38" s="13">
+        <v>39512</v>
+      </c>
+      <c r="E38" s="12" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5">
+      <c r="A39" s="1">
+        <v>38</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C39" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C37" s="1" t="s">
+      <c r="D39" s="17">
+        <v>39533</v>
+      </c>
+      <c r="E39" s="1" t="s">
         <v>11</v>
-      </c>
-      <c r="D37" s="17">
-        <v>39512</v>
-      </c>
-      <c r="E37" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5">
-      <c r="A38" s="1">
-        <v>37</v>
-      </c>
-      <c r="B38" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C38" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="D38" s="17">
-        <v>39512</v>
-      </c>
-      <c r="E38" s="1" t="s">
-        <v>62</v>
       </c>
     </row>
   </sheetData>
@@ -1486,6 +1516,7 @@
   </sortState>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
Updated Action Items list.
</commit_message>
<xml_diff>
--- a/project_management/caArray_caIntegrator_Action_Items.xlsx
+++ b/project_management/caArray_caIntegrator_Action_Items.xlsx
@@ -21,6 +21,188 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="86">
   <si>
+    <t>Provide a list of TCGA data - loadable/not loadable/unknowns and some options</t>
+  </si>
+  <si>
+    <t>Shine Jacob</t>
+  </si>
+  <si>
+    <t>Complete</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Complete</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Get sample data files from Sarah Davis/TRANSCEND team.</t>
+  </si>
+  <si>
+    <t>Create sample experiments in caArray to represent TRANSCEND use cases.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Andy Evans</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Complete</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Complete</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Update permissions wireframes for TRANSCEND to reflect the latest understanding of the data.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Mervi Heiskanen</t>
+  </si>
+  <si>
+    <t>On Hold (I-SPY2 data not yet available)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Complete</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>On Hold</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Send the Agilent 415K ADF custom array design to Zhong.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Henry Schaefer</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Shine and Rashmi to provide latest product roadmaps to Zhong for the MAT-KC.</t>
+  </si>
+  <si>
+    <t>Complete</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Juli Klemm and JJ Pan</t>
+  </si>
+  <si>
+    <t>Forward information re: dependency on EVS</t>
+  </si>
+  <si>
+    <t>Follow up on CIT Security policy change re: resolution of Medium vulnerabilities of app scan.</t>
+  </si>
+  <si>
+    <t>Rashmi Srinivasa</t>
+  </si>
+  <si>
+    <t>Complete</t>
+  </si>
+  <si>
+    <t>Send requirements process to JJ and schedule follow-up meeting.</t>
+  </si>
+  <si>
+    <t>Follow up with Rashmi to see if she can help resolve the problem of running the 508 compliance testing tool against caIntegrator.</t>
+  </si>
+  <si>
+    <t>Quy Phung</t>
+  </si>
+  <si>
+    <t>Tony Kervalage needs list of TRANSCEND requirements and LOE.</t>
+  </si>
+  <si>
+    <t>Rashmi Srinivasa and Shine Jacob</t>
+  </si>
+  <si>
+    <t>Complete</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Set up a meeting to discuss which TCGA data types need to be loaded into caIntegrator. Attendees: Tanya Davidson, Xiaopeng, Juli, Mervi, Shine, JP. (Mervi, Shine and JP all have vacation plans during August.)</t>
+  </si>
+  <si>
+    <t>Complete</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Complete</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Set up an internal meeting to evaluate alternative approaches to setting permissions (common UI versus changes to individual apps)</t>
+  </si>
+  <si>
+    <t>Upgrade Curation tier to caArray 2.4.1.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Don Swan</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Quy Phung</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Eve Shalley</t>
+  </si>
+  <si>
+    <t>Complete</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Create wireframes to depict how permissions will work across caIntegrator and caArray.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Andy Evans and Will Fitzhugh</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Complete</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Follow up with Doug Hosier on BDA-Lite and AntHill Pro 3.0 requirement.</t>
+  </si>
+  <si>
+    <t>Warn caArray community re: planned down time of &lt;1 hour on Thursday at 8am.</t>
+  </si>
+  <si>
+    <t>Juli Klemm and Zhong Li</t>
+  </si>
+  <si>
+    <t>Get modify access to Jira for Jill.</t>
+  </si>
+  <si>
+    <t>Complete</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Set up a meeting to discuss access needs to run caArrayImporter client to load data onto caArray on NCI Production server.</t>
+  </si>
+  <si>
+    <t>JJ Pan</t>
+  </si>
+  <si>
+    <t>Write up a short capability description of caArrayImporter client and QTP for loading large data sets.  Quy and Andrew to support.</t>
+  </si>
+  <si>
+    <t>Write up a requirement for autoloader – short term solution using caArrayImporter or QTP.  Xiaopang to provide input.</t>
+  </si>
+  <si>
+    <t>Complete</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Work with Eve to schedule a meeting with UCSF.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
     <t>Schedule meeting to discuss TRANSCEND architecture recommendations and effect on caArray and caIntegrator project plans.</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -67,10 +249,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>Not Started</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>Answer MAGE-TAB export question sent to App Support</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -145,196 +323,12 @@
   </si>
   <si>
     <t>Discuss need for disaster recovery / backup server solution</t>
-  </si>
-  <si>
-    <t>Juli Klemm and JJ Pan</t>
-  </si>
-  <si>
-    <t>Forward information re: dependency on EVS</t>
-  </si>
-  <si>
-    <t>Follow up on CIT Security policy change re: resolution of Medium vulnerabilities of app scan.</t>
-  </si>
-  <si>
-    <t>Rashmi Srinivasa</t>
-  </si>
-  <si>
-    <t>Complete</t>
-  </si>
-  <si>
-    <t>Send requirements process to JJ and schedule follow-up meeting.</t>
-  </si>
-  <si>
-    <t>Follow up with Rashmi to see if she can help resolve the problem of running the 508 compliance testing tool against caIntegrator.</t>
-  </si>
-  <si>
-    <t>Quy Phung</t>
-  </si>
-  <si>
-    <t>Tony Kervalage needs list of TRANSCEND requirements and LOE.</t>
-  </si>
-  <si>
-    <t>Rashmi Srinivasa and Shine Jacob</t>
-  </si>
-  <si>
-    <t>Complete</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Set up a meeting to discuss which TCGA data types need to be loaded into caIntegrator. Attendees: Tanya Davidson, Xiaopeng, Juli, Mervi, Shine, JP. (Mervi, Shine and JP all have vacation plans during August.)</t>
-  </si>
-  <si>
-    <t>Complete</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Complete</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Set up an internal meeting to evaluate alternative approaches to setting permissions (common UI versus changes to individual apps)</t>
-  </si>
-  <si>
-    <t>Upgrade Curation tier to caArray 2.4.1.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Don Swan</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Quy Phung</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Eve Shalley</t>
-  </si>
-  <si>
-    <t>Complete</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Create wireframes to depict how permissions will work across caIntegrator and caArray.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Andy Evans and Will Fitzhugh</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Complete</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Follow up with Doug Hosier on BDA-Lite and AntHill Pro 3.0 requirement.</t>
-  </si>
-  <si>
-    <t>Warn caArray community re: planned down time of &lt;1 hour on Thursday at 8am.</t>
-  </si>
-  <si>
-    <t>Juli Klemm and Zhong Li</t>
-  </si>
-  <si>
-    <t>Get modify access to Jira for Jill.</t>
-  </si>
-  <si>
-    <t>Complete</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Set up a meeting to discuss access needs to run caArrayImporter client to load data onto caArray on NCI Production server.</t>
-  </si>
-  <si>
-    <t>JJ Pan</t>
-  </si>
-  <si>
-    <t>Write up a short capability description of caArrayImporter client and QTP for loading large data sets.  Quy and Andrew to support.</t>
-  </si>
-  <si>
-    <t>Write up a requirement for autoloader – short term solution using caArrayImporter or QTP.  Xiaopang to provide input.</t>
-  </si>
-  <si>
-    <t>Complete</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Work with Eve to schedule a meeting with UCSF.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Provide a list of TCGA data - loadable/not loadable/unknowns and some options</t>
-  </si>
-  <si>
-    <t>Shine Jacob</t>
-  </si>
-  <si>
-    <t>Complete</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Complete</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Get sample data files from Sarah Davis/TRANSCEND team.</t>
-  </si>
-  <si>
-    <t>Create sample experiments in caArray to represent TRANSCEND use cases.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Andy Evans</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Complete</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Complete</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Update permissions wireframes for TRANSCEND to reflect the latest understanding of the data.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Mervi Heiskanen</t>
-  </si>
-  <si>
-    <t>On Hold (I-SPY2 data not yet available)</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Complete</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>On Hold</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Send the Agilent 415K ADF custom array design to Zhong.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Henry Schaefer</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Shine and Rashmi to provide latest product roadmaps to Zhong for the MAT-KC.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-  </numFmts>
   <fonts count="6">
     <font>
       <sz val="10"/>
@@ -447,7 +441,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -496,9 +490,6 @@
     </xf>
     <xf numFmtId="14" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -831,8 +822,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <dimension ref="A1:E39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="C40" sqref="C40"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A39" sqref="A39:XFD39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -847,19 +838,19 @@
   <sheetData>
     <row r="1" spans="1:5" s="2" customFormat="1" ht="16" thickBot="1">
       <c r="A1" s="3" t="s">
-        <v>19</v>
+        <v>70</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>20</v>
+        <v>71</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>21</v>
+        <v>72</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>22</v>
+        <v>73</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>23</v>
+        <v>74</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="31" thickBot="1">
@@ -867,16 +858,16 @@
         <v>1</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>24</v>
+        <v>75</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>38</v>
+        <v>21</v>
       </c>
       <c r="D2" s="7">
         <v>39297</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>39</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="16" thickBot="1">
@@ -884,16 +875,16 @@
         <v>2</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>40</v>
+        <v>23</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>38</v>
+        <v>21</v>
       </c>
       <c r="D3" s="7">
         <v>39297</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>39</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="31" thickBot="1">
@@ -901,16 +892,16 @@
         <v>3</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>69</v>
+        <v>0</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>70</v>
+        <v>1</v>
       </c>
       <c r="D4" s="7">
         <v>39297</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>39</v>
+        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="46" thickBot="1">
@@ -918,16 +909,16 @@
         <v>4</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>46</v>
+        <v>29</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>79</v>
+        <v>10</v>
       </c>
       <c r="D5" s="7">
         <v>39297</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>39</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="16" thickBot="1">
@@ -935,16 +926,16 @@
         <v>5</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>8</v>
+        <v>60</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>70</v>
+        <v>1</v>
       </c>
       <c r="D6" s="10">
         <v>39297</v>
       </c>
       <c r="E6" s="9" t="s">
-        <v>82</v>
+        <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="31" thickBot="1">
@@ -952,16 +943,16 @@
         <v>6</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>63</v>
+        <v>46</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>64</v>
+        <v>47</v>
       </c>
       <c r="D7" s="7">
         <v>39309</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>39</v>
+        <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="31" thickBot="1">
@@ -969,16 +960,16 @@
         <v>7</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>65</v>
+        <v>48</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>38</v>
+        <v>21</v>
       </c>
       <c r="D8" s="7">
         <v>39309</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>39</v>
+        <v>22</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="31" thickBot="1">
@@ -986,16 +977,16 @@
         <v>8</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>66</v>
+        <v>49</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>38</v>
+        <v>21</v>
       </c>
       <c r="D9" s="7">
         <v>39309</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>39</v>
+        <v>22</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="31" thickBot="1">
@@ -1003,16 +994,16 @@
         <v>9</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>41</v>
+        <v>24</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>42</v>
+        <v>25</v>
       </c>
       <c r="D10" s="7">
         <v>39309</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>39</v>
+        <v>22</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="16" thickBot="1">
@@ -1020,16 +1011,16 @@
         <v>10</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>43</v>
+        <v>26</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>53</v>
+        <v>36</v>
       </c>
       <c r="D11" s="7">
         <v>39309</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>67</v>
+        <v>50</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="31" thickBot="1">
@@ -1037,16 +1028,16 @@
         <v>11</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>85</v>
+        <v>16</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>13</v>
+        <v>64</v>
       </c>
       <c r="D12" s="7">
         <v>39316</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>54</v>
+        <v>37</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="16" thickBot="1">
@@ -1054,16 +1045,16 @@
         <v>12</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>14</v>
+        <v>65</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>70</v>
+        <v>1</v>
       </c>
       <c r="D13" s="7">
         <v>39323</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>39</v>
+        <v>22</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="16" thickBot="1">
@@ -1071,16 +1062,16 @@
         <v>13</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>15</v>
+        <v>66</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>44</v>
+        <v>27</v>
       </c>
       <c r="D14" s="7">
         <v>39330</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>71</v>
+        <v>2</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="31" thickBot="1">
@@ -1088,16 +1079,16 @@
         <v>14</v>
       </c>
       <c r="B15" s="12" t="s">
-        <v>18</v>
+        <v>69</v>
       </c>
       <c r="C15" s="12" t="s">
-        <v>16</v>
+        <v>67</v>
       </c>
       <c r="D15" s="13">
         <v>39330</v>
       </c>
       <c r="E15" s="12" t="s">
-        <v>7</v>
+        <v>59</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="31" thickBot="1">
@@ -1105,16 +1096,16 @@
         <v>15</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>58</v>
+        <v>41</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>64</v>
+        <v>47</v>
       </c>
       <c r="D16" s="7">
         <v>39344</v>
       </c>
       <c r="E16" s="6" t="s">
-        <v>57</v>
+        <v>40</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="31" thickBot="1">
@@ -1122,16 +1113,16 @@
         <v>16</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>37</v>
+        <v>20</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>64</v>
+        <v>47</v>
       </c>
       <c r="D17" s="7">
         <v>39344</v>
       </c>
       <c r="E17" s="6" t="s">
-        <v>57</v>
+        <v>40</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="16" thickBot="1">
@@ -1139,16 +1130,16 @@
         <v>17</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>25</v>
+        <v>76</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>51</v>
+        <v>34</v>
       </c>
       <c r="D18" s="7">
         <v>39372</v>
       </c>
       <c r="E18" s="6" t="s">
-        <v>17</v>
+        <v>68</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="16" thickBot="1">
@@ -1156,16 +1147,16 @@
         <v>18</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>50</v>
+        <v>33</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>52</v>
+        <v>35</v>
       </c>
       <c r="D19" s="7">
         <v>39372</v>
       </c>
       <c r="E19" s="6" t="s">
-        <v>47</v>
+        <v>30</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="31" thickBot="1">
@@ -1173,16 +1164,16 @@
         <v>19</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>55</v>
+        <v>38</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>56</v>
+        <v>39</v>
       </c>
       <c r="D20" s="7">
         <v>39372</v>
       </c>
       <c r="E20" s="6" t="s">
-        <v>47</v>
+        <v>30</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="16" thickBot="1">
@@ -1190,16 +1181,16 @@
         <v>20</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>68</v>
+        <v>51</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>28</v>
+        <v>79</v>
       </c>
       <c r="D21" s="7">
         <v>39400</v>
       </c>
       <c r="E21" s="6" t="s">
-        <v>48</v>
+        <v>31</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="31" thickBot="1">
@@ -1207,16 +1198,16 @@
         <v>21</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>29</v>
+        <v>80</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>30</v>
+        <v>81</v>
       </c>
       <c r="D22" s="7">
         <v>39400</v>
       </c>
       <c r="E22" s="6" t="s">
-        <v>48</v>
+        <v>31</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="31" thickBot="1">
@@ -1224,16 +1215,16 @@
         <v>22</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>74</v>
+        <v>5</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>31</v>
+        <v>82</v>
       </c>
       <c r="D23" s="7">
         <v>39400</v>
       </c>
       <c r="E23" s="6" t="s">
-        <v>48</v>
+        <v>31</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="31" thickBot="1">
@@ -1241,16 +1232,16 @@
         <v>23</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>78</v>
+        <v>9</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>75</v>
+        <v>6</v>
       </c>
       <c r="D24" s="7">
         <v>39400</v>
       </c>
       <c r="E24" s="6" t="s">
-        <v>76</v>
+        <v>7</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="16" thickBot="1">
@@ -1258,16 +1249,16 @@
         <v>24</v>
       </c>
       <c r="B25" s="12" t="s">
-        <v>26</v>
+        <v>77</v>
       </c>
       <c r="C25" s="12" t="s">
-        <v>53</v>
+        <v>36</v>
       </c>
       <c r="D25" s="13">
         <v>39415</v>
       </c>
       <c r="E25" s="12" t="s">
-        <v>77</v>
+        <v>8</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="16" thickBot="1">
@@ -1275,16 +1266,16 @@
         <v>25</v>
       </c>
       <c r="B26" s="12" t="s">
-        <v>27</v>
+        <v>78</v>
       </c>
       <c r="C26" s="12" t="s">
-        <v>79</v>
+        <v>10</v>
       </c>
       <c r="D26" s="13">
         <v>39421</v>
       </c>
       <c r="E26" s="12" t="s">
-        <v>72</v>
+        <v>3</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="31" thickBot="1">
@@ -1292,16 +1283,16 @@
         <v>26</v>
       </c>
       <c r="B27" s="12" t="s">
-        <v>49</v>
+        <v>32</v>
       </c>
       <c r="C27" s="12" t="s">
-        <v>38</v>
+        <v>21</v>
       </c>
       <c r="D27" s="13">
         <v>39421</v>
       </c>
       <c r="E27" s="12" t="s">
-        <v>72</v>
+        <v>3</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="16" thickBot="1">
@@ -1309,16 +1300,16 @@
         <v>27</v>
       </c>
       <c r="B28" s="14" t="s">
-        <v>73</v>
+        <v>4</v>
       </c>
       <c r="C28" s="15" t="s">
-        <v>9</v>
+        <v>61</v>
       </c>
       <c r="D28" s="16">
         <v>39470</v>
       </c>
       <c r="E28" s="15" t="s">
-        <v>80</v>
+        <v>11</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="91" thickBot="1">
@@ -1326,16 +1317,16 @@
         <v>28</v>
       </c>
       <c r="B29" s="12" t="s">
-        <v>2</v>
+        <v>54</v>
       </c>
       <c r="C29" s="12" t="s">
-        <v>3</v>
+        <v>55</v>
       </c>
       <c r="D29" s="13">
         <v>39470</v>
       </c>
       <c r="E29" s="12" t="s">
-        <v>4</v>
+        <v>56</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="31" thickBot="1">
@@ -1343,16 +1334,16 @@
         <v>29</v>
       </c>
       <c r="B30" s="12" t="s">
-        <v>5</v>
+        <v>57</v>
       </c>
       <c r="C30" s="12" t="s">
-        <v>6</v>
+        <v>58</v>
       </c>
       <c r="D30" s="13">
         <v>39477</v>
       </c>
       <c r="E30" s="12" t="s">
-        <v>81</v>
+        <v>12</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="46" thickBot="1">
@@ -1360,16 +1351,16 @@
         <v>30</v>
       </c>
       <c r="B31" s="12" t="s">
-        <v>0</v>
+        <v>52</v>
       </c>
       <c r="C31" s="12" t="s">
-        <v>1</v>
+        <v>53</v>
       </c>
       <c r="D31" s="13">
         <v>39477</v>
       </c>
       <c r="E31" s="12" t="s">
-        <v>81</v>
+        <v>12</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="16" thickBot="1">
@@ -1377,16 +1368,16 @@
         <v>31</v>
       </c>
       <c r="B32" s="12" t="s">
-        <v>83</v>
+        <v>14</v>
       </c>
       <c r="C32" s="12" t="s">
-        <v>84</v>
+        <v>15</v>
       </c>
       <c r="D32" s="13">
         <v>39491</v>
       </c>
       <c r="E32" s="12" t="s">
-        <v>45</v>
+        <v>28</v>
       </c>
     </row>
     <row r="33" spans="1:5" ht="31" thickBot="1">
@@ -1394,16 +1385,16 @@
         <v>32</v>
       </c>
       <c r="B33" s="12" t="s">
-        <v>32</v>
+        <v>83</v>
       </c>
       <c r="C33" s="12" t="s">
-        <v>38</v>
+        <v>21</v>
       </c>
       <c r="D33" s="13">
         <v>39498</v>
       </c>
       <c r="E33" s="12" t="s">
-        <v>39</v>
+        <v>22</v>
       </c>
     </row>
     <row r="34" spans="1:5" ht="16" thickBot="1">
@@ -1411,16 +1402,16 @@
         <v>33</v>
       </c>
       <c r="B34" s="12" t="s">
-        <v>33</v>
+        <v>84</v>
       </c>
       <c r="C34" s="12" t="s">
-        <v>38</v>
+        <v>21</v>
       </c>
       <c r="D34" s="13">
         <v>39498</v>
       </c>
       <c r="E34" s="12" t="s">
-        <v>39</v>
+        <v>22</v>
       </c>
     </row>
     <row r="35" spans="1:5" ht="16" thickBot="1">
@@ -1428,16 +1419,16 @@
         <v>34</v>
       </c>
       <c r="B35" s="12" t="s">
-        <v>34</v>
+        <v>85</v>
       </c>
       <c r="C35" s="12" t="s">
-        <v>35</v>
+        <v>18</v>
       </c>
       <c r="D35" s="13">
         <v>39505</v>
       </c>
       <c r="E35" s="12" t="s">
-        <v>62</v>
+        <v>45</v>
       </c>
     </row>
     <row r="36" spans="1:5" ht="16" thickBot="1">
@@ -1445,16 +1436,16 @@
         <v>35</v>
       </c>
       <c r="B36" s="12" t="s">
-        <v>36</v>
+        <v>19</v>
       </c>
       <c r="C36" s="12" t="s">
-        <v>79</v>
+        <v>10</v>
       </c>
       <c r="D36" s="13">
         <v>39505</v>
       </c>
       <c r="E36" s="12" t="s">
-        <v>39</v>
+        <v>22</v>
       </c>
     </row>
     <row r="37" spans="1:5" ht="31" thickBot="1">
@@ -1462,16 +1453,16 @@
         <v>36</v>
       </c>
       <c r="B37" s="12" t="s">
-        <v>59</v>
+        <v>42</v>
       </c>
       <c r="C37" s="12" t="s">
-        <v>60</v>
+        <v>43</v>
       </c>
       <c r="D37" s="13">
         <v>39512</v>
       </c>
       <c r="E37" s="12" t="s">
-        <v>39</v>
+        <v>22</v>
       </c>
     </row>
     <row r="38" spans="1:5" ht="16" thickBot="1">
@@ -1479,33 +1470,33 @@
         <v>37</v>
       </c>
       <c r="B38" s="12" t="s">
-        <v>61</v>
+        <v>44</v>
       </c>
       <c r="C38" s="12" t="s">
-        <v>38</v>
+        <v>21</v>
       </c>
       <c r="D38" s="13">
         <v>39512</v>
       </c>
       <c r="E38" s="12" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5">
-      <c r="A39" s="1">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" ht="16" thickBot="1">
+      <c r="A39" s="11">
         <v>38</v>
       </c>
-      <c r="B39" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C39" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D39" s="17">
+      <c r="B39" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="C39" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="D39" s="13">
         <v>39533</v>
       </c>
-      <c r="E39" s="1" t="s">
-        <v>11</v>
+      <c r="E39" s="12" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -1516,7 +1507,6 @@
   </sortState>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
Updated Action Items after status meeting.
</commit_message>
<xml_diff>
--- a/project_management/caArray_caIntegrator_Action_Items.xlsx
+++ b/project_management/caArray_caIntegrator_Action_Items.xlsx
@@ -19,143 +19,63 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="86">
-  <si>
-    <t>Provide a list of TCGA data - loadable/not loadable/unknowns and some options</t>
-  </si>
-  <si>
-    <t>Shine Jacob</t>
-  </si>
-  <si>
-    <t>Complete</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Complete</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Get sample data files from Sarah Davis/TRANSCEND team.</t>
-  </si>
-  <si>
-    <t>Create sample experiments in caArray to represent TRANSCEND use cases.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Andy Evans</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Complete</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Complete</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Update permissions wireframes for TRANSCEND to reflect the latest understanding of the data.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Mervi Heiskanen</t>
-  </si>
-  <si>
-    <t>On Hold (I-SPY2 data not yet available)</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Complete</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>On Hold</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Send the Agilent 415K ADF custom array design to Zhong.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Henry Schaefer</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Shine and Rashmi to provide latest product roadmaps to Zhong for the MAT-KC.</t>
-  </si>
-  <si>
-    <t>Complete</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Juli Klemm and JJ Pan</t>
-  </si>
-  <si>
-    <t>Forward information re: dependency on EVS</t>
-  </si>
-  <si>
-    <t>Follow up on CIT Security policy change re: resolution of Medium vulnerabilities of app scan.</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="89">
+  <si>
+    <t>Responsible Party</t>
+  </si>
+  <si>
+    <t>Date Identified</t>
+  </si>
+  <si>
+    <t>Disposition</t>
+  </si>
+  <si>
+    <t>Set up a meeting to discuss alternative short-term solutions to the large data set import problem.</t>
+  </si>
+  <si>
+    <t>Upgrade Training tier to caArray 2.4.1.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Set up regular once-in-2-weeks meetings with TRANSCEND</t>
+  </si>
+  <si>
+    <t>Set up a meeting with the caDSR team to discuss permissible values.</t>
+  </si>
+  <si>
+    <t>Juli Klemm</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Links to the caArray User’s Guide on the Download Center -&gt; Download page are incorrect</t>
   </si>
   <si>
     <t>Rashmi Srinivasa</t>
-  </si>
-  <si>
-    <t>Complete</t>
-  </si>
-  <si>
-    <t>Send requirements process to JJ and schedule follow-up meeting.</t>
-  </si>
-  <si>
-    <t>Follow up with Rashmi to see if she can help resolve the problem of running the 508 compliance testing tool against caIntegrator.</t>
-  </si>
-  <si>
-    <t>Quy Phung</t>
-  </si>
-  <si>
-    <t>Tony Kervalage needs list of TRANSCEND requirements and LOE.</t>
-  </si>
-  <si>
-    <t>Rashmi Srinivasa and Shine Jacob</t>
-  </si>
-  <si>
-    <t>Complete</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Set up a meeting to discuss which TCGA data types need to be loaded into caIntegrator. Attendees: Tanya Davidson, Xiaopeng, Juli, Mervi, Shine, JP. (Mervi, Shine and JP all have vacation plans during August.)</t>
-  </si>
-  <si>
-    <t>Complete</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Complete</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Set up an internal meeting to evaluate alternative approaches to setting permissions (common UI versus changes to individual apps)</t>
-  </si>
-  <si>
-    <t>Upgrade Curation tier to caArray 2.4.1.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Don Swan</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Quy Phung</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Eve Shalley</t>
-  </si>
-  <si>
-    <t>Complete</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Create wireframes to depict how permissions will work across caIntegrator and caArray.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Maureen Colbert</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Send triaged bug list to Juli, JJ, Deb and Larry and schedule a second Bug Triage meeting.</t>
+  </si>
+  <si>
+    <t>Submit ticket for BDALite configuration on the new STAGE tier</t>
+  </si>
+  <si>
+    <t>Discuss need for disaster recovery / backup server solution</t>
+  </si>
+  <si>
+    <t>Juli Klemm</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Not Started</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Send a note to the caArray community about the 2.4.1 bug.</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
@@ -279,56 +199,154 @@
     <t>Description</t>
   </si>
   <si>
-    <t>Responsible Party</t>
-  </si>
-  <si>
-    <t>Date Identified</t>
-  </si>
-  <si>
-    <t>Disposition</t>
-  </si>
-  <si>
-    <t>Set up a meeting to discuss alternative short-term solutions to the large data set import problem.</t>
-  </si>
-  <si>
-    <t>Upgrade Training tier to caArray 2.4.1.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Set up regular once-in-2-weeks meetings with TRANSCEND</t>
-  </si>
-  <si>
-    <t>Set up a meeting with the caDSR team to discuss permissible values.</t>
-  </si>
-  <si>
-    <t>Juli Klemm</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Links to the caArray User’s Guide on the Download Center -&gt; Download page are incorrect</t>
+    <t>Provide a list of TCGA data - loadable/not loadable/unknowns and some options</t>
+  </si>
+  <si>
+    <t>Shine Jacob</t>
+  </si>
+  <si>
+    <t>Complete</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Complete</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Get sample data files from Sarah Davis/TRANSCEND team.</t>
+  </si>
+  <si>
+    <t>Create sample experiments in caArray to represent TRANSCEND use cases.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Andy Evans</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Complete</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Complete</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Update permissions wireframes for TRANSCEND to reflect the latest understanding of the data.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Mervi Heiskanen</t>
+  </si>
+  <si>
+    <t>On Hold (I-SPY2 data not yet available)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Complete</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>On Hold</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Send the Agilent 415K ADF custom array design to Zhong.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Henry Schaefer</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Shine and Rashmi to provide latest product roadmaps to Zhong for the MAT-KC.</t>
+  </si>
+  <si>
+    <t>Complete</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Juli Klemm and JJ Pan</t>
+  </si>
+  <si>
+    <t>Forward information re: dependency on EVS</t>
+  </si>
+  <si>
+    <t>Follow up on CIT Security policy change re: resolution of Medium vulnerabilities of app scan.</t>
   </si>
   <si>
     <t>Rashmi Srinivasa</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Maureen Colbert</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Send triaged bug list to Juli, JJ, Deb and Larry and schedule a second Bug Triage meeting.</t>
-  </si>
-  <si>
-    <t>Submit ticket for BDALite configuration on the new STAGE tier</t>
-  </si>
-  <si>
-    <t>Discuss need for disaster recovery / backup server solution</t>
+  </si>
+  <si>
+    <t>Complete</t>
+  </si>
+  <si>
+    <t>Send requirements process to JJ and schedule follow-up meeting.</t>
+  </si>
+  <si>
+    <t>Follow up with Rashmi to see if she can help resolve the problem of running the 508 compliance testing tool against caIntegrator.</t>
+  </si>
+  <si>
+    <t>Quy Phung</t>
+  </si>
+  <si>
+    <t>Tony Kervalage needs list of TRANSCEND requirements and LOE.</t>
+  </si>
+  <si>
+    <t>Rashmi Srinivasa and Shine Jacob</t>
+  </si>
+  <si>
+    <t>Complete</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Set up a meeting to discuss which TCGA data types need to be loaded into caIntegrator. Attendees: Tanya Davidson, Xiaopeng, Juli, Mervi, Shine, JP. (Mervi, Shine and JP all have vacation plans during August.)</t>
+  </si>
+  <si>
+    <t>Complete</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Complete</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Set up an internal meeting to evaluate alternative approaches to setting permissions (common UI versus changes to individual apps)</t>
+  </si>
+  <si>
+    <t>Upgrade Curation tier to caArray 2.4.1.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Don Swan</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Quy Phung</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Eve Shalley</t>
+  </si>
+  <si>
+    <t>Complete</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Create wireframes to depict how permissions will work across caIntegrator and caArray.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+  </numFmts>
   <fonts count="6">
     <font>
       <sz val="10"/>
@@ -820,10 +838,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
-  <dimension ref="A1:E39"/>
+  <dimension ref="A1:E40"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="A39" sqref="A39:XFD39"/>
+      <selection activeCell="B40" sqref="B40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -838,19 +856,19 @@
   <sheetData>
     <row r="1" spans="1:5" s="2" customFormat="1" ht="16" thickBot="1">
       <c r="A1" s="3" t="s">
-        <v>70</v>
+        <v>48</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>71</v>
+        <v>49</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>72</v>
+        <v>0</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>73</v>
+        <v>1</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>74</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="31" thickBot="1">
@@ -858,16 +876,16 @@
         <v>1</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>75</v>
+        <v>3</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>21</v>
+        <v>71</v>
       </c>
       <c r="D2" s="7">
         <v>39297</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>22</v>
+        <v>72</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="16" thickBot="1">
@@ -875,16 +893,16 @@
         <v>2</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>23</v>
+        <v>73</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>21</v>
+        <v>71</v>
       </c>
       <c r="D3" s="7">
         <v>39297</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>22</v>
+        <v>72</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="31" thickBot="1">
@@ -892,16 +910,16 @@
         <v>3</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>1</v>
+        <v>51</v>
       </c>
       <c r="D4" s="7">
         <v>39297</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>22</v>
+        <v>72</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="46" thickBot="1">
@@ -909,16 +927,16 @@
         <v>4</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>29</v>
+        <v>79</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>10</v>
+        <v>60</v>
       </c>
       <c r="D5" s="7">
         <v>39297</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>22</v>
+        <v>72</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="16" thickBot="1">
@@ -926,16 +944,16 @@
         <v>5</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>60</v>
+        <v>38</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>1</v>
+        <v>51</v>
       </c>
       <c r="D6" s="10">
         <v>39297</v>
       </c>
       <c r="E6" s="9" t="s">
-        <v>13</v>
+        <v>63</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="31" thickBot="1">
@@ -943,16 +961,16 @@
         <v>6</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>46</v>
+        <v>24</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>47</v>
+        <v>25</v>
       </c>
       <c r="D7" s="7">
         <v>39309</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>22</v>
+        <v>72</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="31" thickBot="1">
@@ -960,16 +978,16 @@
         <v>7</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>48</v>
+        <v>26</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>21</v>
+        <v>71</v>
       </c>
       <c r="D8" s="7">
         <v>39309</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>22</v>
+        <v>72</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="31" thickBot="1">
@@ -977,16 +995,16 @@
         <v>8</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>49</v>
+        <v>27</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>21</v>
+        <v>71</v>
       </c>
       <c r="D9" s="7">
         <v>39309</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>22</v>
+        <v>72</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="31" thickBot="1">
@@ -994,16 +1012,16 @@
         <v>9</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>24</v>
+        <v>74</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>25</v>
+        <v>75</v>
       </c>
       <c r="D10" s="7">
         <v>39309</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>22</v>
+        <v>72</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="16" thickBot="1">
@@ -1011,16 +1029,16 @@
         <v>10</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>26</v>
+        <v>76</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>36</v>
+        <v>86</v>
       </c>
       <c r="D11" s="7">
         <v>39309</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>50</v>
+        <v>28</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="31" thickBot="1">
@@ -1028,16 +1046,16 @@
         <v>11</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>16</v>
+        <v>66</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>64</v>
+        <v>42</v>
       </c>
       <c r="D12" s="7">
         <v>39316</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>37</v>
+        <v>87</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="16" thickBot="1">
@@ -1045,16 +1063,16 @@
         <v>12</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>65</v>
+        <v>43</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>1</v>
+        <v>51</v>
       </c>
       <c r="D13" s="7">
         <v>39323</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>22</v>
+        <v>72</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="16" thickBot="1">
@@ -1062,16 +1080,16 @@
         <v>13</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>66</v>
+        <v>44</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>27</v>
+        <v>77</v>
       </c>
       <c r="D14" s="7">
         <v>39330</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>2</v>
+        <v>52</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="31" thickBot="1">
@@ -1079,16 +1097,16 @@
         <v>14</v>
       </c>
       <c r="B15" s="12" t="s">
-        <v>69</v>
+        <v>47</v>
       </c>
       <c r="C15" s="12" t="s">
-        <v>67</v>
+        <v>45</v>
       </c>
       <c r="D15" s="13">
         <v>39330</v>
       </c>
       <c r="E15" s="12" t="s">
-        <v>59</v>
+        <v>37</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="31" thickBot="1">
@@ -1096,16 +1114,16 @@
         <v>15</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>41</v>
+        <v>19</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>47</v>
+        <v>25</v>
       </c>
       <c r="D16" s="7">
         <v>39344</v>
       </c>
       <c r="E16" s="6" t="s">
-        <v>40</v>
+        <v>18</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="31" thickBot="1">
@@ -1113,16 +1131,16 @@
         <v>16</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>20</v>
+        <v>70</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>47</v>
+        <v>25</v>
       </c>
       <c r="D17" s="7">
         <v>39344</v>
       </c>
       <c r="E17" s="6" t="s">
-        <v>40</v>
+        <v>18</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="16" thickBot="1">
@@ -1130,16 +1148,16 @@
         <v>17</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>76</v>
+        <v>4</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>34</v>
+        <v>84</v>
       </c>
       <c r="D18" s="7">
         <v>39372</v>
       </c>
       <c r="E18" s="6" t="s">
-        <v>68</v>
+        <v>46</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="16" thickBot="1">
@@ -1147,16 +1165,16 @@
         <v>18</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>33</v>
+        <v>83</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>35</v>
+        <v>85</v>
       </c>
       <c r="D19" s="7">
         <v>39372</v>
       </c>
       <c r="E19" s="6" t="s">
-        <v>30</v>
+        <v>80</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="31" thickBot="1">
@@ -1164,16 +1182,16 @@
         <v>19</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>38</v>
+        <v>88</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>39</v>
+        <v>17</v>
       </c>
       <c r="D20" s="7">
         <v>39372</v>
       </c>
       <c r="E20" s="6" t="s">
-        <v>30</v>
+        <v>80</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="16" thickBot="1">
@@ -1181,16 +1199,16 @@
         <v>20</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>51</v>
+        <v>29</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>79</v>
+        <v>7</v>
       </c>
       <c r="D21" s="7">
         <v>39400</v>
       </c>
       <c r="E21" s="6" t="s">
-        <v>31</v>
+        <v>81</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="31" thickBot="1">
@@ -1198,16 +1216,16 @@
         <v>21</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>80</v>
+        <v>8</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>81</v>
+        <v>9</v>
       </c>
       <c r="D22" s="7">
         <v>39400</v>
       </c>
       <c r="E22" s="6" t="s">
-        <v>31</v>
+        <v>81</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="31" thickBot="1">
@@ -1215,16 +1233,16 @@
         <v>22</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>5</v>
+        <v>55</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>82</v>
+        <v>10</v>
       </c>
       <c r="D23" s="7">
         <v>39400</v>
       </c>
       <c r="E23" s="6" t="s">
-        <v>31</v>
+        <v>81</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="31" thickBot="1">
@@ -1232,16 +1250,16 @@
         <v>23</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>9</v>
+        <v>59</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>6</v>
+        <v>56</v>
       </c>
       <c r="D24" s="7">
         <v>39400</v>
       </c>
       <c r="E24" s="6" t="s">
-        <v>7</v>
+        <v>57</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="16" thickBot="1">
@@ -1249,16 +1267,16 @@
         <v>24</v>
       </c>
       <c r="B25" s="12" t="s">
-        <v>77</v>
+        <v>5</v>
       </c>
       <c r="C25" s="12" t="s">
-        <v>36</v>
+        <v>86</v>
       </c>
       <c r="D25" s="13">
         <v>39415</v>
       </c>
       <c r="E25" s="12" t="s">
-        <v>8</v>
+        <v>58</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="16" thickBot="1">
@@ -1266,16 +1284,16 @@
         <v>25</v>
       </c>
       <c r="B26" s="12" t="s">
-        <v>78</v>
+        <v>6</v>
       </c>
       <c r="C26" s="12" t="s">
-        <v>10</v>
+        <v>60</v>
       </c>
       <c r="D26" s="13">
         <v>39421</v>
       </c>
       <c r="E26" s="12" t="s">
-        <v>3</v>
+        <v>53</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="31" thickBot="1">
@@ -1283,16 +1301,16 @@
         <v>26</v>
       </c>
       <c r="B27" s="12" t="s">
-        <v>32</v>
+        <v>82</v>
       </c>
       <c r="C27" s="12" t="s">
-        <v>21</v>
+        <v>71</v>
       </c>
       <c r="D27" s="13">
         <v>39421</v>
       </c>
       <c r="E27" s="12" t="s">
-        <v>3</v>
+        <v>53</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="16" thickBot="1">
@@ -1300,16 +1318,16 @@
         <v>27</v>
       </c>
       <c r="B28" s="14" t="s">
-        <v>4</v>
+        <v>54</v>
       </c>
       <c r="C28" s="15" t="s">
-        <v>61</v>
+        <v>39</v>
       </c>
       <c r="D28" s="16">
         <v>39470</v>
       </c>
       <c r="E28" s="15" t="s">
-        <v>11</v>
+        <v>61</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="91" thickBot="1">
@@ -1317,16 +1335,16 @@
         <v>28</v>
       </c>
       <c r="B29" s="12" t="s">
-        <v>54</v>
+        <v>32</v>
       </c>
       <c r="C29" s="12" t="s">
-        <v>55</v>
+        <v>33</v>
       </c>
       <c r="D29" s="13">
         <v>39470</v>
       </c>
       <c r="E29" s="12" t="s">
-        <v>56</v>
+        <v>34</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="31" thickBot="1">
@@ -1334,16 +1352,16 @@
         <v>29</v>
       </c>
       <c r="B30" s="12" t="s">
-        <v>57</v>
+        <v>35</v>
       </c>
       <c r="C30" s="12" t="s">
-        <v>58</v>
+        <v>36</v>
       </c>
       <c r="D30" s="13">
         <v>39477</v>
       </c>
       <c r="E30" s="12" t="s">
-        <v>12</v>
+        <v>62</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="46" thickBot="1">
@@ -1351,16 +1369,16 @@
         <v>30</v>
       </c>
       <c r="B31" s="12" t="s">
-        <v>52</v>
+        <v>30</v>
       </c>
       <c r="C31" s="12" t="s">
-        <v>53</v>
+        <v>31</v>
       </c>
       <c r="D31" s="13">
         <v>39477</v>
       </c>
       <c r="E31" s="12" t="s">
-        <v>12</v>
+        <v>62</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="16" thickBot="1">
@@ -1368,16 +1386,16 @@
         <v>31</v>
       </c>
       <c r="B32" s="12" t="s">
-        <v>14</v>
+        <v>64</v>
       </c>
       <c r="C32" s="12" t="s">
-        <v>15</v>
+        <v>65</v>
       </c>
       <c r="D32" s="13">
         <v>39491</v>
       </c>
       <c r="E32" s="12" t="s">
-        <v>28</v>
+        <v>78</v>
       </c>
     </row>
     <row r="33" spans="1:5" ht="31" thickBot="1">
@@ -1385,16 +1403,16 @@
         <v>32</v>
       </c>
       <c r="B33" s="12" t="s">
-        <v>83</v>
+        <v>11</v>
       </c>
       <c r="C33" s="12" t="s">
-        <v>21</v>
+        <v>71</v>
       </c>
       <c r="D33" s="13">
         <v>39498</v>
       </c>
       <c r="E33" s="12" t="s">
-        <v>22</v>
+        <v>72</v>
       </c>
     </row>
     <row r="34" spans="1:5" ht="16" thickBot="1">
@@ -1402,16 +1420,16 @@
         <v>33</v>
       </c>
       <c r="B34" s="12" t="s">
-        <v>84</v>
+        <v>12</v>
       </c>
       <c r="C34" s="12" t="s">
-        <v>21</v>
+        <v>71</v>
       </c>
       <c r="D34" s="13">
         <v>39498</v>
       </c>
       <c r="E34" s="12" t="s">
-        <v>22</v>
+        <v>72</v>
       </c>
     </row>
     <row r="35" spans="1:5" ht="16" thickBot="1">
@@ -1419,16 +1437,16 @@
         <v>34</v>
       </c>
       <c r="B35" s="12" t="s">
-        <v>85</v>
+        <v>13</v>
       </c>
       <c r="C35" s="12" t="s">
-        <v>18</v>
+        <v>68</v>
       </c>
       <c r="D35" s="13">
         <v>39505</v>
       </c>
       <c r="E35" s="12" t="s">
-        <v>45</v>
+        <v>23</v>
       </c>
     </row>
     <row r="36" spans="1:5" ht="16" thickBot="1">
@@ -1436,16 +1454,16 @@
         <v>35</v>
       </c>
       <c r="B36" s="12" t="s">
-        <v>19</v>
+        <v>69</v>
       </c>
       <c r="C36" s="12" t="s">
-        <v>10</v>
+        <v>60</v>
       </c>
       <c r="D36" s="13">
         <v>39505</v>
       </c>
       <c r="E36" s="12" t="s">
-        <v>22</v>
+        <v>72</v>
       </c>
     </row>
     <row r="37" spans="1:5" ht="31" thickBot="1">
@@ -1453,16 +1471,16 @@
         <v>36</v>
       </c>
       <c r="B37" s="12" t="s">
-        <v>42</v>
+        <v>20</v>
       </c>
       <c r="C37" s="12" t="s">
-        <v>43</v>
+        <v>21</v>
       </c>
       <c r="D37" s="13">
         <v>39512</v>
       </c>
       <c r="E37" s="12" t="s">
-        <v>22</v>
+        <v>72</v>
       </c>
     </row>
     <row r="38" spans="1:5" ht="16" thickBot="1">
@@ -1470,16 +1488,16 @@
         <v>37</v>
       </c>
       <c r="B38" s="12" t="s">
-        <v>44</v>
+        <v>22</v>
       </c>
       <c r="C38" s="12" t="s">
-        <v>21</v>
+        <v>71</v>
       </c>
       <c r="D38" s="13">
         <v>39512</v>
       </c>
       <c r="E38" s="12" t="s">
-        <v>22</v>
+        <v>72</v>
       </c>
     </row>
     <row r="39" spans="1:5" ht="16" thickBot="1">
@@ -1487,16 +1505,33 @@
         <v>38</v>
       </c>
       <c r="B39" s="12" t="s">
-        <v>63</v>
+        <v>41</v>
       </c>
       <c r="C39" s="12" t="s">
-        <v>62</v>
+        <v>40</v>
       </c>
       <c r="D39" s="13">
         <v>39533</v>
       </c>
       <c r="E39" s="12" t="s">
-        <v>17</v>
+        <v>67</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" ht="16" thickBot="1">
+      <c r="A40" s="8">
+        <v>39</v>
+      </c>
+      <c r="B40" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="C40" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="D40" s="16">
+        <v>39547</v>
+      </c>
+      <c r="E40" s="15" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -1507,6 +1542,7 @@
   </sortState>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
New action items from May 8 meeting.
</commit_message>
<xml_diff>
--- a/project_management/caArray_caIntegrator_Action_Items.xlsx
+++ b/project_management/caArray_caIntegrator_Action_Items.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="33440" windowHeight="18920" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="33440" windowHeight="19580" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Action_Items" sheetId="1" r:id="rId1"/>
@@ -19,259 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="92">
-  <si>
-    <t>Follow up with Doug Hosier on BDA-Lite and AntHill Pro 3.0 requirement.</t>
-  </si>
-  <si>
-    <t>Warn caArray community re: planned down time of &lt;1 hour on Thursday at 8am.</t>
-  </si>
-  <si>
-    <t>Juli Klemm and Zhong Li</t>
-  </si>
-  <si>
-    <t>Get modify access to Jira for Jill.</t>
-  </si>
-  <si>
-    <t>Complete</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Set up a meeting to discuss access needs to run caArrayImporter client to load data onto caArray on NCI Production server.</t>
-  </si>
-  <si>
-    <t>JJ Pan</t>
-  </si>
-  <si>
-    <t>Write up a short capability description of caArrayImporter client and QTP for loading large data sets.  Quy and Andrew to support.</t>
-  </si>
-  <si>
-    <t>Write up a requirement for autoloader – short term solution using caArrayImporter or QTP.  Xiaopang to provide input.</t>
-  </si>
-  <si>
-    <t>Complete</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Work with Eve to schedule a meeting with UCSF.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Schedule meeting to discuss TRANSCEND architecture recommendations and effect on caArray and caIntegrator project plans.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Rashmi Srinivasa</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Check with Matt Kennedy and Eve re: getting hardware requirements to UCSF</t>
-  </si>
-  <si>
-    <t>Check with Eve re: bringing back the risk related to unavailability of I-SPY2 data</t>
-  </si>
-  <si>
-    <t>Complete (TRANSCEND-127 is open.)</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Complete</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Talk to the UPT team re: dissuading caArray users from creating groups within UPT.</t>
-  </si>
-  <si>
-    <t>Item #</t>
-  </si>
-  <si>
-    <t>Description</t>
-  </si>
-  <si>
-    <t>Provide a list of TCGA data - loadable/not loadable/unknowns and some options</t>
-  </si>
-  <si>
-    <t>Shine Jacob</t>
-  </si>
-  <si>
-    <t>Complete</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Complete</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Get sample data files from Sarah Davis/TRANSCEND team.</t>
-  </si>
-  <si>
-    <t>Create sample experiments in caArray to represent TRANSCEND use cases.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Andy Evans</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Complete</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Complete</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Update permissions wireframes for TRANSCEND to reflect the latest understanding of the data.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Mervi Heiskanen</t>
-  </si>
-  <si>
-    <t>On Hold (I-SPY2 data not yet available)</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Complete</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Send the Agilent 415K ADF custom array design to Zhong.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Henry Schaefer</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Shine and Rashmi to provide latest product roadmaps to Zhong for the MAT-KC.</t>
-  </si>
-  <si>
-    <t>Complete</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Juli Klemm and JJ Pan</t>
-  </si>
-  <si>
-    <t>Forward information re: dependency on EVS</t>
-  </si>
-  <si>
-    <t>Follow up on CIT Security policy change re: resolution of Medium vulnerabilities of app scan.</t>
-  </si>
-  <si>
-    <t>Responsible Party</t>
-  </si>
-  <si>
-    <t>Date Identified</t>
-  </si>
-  <si>
-    <t>Disposition</t>
-  </si>
-  <si>
-    <t>Set up a meeting to discuss alternative short-term solutions to the large data set import problem.</t>
-  </si>
-  <si>
-    <t>Upgrade Training tier to caArray 2.4.1.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Set up regular once-in-2-weeks meetings with TRANSCEND</t>
-  </si>
-  <si>
-    <t>Set up a meeting with the caDSR team to discuss permissible values.</t>
-  </si>
-  <si>
-    <t>Juli Klemm</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Links to the caArray User’s Guide on the Download Center -&gt; Download page are incorrect</t>
-  </si>
-  <si>
-    <t>Rashmi Srinivasa</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Maureen Colbert</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Send triaged bug list to Juli, JJ, Deb and Larry and schedule a second Bug Triage meeting.</t>
-  </si>
-  <si>
-    <t>Submit ticket for BDALite configuration on the new STAGE tier</t>
-  </si>
-  <si>
-    <t>Discuss need for disaster recovery / backup server solution</t>
-  </si>
-  <si>
-    <t>Juli Klemm</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Send a note to the caArray community about the 2.4.1 bug.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Andy Evans and Will Fitzhugh</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Complete</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Rashmi Srinivasa</t>
-  </si>
-  <si>
-    <t>Complete</t>
-  </si>
-  <si>
-    <t>Send requirements process to JJ and schedule follow-up meeting.</t>
-  </si>
-  <si>
-    <t>Follow up with Rashmi to see if she can help resolve the problem of running the 508 compliance testing tool against caIntegrator.</t>
-  </si>
-  <si>
-    <t>Quy Phung</t>
-  </si>
-  <si>
-    <t>Tony Kervalage needs list of TRANSCEND requirements and LOE.</t>
-  </si>
-  <si>
-    <t>Rashmi Srinivasa and Shine Jacob</t>
-  </si>
-  <si>
-    <t>Complete</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Set up a meeting to discuss which TCGA data types need to be loaded into caIntegrator. Attendees: Tanya Davidson, Xiaopeng, Juli, Mervi, Shine, JP. (Mervi, Shine and JP all have vacation plans during August.)</t>
-  </si>
-  <si>
-    <t>Complete</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Complete</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Set up an internal meeting to evaluate alternative approaches to setting permissions (common UI versus changes to individual apps)</t>
-  </si>
-  <si>
-    <t>Upgrade Curation tier to caArray 2.4.1.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Don Swan</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Quy Phung</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="96">
   <si>
     <t>Eve Shalley</t>
   </si>
@@ -345,6 +93,274 @@
   <si>
     <t>Complete</t>
     <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Schedule follow-up meeting re: caGrid upgrade with Todd, Larry, JJ and Deb.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Not Started</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Send information to Mervi about user/lab who is installing caIntegrator.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Don Swan</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Complete</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Juli Klemm and JJ Pan</t>
+  </si>
+  <si>
+    <t>Forward information re: dependency on EVS</t>
+  </si>
+  <si>
+    <t>Follow up on CIT Security policy change re: resolution of Medium vulnerabilities of app scan.</t>
+  </si>
+  <si>
+    <t>Responsible Party</t>
+  </si>
+  <si>
+    <t>Date Identified</t>
+  </si>
+  <si>
+    <t>Disposition</t>
+  </si>
+  <si>
+    <t>Set up a meeting to discuss alternative short-term solutions to the large data set import problem.</t>
+  </si>
+  <si>
+    <t>Upgrade Training tier to caArray 2.4.1.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Set up regular once-in-2-weeks meetings with TRANSCEND</t>
+  </si>
+  <si>
+    <t>Set up a meeting with the caDSR team to discuss permissible values.</t>
+  </si>
+  <si>
+    <t>Juli Klemm</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Links to the caArray User’s Guide on the Download Center -&gt; Download page are incorrect</t>
+  </si>
+  <si>
+    <t>Rashmi Srinivasa</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Maureen Colbert</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Send triaged bug list to Juli, JJ, Deb and Larry and schedule a second Bug Triage meeting.</t>
+  </si>
+  <si>
+    <t>Submit ticket for BDALite configuration on the new STAGE tier</t>
+  </si>
+  <si>
+    <t>Discuss need for disaster recovery / backup server solution</t>
+  </si>
+  <si>
+    <t>Juli Klemm</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Send a note to the caArray community about the 2.4.1 bug.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Andy Evans and Will Fitzhugh</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Complete</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Rashmi Srinivasa</t>
+  </si>
+  <si>
+    <t>Complete</t>
+  </si>
+  <si>
+    <t>Send requirements process to JJ and schedule follow-up meeting.</t>
+  </si>
+  <si>
+    <t>Follow up with Rashmi to see if she can help resolve the problem of running the 508 compliance testing tool against caIntegrator.</t>
+  </si>
+  <si>
+    <t>Quy Phung</t>
+  </si>
+  <si>
+    <t>Tony Kervalage needs list of TRANSCEND requirements and LOE.</t>
+  </si>
+  <si>
+    <t>Rashmi Srinivasa and Shine Jacob</t>
+  </si>
+  <si>
+    <t>Complete</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Set up a meeting to discuss which TCGA data types need to be loaded into caIntegrator. Attendees: Tanya Davidson, Xiaopeng, Juli, Mervi, Shine, JP. (Mervi, Shine and JP all have vacation plans during August.)</t>
+  </si>
+  <si>
+    <t>Complete</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Complete</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Set up an internal meeting to evaluate alternative approaches to setting permissions (common UI versus changes to individual apps)</t>
+  </si>
+  <si>
+    <t>Upgrade Curation tier to caArray 2.4.1.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Don Swan</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Quy Phung</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Follow up with Doug Hosier on BDA-Lite and AntHill Pro 3.0 requirement.</t>
+  </si>
+  <si>
+    <t>Warn caArray community re: planned down time of &lt;1 hour on Thursday at 8am.</t>
+  </si>
+  <si>
+    <t>Juli Klemm and Zhong Li</t>
+  </si>
+  <si>
+    <t>Get modify access to Jira for Jill.</t>
+  </si>
+  <si>
+    <t>Complete</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Set up a meeting to discuss access needs to run caArrayImporter client to load data onto caArray on NCI Production server.</t>
+  </si>
+  <si>
+    <t>JJ Pan</t>
+  </si>
+  <si>
+    <t>Write up a short capability description of caArrayImporter client and QTP for loading large data sets.  Quy and Andrew to support.</t>
+  </si>
+  <si>
+    <t>Write up a requirement for autoloader – short term solution using caArrayImporter or QTP.  Xiaopang to provide input.</t>
+  </si>
+  <si>
+    <t>Complete</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Work with Eve to schedule a meeting with UCSF.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Schedule meeting to discuss TRANSCEND architecture recommendations and effect on caArray and caIntegrator project plans.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Rashmi Srinivasa</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Check with Matt Kennedy and Eve re: getting hardware requirements to UCSF</t>
+  </si>
+  <si>
+    <t>Check with Eve re: bringing back the risk related to unavailability of I-SPY2 data</t>
+  </si>
+  <si>
+    <t>Complete (TRANSCEND-127 is open.)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Complete</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Talk to the UPT team re: dissuading caArray users from creating groups within UPT.</t>
+  </si>
+  <si>
+    <t>Item #</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Provide a list of TCGA data - loadable/not loadable/unknowns and some options</t>
+  </si>
+  <si>
+    <t>Shine Jacob</t>
+  </si>
+  <si>
+    <t>Complete</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Complete</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Get sample data files from Sarah Davis/TRANSCEND team.</t>
+  </si>
+  <si>
+    <t>Create sample experiments in caArray to represent TRANSCEND use cases.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Andy Evans</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Complete</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Complete</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Update permissions wireframes for TRANSCEND to reflect the latest understanding of the data.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Mervi Heiskanen</t>
+  </si>
+  <si>
+    <t>On Hold (I-SPY2 data not yet available)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Complete</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Send the Agilent 415K ADF custom array design to Zhong.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Henry Schaefer</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Shine and Rashmi to provide latest product roadmaps to Zhong for the MAT-KC.</t>
   </si>
 </sst>
 </file>
@@ -842,16 +858,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
-  <dimension ref="A1:E42"/>
+  <dimension ref="A1:E44"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="D31" sqref="D31"/>
+      <selection activeCell="A43" sqref="A43:E44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
   <cols>
     <col min="1" max="1" width="7" style="1" customWidth="1"/>
-    <col min="2" max="2" width="52.140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="57.85546875" style="1" customWidth="1"/>
     <col min="3" max="3" width="47.140625" style="1" customWidth="1"/>
     <col min="4" max="4" width="15.42578125" style="1" customWidth="1"/>
     <col min="5" max="5" width="51.42578125" style="1" customWidth="1"/>
@@ -860,19 +876,19 @@
   <sheetData>
     <row r="1" spans="1:5" s="2" customFormat="1" ht="16" thickBot="1">
       <c r="A1" s="3" t="s">
-        <v>18</v>
+        <v>78</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>19</v>
+        <v>79</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>42</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="31" thickBot="1">
@@ -880,16 +896,16 @@
         <v>1</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>43</v>
+        <v>30</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>58</v>
+        <v>45</v>
       </c>
       <c r="D2" s="7">
         <v>39297</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>59</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="16" thickBot="1">
@@ -897,16 +913,16 @@
         <v>2</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>60</v>
+        <v>47</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>58</v>
+        <v>45</v>
       </c>
       <c r="D3" s="7">
         <v>39297</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>59</v>
+        <v>46</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="31" thickBot="1">
@@ -914,16 +930,16 @@
         <v>3</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>21</v>
+        <v>81</v>
       </c>
       <c r="D4" s="7">
         <v>39297</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>59</v>
+        <v>46</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="46" thickBot="1">
@@ -931,16 +947,16 @@
         <v>4</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>66</v>
+        <v>53</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>30</v>
+        <v>90</v>
       </c>
       <c r="D5" s="7">
         <v>39297</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>59</v>
+        <v>46</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="16" thickBot="1">
@@ -948,16 +964,16 @@
         <v>5</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>83</v>
+        <v>10</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>21</v>
+        <v>81</v>
       </c>
       <c r="D6" s="7">
         <v>39297</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>16</v>
+        <v>76</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="31" thickBot="1">
@@ -965,16 +981,16 @@
         <v>6</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>5</v>
+        <v>65</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>6</v>
+        <v>66</v>
       </c>
       <c r="D7" s="7">
         <v>39309</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>59</v>
+        <v>46</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="31" thickBot="1">
@@ -982,16 +998,16 @@
         <v>7</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>7</v>
+        <v>67</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>58</v>
+        <v>45</v>
       </c>
       <c r="D8" s="7">
         <v>39309</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>59</v>
+        <v>46</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="31" thickBot="1">
@@ -999,16 +1015,16 @@
         <v>8</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>8</v>
+        <v>68</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>58</v>
+        <v>45</v>
       </c>
       <c r="D9" s="7">
         <v>39309</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>59</v>
+        <v>46</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="31" thickBot="1">
@@ -1016,16 +1032,16 @@
         <v>9</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>61</v>
+        <v>48</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
       <c r="D10" s="7">
         <v>39309</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>59</v>
+        <v>46</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="16" thickBot="1">
@@ -1033,16 +1049,16 @@
         <v>10</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>63</v>
+        <v>50</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>73</v>
+        <v>0</v>
       </c>
       <c r="D11" s="7">
         <v>39309</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>9</v>
+        <v>69</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="31" thickBot="1">
@@ -1050,16 +1066,16 @@
         <v>11</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>35</v>
+        <v>95</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>87</v>
+        <v>14</v>
       </c>
       <c r="D12" s="7">
         <v>39316</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>74</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="16" thickBot="1">
@@ -1067,16 +1083,16 @@
         <v>12</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>88</v>
+        <v>15</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>21</v>
+        <v>81</v>
       </c>
       <c r="D13" s="7">
         <v>39323</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>59</v>
+        <v>46</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="16" thickBot="1">
@@ -1084,16 +1100,16 @@
         <v>13</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>89</v>
+        <v>16</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>64</v>
+        <v>51</v>
       </c>
       <c r="D14" s="7">
         <v>39330</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>22</v>
+        <v>82</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="31" thickBot="1">
@@ -1101,33 +1117,33 @@
         <v>14</v>
       </c>
       <c r="B15" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="C15" s="10" t="s">
         <v>17</v>
-      </c>
-      <c r="C15" s="10" t="s">
-        <v>90</v>
       </c>
       <c r="D15" s="11">
         <v>39330</v>
       </c>
       <c r="E15" s="10" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" ht="31" thickBot="1">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="16" thickBot="1">
       <c r="A16" s="5">
         <v>15</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>6</v>
+        <v>66</v>
       </c>
       <c r="D16" s="7">
         <v>39344</v>
       </c>
       <c r="E16" s="6" t="s">
-        <v>57</v>
+        <v>44</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="31" thickBot="1">
@@ -1135,16 +1151,16 @@
         <v>16</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>39</v>
+        <v>26</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>6</v>
+        <v>66</v>
       </c>
       <c r="D17" s="7">
         <v>39344</v>
       </c>
       <c r="E17" s="6" t="s">
-        <v>57</v>
+        <v>44</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="16" thickBot="1">
@@ -1152,16 +1168,16 @@
         <v>17</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>44</v>
+        <v>31</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>71</v>
+        <v>58</v>
       </c>
       <c r="D18" s="7">
         <v>39372</v>
       </c>
       <c r="E18" s="6" t="s">
-        <v>91</v>
+        <v>18</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="16" thickBot="1">
@@ -1169,16 +1185,16 @@
         <v>18</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>70</v>
+        <v>57</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>72</v>
+        <v>59</v>
       </c>
       <c r="D19" s="7">
         <v>39372</v>
       </c>
       <c r="E19" s="6" t="s">
-        <v>67</v>
+        <v>54</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="31" thickBot="1">
@@ -1186,16 +1202,16 @@
         <v>19</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>75</v>
+        <v>2</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>56</v>
+        <v>43</v>
       </c>
       <c r="D20" s="7">
         <v>39372</v>
       </c>
       <c r="E20" s="6" t="s">
-        <v>67</v>
+        <v>54</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="16" thickBot="1">
@@ -1203,16 +1219,16 @@
         <v>20</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>10</v>
+        <v>70</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>47</v>
+        <v>34</v>
       </c>
       <c r="D21" s="7">
         <v>39400</v>
       </c>
       <c r="E21" s="6" t="s">
-        <v>68</v>
+        <v>55</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="31" thickBot="1">
@@ -1220,33 +1236,33 @@
         <v>21</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>48</v>
+        <v>35</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>49</v>
+        <v>36</v>
       </c>
       <c r="D22" s="7">
         <v>39400</v>
       </c>
       <c r="E22" s="6" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" ht="31" thickBot="1">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="16" thickBot="1">
       <c r="A23" s="5">
         <v>22</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>25</v>
+        <v>85</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>50</v>
+        <v>37</v>
       </c>
       <c r="D23" s="7">
         <v>39400</v>
       </c>
       <c r="E23" s="6" t="s">
-        <v>68</v>
+        <v>55</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="31" thickBot="1">
@@ -1254,16 +1270,16 @@
         <v>23</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>29</v>
+        <v>89</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>26</v>
+        <v>86</v>
       </c>
       <c r="D24" s="7">
         <v>39400</v>
       </c>
       <c r="E24" s="6" t="s">
-        <v>27</v>
+        <v>87</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="16" thickBot="1">
@@ -1271,16 +1287,16 @@
         <v>24</v>
       </c>
       <c r="B25" s="10" t="s">
-        <v>45</v>
+        <v>32</v>
       </c>
       <c r="C25" s="10" t="s">
-        <v>73</v>
+        <v>0</v>
       </c>
       <c r="D25" s="11">
         <v>39415</v>
       </c>
       <c r="E25" s="10" t="s">
-        <v>28</v>
+        <v>88</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="16" thickBot="1">
@@ -1288,16 +1304,16 @@
         <v>25</v>
       </c>
       <c r="B26" s="10" t="s">
-        <v>46</v>
+        <v>33</v>
       </c>
       <c r="C26" s="10" t="s">
-        <v>30</v>
+        <v>90</v>
       </c>
       <c r="D26" s="11">
         <v>39421</v>
       </c>
       <c r="E26" s="10" t="s">
-        <v>23</v>
+        <v>83</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="31" thickBot="1">
@@ -1305,16 +1321,16 @@
         <v>26</v>
       </c>
       <c r="B27" s="10" t="s">
-        <v>69</v>
+        <v>56</v>
       </c>
       <c r="C27" s="10" t="s">
-        <v>58</v>
+        <v>45</v>
       </c>
       <c r="D27" s="11">
         <v>39421</v>
       </c>
       <c r="E27" s="10" t="s">
-        <v>23</v>
+        <v>83</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="16" thickBot="1">
@@ -1322,16 +1338,16 @@
         <v>27</v>
       </c>
       <c r="B28" s="12" t="s">
-        <v>24</v>
+        <v>84</v>
       </c>
       <c r="C28" s="13" t="s">
-        <v>84</v>
+        <v>11</v>
       </c>
       <c r="D28" s="14">
         <v>39470</v>
       </c>
       <c r="E28" s="13" t="s">
-        <v>31</v>
+        <v>91</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="91" thickBot="1">
@@ -1339,16 +1355,16 @@
         <v>28</v>
       </c>
       <c r="B29" s="10" t="s">
-        <v>77</v>
+        <v>4</v>
       </c>
       <c r="C29" s="10" t="s">
-        <v>78</v>
+        <v>5</v>
       </c>
       <c r="D29" s="11">
         <v>39470</v>
       </c>
       <c r="E29" s="10" t="s">
-        <v>79</v>
+        <v>6</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="31" thickBot="1">
@@ -1356,33 +1372,33 @@
         <v>29</v>
       </c>
       <c r="B30" s="10" t="s">
-        <v>80</v>
+        <v>7</v>
       </c>
       <c r="C30" s="10" t="s">
-        <v>81</v>
+        <v>8</v>
       </c>
       <c r="D30" s="11">
         <v>39477</v>
       </c>
       <c r="E30" s="10" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" ht="46" thickBot="1">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="31" thickBot="1">
       <c r="A31" s="9">
         <v>30</v>
       </c>
       <c r="B31" s="10" t="s">
-        <v>11</v>
+        <v>71</v>
       </c>
       <c r="C31" s="10" t="s">
-        <v>12</v>
+        <v>72</v>
       </c>
       <c r="D31" s="11">
         <v>39477</v>
       </c>
       <c r="E31" s="10" t="s">
-        <v>32</v>
+        <v>92</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="16" thickBot="1">
@@ -1390,16 +1406,16 @@
         <v>31</v>
       </c>
       <c r="B32" s="10" t="s">
-        <v>33</v>
+        <v>93</v>
       </c>
       <c r="C32" s="10" t="s">
-        <v>34</v>
+        <v>94</v>
       </c>
       <c r="D32" s="11">
         <v>39491</v>
       </c>
       <c r="E32" s="10" t="s">
-        <v>65</v>
+        <v>52</v>
       </c>
     </row>
     <row r="33" spans="1:5" ht="31" thickBot="1">
@@ -1407,16 +1423,16 @@
         <v>32</v>
       </c>
       <c r="B33" s="10" t="s">
-        <v>51</v>
+        <v>38</v>
       </c>
       <c r="C33" s="10" t="s">
-        <v>58</v>
+        <v>45</v>
       </c>
       <c r="D33" s="11">
         <v>39498</v>
       </c>
       <c r="E33" s="10" t="s">
-        <v>59</v>
+        <v>46</v>
       </c>
     </row>
     <row r="34" spans="1:5" ht="16" thickBot="1">
@@ -1424,16 +1440,16 @@
         <v>33</v>
       </c>
       <c r="B34" s="10" t="s">
-        <v>52</v>
+        <v>39</v>
       </c>
       <c r="C34" s="10" t="s">
-        <v>58</v>
+        <v>45</v>
       </c>
       <c r="D34" s="11">
         <v>39498</v>
       </c>
       <c r="E34" s="10" t="s">
-        <v>59</v>
+        <v>46</v>
       </c>
     </row>
     <row r="35" spans="1:5" ht="16" thickBot="1">
@@ -1441,16 +1457,16 @@
         <v>34</v>
       </c>
       <c r="B35" s="10" t="s">
-        <v>53</v>
+        <v>40</v>
       </c>
       <c r="C35" s="10" t="s">
-        <v>37</v>
+        <v>24</v>
       </c>
       <c r="D35" s="11">
         <v>39505</v>
       </c>
       <c r="E35" s="10" t="s">
-        <v>4</v>
+        <v>64</v>
       </c>
     </row>
     <row r="36" spans="1:5" ht="16" thickBot="1">
@@ -1458,16 +1474,16 @@
         <v>35</v>
       </c>
       <c r="B36" s="10" t="s">
-        <v>38</v>
+        <v>25</v>
       </c>
       <c r="C36" s="10" t="s">
-        <v>30</v>
+        <v>90</v>
       </c>
       <c r="D36" s="11">
         <v>39505</v>
       </c>
       <c r="E36" s="10" t="s">
-        <v>59</v>
+        <v>46</v>
       </c>
     </row>
     <row r="37" spans="1:5" ht="31" thickBot="1">
@@ -1475,16 +1491,16 @@
         <v>36</v>
       </c>
       <c r="B37" s="10" t="s">
-        <v>1</v>
+        <v>61</v>
       </c>
       <c r="C37" s="10" t="s">
-        <v>2</v>
+        <v>62</v>
       </c>
       <c r="D37" s="11">
         <v>39512</v>
       </c>
       <c r="E37" s="10" t="s">
-        <v>59</v>
+        <v>46</v>
       </c>
     </row>
     <row r="38" spans="1:5" ht="16" thickBot="1">
@@ -1492,16 +1508,16 @@
         <v>37</v>
       </c>
       <c r="B38" s="10" t="s">
-        <v>3</v>
+        <v>63</v>
       </c>
       <c r="C38" s="10" t="s">
-        <v>58</v>
+        <v>45</v>
       </c>
       <c r="D38" s="11">
         <v>39512</v>
       </c>
       <c r="E38" s="10" t="s">
-        <v>59</v>
+        <v>46</v>
       </c>
     </row>
     <row r="39" spans="1:5" ht="16" thickBot="1">
@@ -1509,16 +1525,16 @@
         <v>38</v>
       </c>
       <c r="B39" s="10" t="s">
-        <v>86</v>
+        <v>13</v>
       </c>
       <c r="C39" s="10" t="s">
-        <v>85</v>
+        <v>12</v>
       </c>
       <c r="D39" s="11">
         <v>39533</v>
       </c>
       <c r="E39" s="10" t="s">
-        <v>36</v>
+        <v>23</v>
       </c>
     </row>
     <row r="40" spans="1:5" ht="16" thickBot="1">
@@ -1526,33 +1542,33 @@
         <v>39</v>
       </c>
       <c r="B40" s="10" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="C40" s="10" t="s">
-        <v>54</v>
+        <v>41</v>
       </c>
       <c r="D40" s="11">
         <v>39547</v>
       </c>
       <c r="E40" s="10" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" ht="31" thickBot="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" ht="16" thickBot="1">
       <c r="A41" s="9">
         <v>40</v>
       </c>
       <c r="B41" s="10" t="s">
-        <v>13</v>
+        <v>73</v>
       </c>
       <c r="C41" s="10" t="s">
-        <v>58</v>
+        <v>45</v>
       </c>
       <c r="D41" s="11">
         <v>39554</v>
       </c>
       <c r="E41" s="10" t="s">
-        <v>59</v>
+        <v>46</v>
       </c>
     </row>
     <row r="42" spans="1:5" ht="31" thickBot="1">
@@ -1560,16 +1576,50 @@
         <v>41</v>
       </c>
       <c r="B42" s="10" t="s">
-        <v>14</v>
+        <v>74</v>
       </c>
       <c r="C42" s="10" t="s">
-        <v>58</v>
+        <v>45</v>
       </c>
       <c r="D42" s="11">
         <v>39554</v>
       </c>
       <c r="E42" s="10" t="s">
-        <v>15</v>
+        <v>75</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" ht="16" thickBot="1">
+      <c r="A43" s="8">
+        <v>42</v>
+      </c>
+      <c r="B43" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="C43" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="D43" s="14">
+        <v>39575</v>
+      </c>
+      <c r="E43" s="13" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" ht="16" thickBot="1">
+      <c r="A44" s="8">
+        <v>43</v>
+      </c>
+      <c r="B44" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="C44" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="D44" s="14">
+        <v>39575</v>
+      </c>
+      <c r="E44" s="13" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated status of action items.
</commit_message>
<xml_diff>
--- a/project_management/caArray_caIntegrator_Action_Items.xlsx
+++ b/project_management/caArray_caIntegrator_Action_Items.xlsx
@@ -19,18 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="96">
-  <si>
-    <t>Eve Shalley</t>
-  </si>
-  <si>
-    <t>Complete</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Create wireframes to depict how permissions will work across caIntegrator and caArray.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="105">
   <si>
     <t>Complete (Not required)</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -99,10 +88,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>Not Started</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>Send information to Mervi about user/lab who is installing caIntegrator.</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -153,7 +138,257 @@
     <t>Links to the caArray User’s Guide on the Download Center -&gt; Download page are incorrect</t>
   </si>
   <si>
+    <t>Complete</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Submit ticket for BDALite configuration on the new STAGE tier</t>
+  </si>
+  <si>
+    <t>Discuss need for disaster recovery / backup server solution</t>
+  </si>
+  <si>
+    <t>Juli Klemm</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Send a note to the caArray community about the 2.4.1 bug.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Andy Evans and Will Fitzhugh</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Complete</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
     <t>Rashmi Srinivasa</t>
+  </si>
+  <si>
+    <t>Complete</t>
+  </si>
+  <si>
+    <t>Send requirements process to JJ and schedule follow-up meeting.</t>
+  </si>
+  <si>
+    <t>Follow up with Rashmi to see if she can help resolve the problem of running the 508 compliance testing tool against caIntegrator.</t>
+  </si>
+  <si>
+    <t>Quy Phung</t>
+  </si>
+  <si>
+    <t>Tony Kervalage needs list of TRANSCEND requirements and LOE.</t>
+  </si>
+  <si>
+    <t>Rashmi Srinivasa and Shine Jacob</t>
+  </si>
+  <si>
+    <t>Complete</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Set up a meeting to discuss which TCGA data types need to be loaded into caIntegrator. Attendees: Tanya Davidson, Xiaopeng, Juli, Mervi, Shine, JP. (Mervi, Shine and JP all have vacation plans during August.)</t>
+  </si>
+  <si>
+    <t>Complete</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Complete</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Set up an internal meeting to evaluate alternative approaches to setting permissions (common UI versus changes to individual apps)</t>
+  </si>
+  <si>
+    <t>Upgrade Curation tier to caArray 2.4.1.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Don Swan</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Quy Phung</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Follow up with Doug Hosier on BDA-Lite and AntHill Pro 3.0 requirement.</t>
+  </si>
+  <si>
+    <t>Warn caArray community re: planned down time of &lt;1 hour on Thursday at 8am.</t>
+  </si>
+  <si>
+    <t>Juli Klemm and Zhong Li</t>
+  </si>
+  <si>
+    <t>Get modify access to Jira for Jill.</t>
+  </si>
+  <si>
+    <t>Complete</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Set up a meeting to discuss access needs to run caArrayImporter client to load data onto caArray on NCI Production server.</t>
+  </si>
+  <si>
+    <t>JJ Pan</t>
+  </si>
+  <si>
+    <t>Write up a short capability description of caArrayImporter client and QTP for loading large data sets.  Quy and Andrew to support.</t>
+  </si>
+  <si>
+    <t>Write up a requirement for autoloader – short term solution using caArrayImporter or QTP.  Xiaopang to provide input.</t>
+  </si>
+  <si>
+    <t>Complete</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Eve Shalley</t>
+  </si>
+  <si>
+    <t>Complete</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Create wireframes to depict how permissions will work across caIntegrator and caArray.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Quy Phung and Henry Schaefer</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Work with Eve to schedule a meeting with UCSF.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Schedule meeting to discuss TRANSCEND architecture recommendations and effect on caArray and caIntegrator project plans.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Rashmi Srinivasa</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Check with Matt Kennedy and Eve re: getting hardware requirements to UCSF</t>
+  </si>
+  <si>
+    <t>Check with Eve re: bringing back the risk related to unavailability of I-SPY2 data</t>
+  </si>
+  <si>
+    <t>Complete (TRANSCEND-127 is open.)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Complete</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Talk to the UPT team re: dissuading caArray users from creating groups within UPT.</t>
+  </si>
+  <si>
+    <t>Item #</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Provide a list of TCGA data - loadable/not loadable/unknowns and some options</t>
+  </si>
+  <si>
+    <t>Shine Jacob</t>
+  </si>
+  <si>
+    <t>Complete</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Complete</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Get sample data files from Sarah Davis/TRANSCEND team.</t>
+  </si>
+  <si>
+    <t>Create sample experiments in caArray to represent TRANSCEND use cases.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Andy Evans</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Complete</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Complete</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Update permissions wireframes for TRANSCEND to reflect the latest understanding of the data.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Mervi Heiskanen</t>
+  </si>
+  <si>
+    <t>On Hold (I-SPY2 data not yet available)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Complete</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Send the Agilent 415K ADF custom array design to Zhong.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Henry Schaefer</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Shine and Rashmi to provide latest product roadmaps to Zhong for the MAT-KC.</t>
+  </si>
+  <si>
+    <t>Talk to Sudha re: QA backup during Quy’s absence in the end of July.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Quy Phung and Rashmi Srinivasa</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Complete</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Complete</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Send TRANSCEND Use Cases document to JJ and Deb.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Rashmi Srinivasa</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Confirm with Jill regarding the documentation updates for caArray.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Review Test Plan for SSO and Non-SSO.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Rashmi Srinivasa</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
@@ -162,217 +397,12 @@
   </si>
   <si>
     <t>Send triaged bug list to Juli, JJ, Deb and Larry and schedule a second Bug Triage meeting.</t>
-  </si>
-  <si>
-    <t>Submit ticket for BDALite configuration on the new STAGE tier</t>
-  </si>
-  <si>
-    <t>Discuss need for disaster recovery / backup server solution</t>
-  </si>
-  <si>
-    <t>Juli Klemm</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Send a note to the caArray community about the 2.4.1 bug.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Andy Evans and Will Fitzhugh</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Complete</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Rashmi Srinivasa</t>
-  </si>
-  <si>
-    <t>Complete</t>
-  </si>
-  <si>
-    <t>Send requirements process to JJ and schedule follow-up meeting.</t>
-  </si>
-  <si>
-    <t>Follow up with Rashmi to see if she can help resolve the problem of running the 508 compliance testing tool against caIntegrator.</t>
-  </si>
-  <si>
-    <t>Quy Phung</t>
-  </si>
-  <si>
-    <t>Tony Kervalage needs list of TRANSCEND requirements and LOE.</t>
-  </si>
-  <si>
-    <t>Rashmi Srinivasa and Shine Jacob</t>
-  </si>
-  <si>
-    <t>Complete</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Set up a meeting to discuss which TCGA data types need to be loaded into caIntegrator. Attendees: Tanya Davidson, Xiaopeng, Juli, Mervi, Shine, JP. (Mervi, Shine and JP all have vacation plans during August.)</t>
-  </si>
-  <si>
-    <t>Complete</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Complete</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Set up an internal meeting to evaluate alternative approaches to setting permissions (common UI versus changes to individual apps)</t>
-  </si>
-  <si>
-    <t>Upgrade Curation tier to caArray 2.4.1.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Don Swan</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Quy Phung</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Follow up with Doug Hosier on BDA-Lite and AntHill Pro 3.0 requirement.</t>
-  </si>
-  <si>
-    <t>Warn caArray community re: planned down time of &lt;1 hour on Thursday at 8am.</t>
-  </si>
-  <si>
-    <t>Juli Klemm and Zhong Li</t>
-  </si>
-  <si>
-    <t>Get modify access to Jira for Jill.</t>
-  </si>
-  <si>
-    <t>Complete</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Set up a meeting to discuss access needs to run caArrayImporter client to load data onto caArray on NCI Production server.</t>
-  </si>
-  <si>
-    <t>JJ Pan</t>
-  </si>
-  <si>
-    <t>Write up a short capability description of caArrayImporter client and QTP for loading large data sets.  Quy and Andrew to support.</t>
-  </si>
-  <si>
-    <t>Write up a requirement for autoloader – short term solution using caArrayImporter or QTP.  Xiaopang to provide input.</t>
-  </si>
-  <si>
-    <t>Complete</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Work with Eve to schedule a meeting with UCSF.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Schedule meeting to discuss TRANSCEND architecture recommendations and effect on caArray and caIntegrator project plans.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Rashmi Srinivasa</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Check with Matt Kennedy and Eve re: getting hardware requirements to UCSF</t>
-  </si>
-  <si>
-    <t>Check with Eve re: bringing back the risk related to unavailability of I-SPY2 data</t>
-  </si>
-  <si>
-    <t>Complete (TRANSCEND-127 is open.)</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Complete</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Talk to the UPT team re: dissuading caArray users from creating groups within UPT.</t>
-  </si>
-  <si>
-    <t>Item #</t>
-  </si>
-  <si>
-    <t>Description</t>
-  </si>
-  <si>
-    <t>Provide a list of TCGA data - loadable/not loadable/unknowns and some options</t>
-  </si>
-  <si>
-    <t>Shine Jacob</t>
-  </si>
-  <si>
-    <t>Complete</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Complete</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Get sample data files from Sarah Davis/TRANSCEND team.</t>
-  </si>
-  <si>
-    <t>Create sample experiments in caArray to represent TRANSCEND use cases.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Andy Evans</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Complete</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Complete</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Update permissions wireframes for TRANSCEND to reflect the latest understanding of the data.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Mervi Heiskanen</t>
-  </si>
-  <si>
-    <t>On Hold (I-SPY2 data not yet available)</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Complete</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Send the Agilent 415K ADF custom array design to Zhong.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Henry Schaefer</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Shine and Rashmi to provide latest product roadmaps to Zhong for the MAT-KC.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-  </numFmts>
   <fonts count="6">
     <font>
       <sz val="10"/>
@@ -858,10 +888,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
-  <dimension ref="A1:E44"/>
+  <dimension ref="A1:E48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="A43" sqref="A43:E44"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="A48" sqref="A48:XFD48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -876,19 +906,19 @@
   <sheetData>
     <row r="1" spans="1:5" s="2" customFormat="1" ht="16" thickBot="1">
       <c r="A1" s="3" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="31" thickBot="1">
@@ -896,16 +926,16 @@
         <v>1</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="D2" s="7">
         <v>39297</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="16" thickBot="1">
@@ -913,16 +943,16 @@
         <v>2</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="D3" s="7">
         <v>39297</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="31" thickBot="1">
@@ -930,16 +960,16 @@
         <v>3</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D4" s="7">
         <v>39297</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="46" thickBot="1">
@@ -947,16 +977,16 @@
         <v>4</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D5" s="7">
         <v>39297</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="16" thickBot="1">
@@ -964,16 +994,16 @@
         <v>5</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D6" s="7">
         <v>39297</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="31" thickBot="1">
@@ -981,16 +1011,16 @@
         <v>6</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="D7" s="7">
         <v>39309</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="31" thickBot="1">
@@ -998,16 +1028,16 @@
         <v>7</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="D8" s="7">
         <v>39309</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="31" thickBot="1">
@@ -1015,16 +1045,16 @@
         <v>8</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="D9" s="7">
         <v>39309</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="31" thickBot="1">
@@ -1032,16 +1062,16 @@
         <v>9</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="D10" s="7">
         <v>39309</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="16" thickBot="1">
@@ -1049,16 +1079,16 @@
         <v>10</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>0</v>
+        <v>64</v>
       </c>
       <c r="D11" s="7">
         <v>39309</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="31" thickBot="1">
@@ -1066,16 +1096,16 @@
         <v>11</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D12" s="7">
         <v>39316</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>1</v>
+        <v>65</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="16" thickBot="1">
@@ -1083,16 +1113,16 @@
         <v>12</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D13" s="7">
         <v>39323</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="16" thickBot="1">
@@ -1100,16 +1130,16 @@
         <v>13</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="D14" s="7">
         <v>39330</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="31" thickBot="1">
@@ -1117,16 +1147,16 @@
         <v>14</v>
       </c>
       <c r="B15" s="10" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C15" s="10" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="D15" s="11">
         <v>39330</v>
       </c>
       <c r="E15" s="10" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="16" thickBot="1">
@@ -1134,16 +1164,16 @@
         <v>15</v>
       </c>
       <c r="B16" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="C16" s="6" t="s">
         <v>60</v>
-      </c>
-      <c r="C16" s="6" t="s">
-        <v>66</v>
       </c>
       <c r="D16" s="7">
         <v>39344</v>
       </c>
       <c r="E16" s="6" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="31" thickBot="1">
@@ -1151,16 +1181,16 @@
         <v>16</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="D17" s="7">
         <v>39344</v>
       </c>
       <c r="E17" s="6" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="16" thickBot="1">
@@ -1168,16 +1198,16 @@
         <v>17</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="D18" s="7">
         <v>39372</v>
       </c>
       <c r="E18" s="6" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="16" thickBot="1">
@@ -1185,16 +1215,16 @@
         <v>18</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="D19" s="7">
         <v>39372</v>
       </c>
       <c r="E19" s="6" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="31" thickBot="1">
@@ -1202,16 +1232,16 @@
         <v>19</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>2</v>
+        <v>66</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="D20" s="7">
         <v>39372</v>
       </c>
       <c r="E20" s="6" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="16" thickBot="1">
@@ -1219,16 +1249,16 @@
         <v>20</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="D21" s="7">
         <v>39400</v>
       </c>
       <c r="E21" s="6" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="31" thickBot="1">
@@ -1236,16 +1266,16 @@
         <v>21</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>36</v>
+        <v>102</v>
       </c>
       <c r="D22" s="7">
         <v>39400</v>
       </c>
       <c r="E22" s="6" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="16" thickBot="1">
@@ -1253,16 +1283,16 @@
         <v>22</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>37</v>
+        <v>103</v>
       </c>
       <c r="D23" s="7">
         <v>39400</v>
       </c>
       <c r="E23" s="6" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="31" thickBot="1">
@@ -1270,16 +1300,16 @@
         <v>23</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D24" s="7">
         <v>39400</v>
       </c>
       <c r="E24" s="6" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="16" thickBot="1">
@@ -1287,16 +1317,16 @@
         <v>24</v>
       </c>
       <c r="B25" s="10" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C25" s="10" t="s">
-        <v>0</v>
+        <v>64</v>
       </c>
       <c r="D25" s="11">
         <v>39415</v>
       </c>
       <c r="E25" s="10" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="16" thickBot="1">
@@ -1304,16 +1334,16 @@
         <v>25</v>
       </c>
       <c r="B26" s="10" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C26" s="10" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D26" s="11">
         <v>39421</v>
       </c>
       <c r="E26" s="10" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="31" thickBot="1">
@@ -1321,16 +1351,16 @@
         <v>26</v>
       </c>
       <c r="B27" s="10" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="C27" s="10" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="D27" s="11">
         <v>39421</v>
       </c>
       <c r="E27" s="10" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="16" thickBot="1">
@@ -1338,16 +1368,16 @@
         <v>27</v>
       </c>
       <c r="B28" s="12" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C28" s="13" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="D28" s="14">
         <v>39470</v>
       </c>
       <c r="E28" s="13" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="91" thickBot="1">
@@ -1355,16 +1385,16 @@
         <v>28</v>
       </c>
       <c r="B29" s="10" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C29" s="10" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D29" s="11">
         <v>39470</v>
       </c>
       <c r="E29" s="10" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="31" thickBot="1">
@@ -1372,16 +1402,16 @@
         <v>29</v>
       </c>
       <c r="B30" s="10" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C30" s="10" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D30" s="11">
         <v>39477</v>
       </c>
       <c r="E30" s="10" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="31" thickBot="1">
@@ -1389,16 +1419,16 @@
         <v>30</v>
       </c>
       <c r="B31" s="10" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C31" s="10" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D31" s="11">
         <v>39477</v>
       </c>
       <c r="E31" s="10" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="16" thickBot="1">
@@ -1406,16 +1436,16 @@
         <v>31</v>
       </c>
       <c r="B32" s="10" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C32" s="10" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D32" s="11">
         <v>39491</v>
       </c>
       <c r="E32" s="10" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
     </row>
     <row r="33" spans="1:5" ht="31" thickBot="1">
@@ -1423,16 +1453,16 @@
         <v>32</v>
       </c>
       <c r="B33" s="10" t="s">
-        <v>38</v>
+        <v>104</v>
       </c>
       <c r="C33" s="10" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="D33" s="11">
         <v>39498</v>
       </c>
       <c r="E33" s="10" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
     </row>
     <row r="34" spans="1:5" ht="16" thickBot="1">
@@ -1440,16 +1470,16 @@
         <v>33</v>
       </c>
       <c r="B34" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="C34" s="10" t="s">
         <v>39</v>
-      </c>
-      <c r="C34" s="10" t="s">
-        <v>45</v>
       </c>
       <c r="D34" s="11">
         <v>39498</v>
       </c>
       <c r="E34" s="10" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
     </row>
     <row r="35" spans="1:5" ht="16" thickBot="1">
@@ -1457,16 +1487,16 @@
         <v>34</v>
       </c>
       <c r="B35" s="10" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="C35" s="10" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="D35" s="11">
         <v>39505</v>
       </c>
       <c r="E35" s="10" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
     </row>
     <row r="36" spans="1:5" ht="16" thickBot="1">
@@ -1474,16 +1504,16 @@
         <v>35</v>
       </c>
       <c r="B36" s="10" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C36" s="10" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D36" s="11">
         <v>39505</v>
       </c>
       <c r="E36" s="10" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
     </row>
     <row r="37" spans="1:5" ht="31" thickBot="1">
@@ -1491,16 +1521,16 @@
         <v>36</v>
       </c>
       <c r="B37" s="10" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="C37" s="10" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="D37" s="11">
         <v>39512</v>
       </c>
       <c r="E37" s="10" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
     </row>
     <row r="38" spans="1:5" ht="16" thickBot="1">
@@ -1508,16 +1538,16 @@
         <v>37</v>
       </c>
       <c r="B38" s="10" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="C38" s="10" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="D38" s="11">
         <v>39512</v>
       </c>
       <c r="E38" s="10" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
     </row>
     <row r="39" spans="1:5" ht="16" thickBot="1">
@@ -1525,16 +1555,16 @@
         <v>38</v>
       </c>
       <c r="B39" s="10" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C39" s="10" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D39" s="11">
         <v>39533</v>
       </c>
       <c r="E39" s="10" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
     </row>
     <row r="40" spans="1:5" ht="16" thickBot="1">
@@ -1542,16 +1572,16 @@
         <v>39</v>
       </c>
       <c r="B40" s="10" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="C40" s="10" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="D40" s="11">
         <v>39547</v>
       </c>
       <c r="E40" s="10" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="41" spans="1:5" ht="16" thickBot="1">
@@ -1559,16 +1589,16 @@
         <v>40</v>
       </c>
       <c r="B41" s="10" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C41" s="10" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="D41" s="11">
         <v>39554</v>
       </c>
       <c r="E41" s="10" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
     </row>
     <row r="42" spans="1:5" ht="31" thickBot="1">
@@ -1576,53 +1606,122 @@
         <v>41</v>
       </c>
       <c r="B42" s="10" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C42" s="10" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="D42" s="11">
         <v>39554</v>
       </c>
       <c r="E42" s="10" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="43" spans="1:5" ht="16" thickBot="1">
-      <c r="A43" s="8">
+      <c r="A43" s="9">
         <v>42</v>
       </c>
-      <c r="B43" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="C43" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="D43" s="14">
+      <c r="B43" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="C43" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="D43" s="11">
         <v>39575</v>
       </c>
-      <c r="E43" s="13" t="s">
-        <v>20</v>
+      <c r="E43" s="10" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="44" spans="1:5" ht="16" thickBot="1">
-      <c r="A44" s="8">
+      <c r="A44" s="9">
         <v>43</v>
       </c>
-      <c r="B44" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="C44" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="D44" s="14">
+      <c r="B44" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="C44" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="D44" s="11">
         <v>39575</v>
       </c>
-      <c r="E44" s="13" t="s">
-        <v>20</v>
+      <c r="E44" s="10" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" ht="16" thickBot="1">
+      <c r="A45" s="9">
+        <v>44</v>
+      </c>
+      <c r="B45" s="10" t="s">
+        <v>94</v>
+      </c>
+      <c r="C45" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="D45" s="11">
+        <v>39582</v>
+      </c>
+      <c r="E45" s="10" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" ht="16" thickBot="1">
+      <c r="A46" s="9">
+        <v>45</v>
+      </c>
+      <c r="B46" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="C46" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="D46" s="11">
+        <v>39589</v>
+      </c>
+      <c r="E46" s="10" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" ht="16" thickBot="1">
+      <c r="A47" s="9">
+        <v>46</v>
+      </c>
+      <c r="B47" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="C47" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="D47" s="11">
+        <v>39596</v>
+      </c>
+      <c r="E47" s="10" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" ht="16" thickBot="1">
+      <c r="A48" s="9">
+        <v>47</v>
+      </c>
+      <c r="B48" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="C48" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="D48" s="11">
+        <v>39596</v>
+      </c>
+      <c r="E48" s="10" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>
+  <sheetCalcPr fullCalcOnLoad="1"/>
   <sortState ref="A2:H13">
     <sortCondition ref="D3:D13"/>
     <sortCondition ref="E3:E13"/>
@@ -1630,7 +1729,6 @@
   </sortState>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
Updated action items based on status meeting.
</commit_message>
<xml_diff>
--- a/project_management/caArray_caIntegrator_Action_Items.xlsx
+++ b/project_management/caArray_caIntegrator_Action_Items.xlsx
@@ -19,7 +19,274 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="110">
+  <si>
+    <t>Send NCI-Frederick caIntegrator user contact info to Larry Brem.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Don Swan</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Schedule meeting to discuss TRANSCEND architecture recommendations and effect on caArray and caIntegrator project plans.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Rashmi Srinivasa</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Check with Matt Kennedy and Eve re: getting hardware requirements to UCSF</t>
+  </si>
+  <si>
+    <t>Check with Eve re: bringing back the risk related to unavailability of I-SPY2 data</t>
+  </si>
+  <si>
+    <t>Complete (TRANSCEND-127 is open.)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Complete</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Talk to the UPT team re: dissuading caArray users from creating groups within UPT.</t>
+  </si>
+  <si>
+    <t>Item #</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Provide a list of TCGA data - loadable/not loadable/unknowns and some options</t>
+  </si>
+  <si>
+    <t>Shine Jacob</t>
+  </si>
+  <si>
+    <t>Complete</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Complete</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Get sample data files from Sarah Davis/TRANSCEND team.</t>
+  </si>
+  <si>
+    <t>Create sample experiments in caArray to represent TRANSCEND use cases.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Andy Evans</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Complete</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Complete</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Update permissions wireframes for TRANSCEND to reflect the latest understanding of the data.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Mervi Heiskanen</t>
+  </si>
+  <si>
+    <t>On Hold (I-SPY2 data not yet available)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Complete</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Send the Agilent 415K ADF custom array design to Zhong.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Henry Schaefer</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Shine and Rashmi to provide latest product roadmaps to Zhong for the MAT-KC.</t>
+  </si>
+  <si>
+    <t>Talk to Sudha re: QA backup during Quy’s absence in the end of July.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Quy Phung and Rashmi Srinivasa</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Complete</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Complete</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Send TRANSCEND Use Cases document to JJ and Deb.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Rashmi Srinivasa</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Confirm with Jill regarding the documentation updates for caArray.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Review Test Plan for SSO and Non-SSO.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Rashmi Srinivasa</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Maureen Colbert</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Send triaged bug list to Juli, JJ, Deb and Larry and schedule a second Bug Triage meeting.</t>
+  </si>
+  <si>
+    <t>Send caIntegrator bug estimates to JJ and Mervi</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Shine</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Not Started</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Send a note to the caArray community about the 2.4.1 bug.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Andy Evans and Will Fitzhugh</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Complete</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Rashmi Srinivasa</t>
+  </si>
+  <si>
+    <t>Complete</t>
+  </si>
+  <si>
+    <t>Send requirements process to JJ and schedule follow-up meeting.</t>
+  </si>
+  <si>
+    <t>Follow up with Rashmi to see if she can help resolve the problem of running the 508 compliance testing tool against caIntegrator.</t>
+  </si>
+  <si>
+    <t>Quy Phung</t>
+  </si>
+  <si>
+    <t>Tony Kervalage needs list of TRANSCEND requirements and LOE.</t>
+  </si>
+  <si>
+    <t>Rashmi Srinivasa and Shine Jacob</t>
+  </si>
+  <si>
+    <t>Complete</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Set up a meeting to discuss which TCGA data types need to be loaded into caIntegrator. Attendees: Tanya Davidson, Xiaopeng, Juli, Mervi, Shine, JP. (Mervi, Shine and JP all have vacation plans during August.)</t>
+  </si>
+  <si>
+    <t>Complete</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Complete</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Set up an internal meeting to evaluate alternative approaches to setting permissions (common UI versus changes to individual apps)</t>
+  </si>
+  <si>
+    <t>Upgrade Curation tier to caArray 2.4.1.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Don Swan</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Quy Phung</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Follow up with Doug Hosier on BDA-Lite and AntHill Pro 3.0 requirement.</t>
+  </si>
+  <si>
+    <t>Warn caArray community re: planned down time of &lt;1 hour on Thursday at 8am.</t>
+  </si>
+  <si>
+    <t>Juli Klemm and Zhong Li</t>
+  </si>
+  <si>
+    <t>Get modify access to Jira for Jill.</t>
+  </si>
+  <si>
+    <t>Complete</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Set up a meeting to discuss access needs to run caArrayImporter client to load data onto caArray on NCI Production server.</t>
+  </si>
+  <si>
+    <t>JJ Pan</t>
+  </si>
+  <si>
+    <t>Write up a short capability description of caArrayImporter client and QTP for loading large data sets.  Quy and Andrew to support.</t>
+  </si>
+  <si>
+    <t>Write up a requirement for autoloader – short term solution using caArrayImporter or QTP.  Xiaopang to provide input.</t>
+  </si>
+  <si>
+    <t>Complete</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Eve Shalley</t>
+  </si>
+  <si>
+    <t>Complete</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Create wireframes to depict how permissions will work across caIntegrator and caArray.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Quy Phung and Henry Schaefer</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Work with Eve to schedule a meeting with UCSF.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
   <si>
     <t>Complete (Not required)</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -150,259 +417,18 @@
   <si>
     <t>Juli Klemm</t>
     <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Send a note to the caArray community about the 2.4.1 bug.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Andy Evans and Will Fitzhugh</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Complete</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Rashmi Srinivasa</t>
-  </si>
-  <si>
-    <t>Complete</t>
-  </si>
-  <si>
-    <t>Send requirements process to JJ and schedule follow-up meeting.</t>
-  </si>
-  <si>
-    <t>Follow up with Rashmi to see if she can help resolve the problem of running the 508 compliance testing tool against caIntegrator.</t>
-  </si>
-  <si>
-    <t>Quy Phung</t>
-  </si>
-  <si>
-    <t>Tony Kervalage needs list of TRANSCEND requirements and LOE.</t>
-  </si>
-  <si>
-    <t>Rashmi Srinivasa and Shine Jacob</t>
-  </si>
-  <si>
-    <t>Complete</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Set up a meeting to discuss which TCGA data types need to be loaded into caIntegrator. Attendees: Tanya Davidson, Xiaopeng, Juli, Mervi, Shine, JP. (Mervi, Shine and JP all have vacation plans during August.)</t>
-  </si>
-  <si>
-    <t>Complete</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Complete</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Set up an internal meeting to evaluate alternative approaches to setting permissions (common UI versus changes to individual apps)</t>
-  </si>
-  <si>
-    <t>Upgrade Curation tier to caArray 2.4.1.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Don Swan</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Quy Phung</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Follow up with Doug Hosier on BDA-Lite and AntHill Pro 3.0 requirement.</t>
-  </si>
-  <si>
-    <t>Warn caArray community re: planned down time of &lt;1 hour on Thursday at 8am.</t>
-  </si>
-  <si>
-    <t>Juli Klemm and Zhong Li</t>
-  </si>
-  <si>
-    <t>Get modify access to Jira for Jill.</t>
-  </si>
-  <si>
-    <t>Complete</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Set up a meeting to discuss access needs to run caArrayImporter client to load data onto caArray on NCI Production server.</t>
-  </si>
-  <si>
-    <t>JJ Pan</t>
-  </si>
-  <si>
-    <t>Write up a short capability description of caArrayImporter client and QTP for loading large data sets.  Quy and Andrew to support.</t>
-  </si>
-  <si>
-    <t>Write up a requirement for autoloader – short term solution using caArrayImporter or QTP.  Xiaopang to provide input.</t>
-  </si>
-  <si>
-    <t>Complete</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Eve Shalley</t>
-  </si>
-  <si>
-    <t>Complete</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Create wireframes to depict how permissions will work across caIntegrator and caArray.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Quy Phung and Henry Schaefer</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Work with Eve to schedule a meeting with UCSF.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Schedule meeting to discuss TRANSCEND architecture recommendations and effect on caArray and caIntegrator project plans.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Rashmi Srinivasa</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Check with Matt Kennedy and Eve re: getting hardware requirements to UCSF</t>
-  </si>
-  <si>
-    <t>Check with Eve re: bringing back the risk related to unavailability of I-SPY2 data</t>
-  </si>
-  <si>
-    <t>Complete (TRANSCEND-127 is open.)</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Complete</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Talk to the UPT team re: dissuading caArray users from creating groups within UPT.</t>
-  </si>
-  <si>
-    <t>Item #</t>
-  </si>
-  <si>
-    <t>Description</t>
-  </si>
-  <si>
-    <t>Provide a list of TCGA data - loadable/not loadable/unknowns and some options</t>
-  </si>
-  <si>
-    <t>Shine Jacob</t>
-  </si>
-  <si>
-    <t>Complete</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Complete</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Get sample data files from Sarah Davis/TRANSCEND team.</t>
-  </si>
-  <si>
-    <t>Create sample experiments in caArray to represent TRANSCEND use cases.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Andy Evans</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Complete</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Complete</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Update permissions wireframes for TRANSCEND to reflect the latest understanding of the data.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Mervi Heiskanen</t>
-  </si>
-  <si>
-    <t>On Hold (I-SPY2 data not yet available)</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Complete</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Send the Agilent 415K ADF custom array design to Zhong.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Henry Schaefer</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Shine and Rashmi to provide latest product roadmaps to Zhong for the MAT-KC.</t>
-  </si>
-  <si>
-    <t>Talk to Sudha re: QA backup during Quy’s absence in the end of July.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Quy Phung and Rashmi Srinivasa</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Complete</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Complete</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Send TRANSCEND Use Cases document to JJ and Deb.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Rashmi Srinivasa</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Confirm with Jill regarding the documentation updates for caArray.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Review Test Plan for SSO and Non-SSO.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Rashmi Srinivasa</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Maureen Colbert</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Send triaged bug list to Juli, JJ, Deb and Larry and schedule a second Bug Triage meeting.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+  </numFmts>
   <fonts count="6">
     <font>
       <sz val="10"/>
@@ -888,10 +914,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
-  <dimension ref="A1:E48"/>
+  <dimension ref="A1:E50"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="A48" sqref="A48:XFD48"/>
+      <selection activeCell="A49" sqref="A49:E50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -906,19 +932,19 @@
   <sheetData>
     <row r="1" spans="1:5" s="2" customFormat="1" ht="16" thickBot="1">
       <c r="A1" s="3" t="s">
-        <v>76</v>
+        <v>9</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>77</v>
+        <v>10</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>23</v>
+        <v>97</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>24</v>
+        <v>98</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>25</v>
+        <v>99</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="31" thickBot="1">
@@ -926,16 +952,16 @@
         <v>1</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>26</v>
+        <v>100</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="D2" s="7">
         <v>39297</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="16" thickBot="1">
@@ -943,16 +969,16 @@
         <v>2</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="D3" s="7">
         <v>39297</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="31" thickBot="1">
@@ -960,16 +986,16 @@
         <v>3</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>78</v>
+        <v>11</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>79</v>
+        <v>12</v>
       </c>
       <c r="D4" s="7">
         <v>39297</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="46" thickBot="1">
@@ -977,16 +1003,16 @@
         <v>4</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>88</v>
+        <v>21</v>
       </c>
       <c r="D5" s="7">
         <v>39297</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="16" thickBot="1">
@@ -994,16 +1020,16 @@
         <v>5</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>7</v>
+        <v>81</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>79</v>
+        <v>12</v>
       </c>
       <c r="D6" s="7">
         <v>39297</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>74</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="31" thickBot="1">
@@ -1011,16 +1037,16 @@
         <v>6</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="D7" s="7">
         <v>39309</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="31" thickBot="1">
@@ -1028,16 +1054,16 @@
         <v>7</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="D8" s="7">
         <v>39309</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="31" thickBot="1">
@@ -1045,16 +1071,16 @@
         <v>8</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="D9" s="7">
         <v>39309</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="31" thickBot="1">
@@ -1062,16 +1088,16 @@
         <v>9</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="D10" s="7">
         <v>39309</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="16" thickBot="1">
@@ -1079,16 +1105,16 @@
         <v>10</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="D11" s="7">
         <v>39309</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>63</v>
+        <v>68</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="31" thickBot="1">
@@ -1096,16 +1122,16 @@
         <v>11</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>93</v>
+        <v>26</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>11</v>
+        <v>85</v>
       </c>
       <c r="D12" s="7">
         <v>39316</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="16" thickBot="1">
@@ -1113,16 +1139,16 @@
         <v>12</v>
       </c>
       <c r="B13" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="C13" s="6" t="s">
         <v>12</v>
-      </c>
-      <c r="C13" s="6" t="s">
-        <v>79</v>
       </c>
       <c r="D13" s="7">
         <v>39323</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="16" thickBot="1">
@@ -1130,16 +1156,16 @@
         <v>13</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>13</v>
+        <v>87</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="D14" s="7">
         <v>39330</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>80</v>
+        <v>13</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="31" thickBot="1">
@@ -1147,16 +1173,16 @@
         <v>14</v>
       </c>
       <c r="B15" s="10" t="s">
-        <v>75</v>
+        <v>8</v>
       </c>
       <c r="C15" s="10" t="s">
-        <v>14</v>
+        <v>88</v>
       </c>
       <c r="D15" s="11">
         <v>39330</v>
       </c>
       <c r="E15" s="10" t="s">
-        <v>6</v>
+        <v>80</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="16" thickBot="1">
@@ -1164,16 +1190,16 @@
         <v>15</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="D16" s="7">
         <v>39344</v>
       </c>
       <c r="E16" s="6" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="31" thickBot="1">
@@ -1181,16 +1207,16 @@
         <v>16</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>22</v>
+        <v>96</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="D17" s="7">
         <v>39344</v>
       </c>
       <c r="E17" s="6" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="16" thickBot="1">
@@ -1198,16 +1224,16 @@
         <v>17</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>27</v>
+        <v>101</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="D18" s="7">
         <v>39372</v>
       </c>
       <c r="E18" s="6" t="s">
-        <v>15</v>
+        <v>89</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="16" thickBot="1">
@@ -1215,16 +1241,16 @@
         <v>18</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="D19" s="7">
         <v>39372</v>
       </c>
       <c r="E19" s="6" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="31" thickBot="1">
@@ -1232,16 +1258,16 @@
         <v>19</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="D20" s="7">
         <v>39372</v>
       </c>
       <c r="E20" s="6" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="16" thickBot="1">
@@ -1249,16 +1275,16 @@
         <v>20</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>30</v>
+        <v>104</v>
       </c>
       <c r="D21" s="7">
         <v>39400</v>
       </c>
       <c r="E21" s="6" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="31" thickBot="1">
@@ -1266,16 +1292,16 @@
         <v>21</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>31</v>
+        <v>105</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>102</v>
+        <v>35</v>
       </c>
       <c r="D22" s="7">
         <v>39400</v>
       </c>
       <c r="E22" s="6" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="16" thickBot="1">
@@ -1283,16 +1309,16 @@
         <v>22</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>83</v>
+        <v>16</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>103</v>
+        <v>36</v>
       </c>
       <c r="D23" s="7">
         <v>39400</v>
       </c>
       <c r="E23" s="6" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="31" thickBot="1">
@@ -1300,16 +1326,16 @@
         <v>23</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>87</v>
+        <v>20</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>84</v>
+        <v>17</v>
       </c>
       <c r="D24" s="7">
         <v>39400</v>
       </c>
       <c r="E24" s="6" t="s">
-        <v>85</v>
+        <v>18</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="16" thickBot="1">
@@ -1317,16 +1343,16 @@
         <v>24</v>
       </c>
       <c r="B25" s="10" t="s">
-        <v>28</v>
+        <v>102</v>
       </c>
       <c r="C25" s="10" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="D25" s="11">
         <v>39415</v>
       </c>
       <c r="E25" s="10" t="s">
-        <v>86</v>
+        <v>19</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="16" thickBot="1">
@@ -1334,16 +1360,16 @@
         <v>25</v>
       </c>
       <c r="B26" s="10" t="s">
-        <v>29</v>
+        <v>103</v>
       </c>
       <c r="C26" s="10" t="s">
-        <v>88</v>
+        <v>21</v>
       </c>
       <c r="D26" s="11">
         <v>39421</v>
       </c>
       <c r="E26" s="10" t="s">
-        <v>81</v>
+        <v>14</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="31" thickBot="1">
@@ -1351,16 +1377,16 @@
         <v>26</v>
       </c>
       <c r="B27" s="10" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="C27" s="10" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="D27" s="11">
         <v>39421</v>
       </c>
       <c r="E27" s="10" t="s">
-        <v>81</v>
+        <v>14</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="16" thickBot="1">
@@ -1368,16 +1394,16 @@
         <v>27</v>
       </c>
       <c r="B28" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="C28" s="13" t="s">
         <v>82</v>
-      </c>
-      <c r="C28" s="13" t="s">
-        <v>8</v>
       </c>
       <c r="D28" s="14">
         <v>39470</v>
       </c>
       <c r="E28" s="13" t="s">
-        <v>89</v>
+        <v>22</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="91" thickBot="1">
@@ -1385,16 +1411,16 @@
         <v>28</v>
       </c>
       <c r="B29" s="10" t="s">
-        <v>1</v>
+        <v>75</v>
       </c>
       <c r="C29" s="10" t="s">
-        <v>2</v>
+        <v>76</v>
       </c>
       <c r="D29" s="11">
         <v>39470</v>
       </c>
       <c r="E29" s="10" t="s">
-        <v>3</v>
+        <v>77</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="31" thickBot="1">
@@ -1402,16 +1428,16 @@
         <v>29</v>
       </c>
       <c r="B30" s="10" t="s">
-        <v>4</v>
+        <v>78</v>
       </c>
       <c r="C30" s="10" t="s">
-        <v>5</v>
+        <v>79</v>
       </c>
       <c r="D30" s="11">
         <v>39477</v>
       </c>
       <c r="E30" s="10" t="s">
-        <v>90</v>
+        <v>23</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="31" thickBot="1">
@@ -1419,16 +1445,16 @@
         <v>30</v>
       </c>
       <c r="B31" s="10" t="s">
-        <v>69</v>
+        <v>2</v>
       </c>
       <c r="C31" s="10" t="s">
-        <v>70</v>
+        <v>3</v>
       </c>
       <c r="D31" s="11">
         <v>39477</v>
       </c>
       <c r="E31" s="10" t="s">
-        <v>90</v>
+        <v>23</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="16" thickBot="1">
@@ -1436,16 +1462,16 @@
         <v>31</v>
       </c>
       <c r="B32" s="10" t="s">
-        <v>91</v>
+        <v>24</v>
       </c>
       <c r="C32" s="10" t="s">
-        <v>92</v>
+        <v>25</v>
       </c>
       <c r="D32" s="11">
         <v>39491</v>
       </c>
       <c r="E32" s="10" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
     </row>
     <row r="33" spans="1:5" ht="31" thickBot="1">
@@ -1453,16 +1479,16 @@
         <v>32</v>
       </c>
       <c r="B33" s="10" t="s">
-        <v>104</v>
+        <v>37</v>
       </c>
       <c r="C33" s="10" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="D33" s="11">
         <v>39498</v>
       </c>
       <c r="E33" s="10" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
     </row>
     <row r="34" spans="1:5" ht="16" thickBot="1">
@@ -1470,16 +1496,16 @@
         <v>33</v>
       </c>
       <c r="B34" s="10" t="s">
-        <v>33</v>
+        <v>107</v>
       </c>
       <c r="C34" s="10" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="D34" s="11">
         <v>39498</v>
       </c>
       <c r="E34" s="10" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
     </row>
     <row r="35" spans="1:5" ht="16" thickBot="1">
@@ -1487,16 +1513,16 @@
         <v>34</v>
       </c>
       <c r="B35" s="10" t="s">
-        <v>34</v>
+        <v>108</v>
       </c>
       <c r="C35" s="10" t="s">
-        <v>20</v>
+        <v>94</v>
       </c>
       <c r="D35" s="11">
         <v>39505</v>
       </c>
       <c r="E35" s="10" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
     </row>
     <row r="36" spans="1:5" ht="16" thickBot="1">
@@ -1504,16 +1530,16 @@
         <v>35</v>
       </c>
       <c r="B36" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="C36" s="10" t="s">
         <v>21</v>
-      </c>
-      <c r="C36" s="10" t="s">
-        <v>88</v>
       </c>
       <c r="D36" s="11">
         <v>39505</v>
       </c>
       <c r="E36" s="10" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
     </row>
     <row r="37" spans="1:5" ht="31" thickBot="1">
@@ -1521,16 +1547,16 @@
         <v>36</v>
       </c>
       <c r="B37" s="10" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="C37" s="10" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="D37" s="11">
         <v>39512</v>
       </c>
       <c r="E37" s="10" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
     </row>
     <row r="38" spans="1:5" ht="16" thickBot="1">
@@ -1538,16 +1564,16 @@
         <v>37</v>
       </c>
       <c r="B38" s="10" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="C38" s="10" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="D38" s="11">
         <v>39512</v>
       </c>
       <c r="E38" s="10" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
     </row>
     <row r="39" spans="1:5" ht="16" thickBot="1">
@@ -1555,16 +1581,16 @@
         <v>38</v>
       </c>
       <c r="B39" s="10" t="s">
-        <v>10</v>
+        <v>84</v>
       </c>
       <c r="C39" s="10" t="s">
-        <v>9</v>
+        <v>83</v>
       </c>
       <c r="D39" s="11">
         <v>39533</v>
       </c>
       <c r="E39" s="10" t="s">
-        <v>19</v>
+        <v>93</v>
       </c>
     </row>
     <row r="40" spans="1:5" ht="16" thickBot="1">
@@ -1572,16 +1598,16 @@
         <v>39</v>
       </c>
       <c r="B40" s="10" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="C40" s="10" t="s">
-        <v>35</v>
+        <v>109</v>
       </c>
       <c r="D40" s="11">
         <v>39547</v>
       </c>
       <c r="E40" s="10" t="s">
-        <v>0</v>
+        <v>74</v>
       </c>
     </row>
     <row r="41" spans="1:5" ht="16" thickBot="1">
@@ -1589,16 +1615,16 @@
         <v>40</v>
       </c>
       <c r="B41" s="10" t="s">
-        <v>71</v>
+        <v>4</v>
       </c>
       <c r="C41" s="10" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="D41" s="11">
         <v>39554</v>
       </c>
       <c r="E41" s="10" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
     </row>
     <row r="42" spans="1:5" ht="31" thickBot="1">
@@ -1606,16 +1632,16 @@
         <v>41</v>
       </c>
       <c r="B42" s="10" t="s">
-        <v>72</v>
+        <v>5</v>
       </c>
       <c r="C42" s="10" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="D42" s="11">
         <v>39554</v>
       </c>
       <c r="E42" s="10" t="s">
-        <v>73</v>
+        <v>6</v>
       </c>
     </row>
     <row r="43" spans="1:5" ht="16" thickBot="1">
@@ -1623,16 +1649,16 @@
         <v>42</v>
       </c>
       <c r="B43" s="10" t="s">
-        <v>16</v>
+        <v>90</v>
       </c>
       <c r="C43" s="10" t="s">
-        <v>9</v>
+        <v>83</v>
       </c>
       <c r="D43" s="11">
         <v>39575</v>
       </c>
       <c r="E43" s="10" t="s">
-        <v>97</v>
+        <v>30</v>
       </c>
     </row>
     <row r="44" spans="1:5" ht="16" thickBot="1">
@@ -1640,16 +1666,16 @@
         <v>43</v>
       </c>
       <c r="B44" s="10" t="s">
-        <v>17</v>
+        <v>91</v>
       </c>
       <c r="C44" s="10" t="s">
-        <v>18</v>
+        <v>92</v>
       </c>
       <c r="D44" s="11">
         <v>39575</v>
       </c>
       <c r="E44" s="10" t="s">
-        <v>97</v>
+        <v>30</v>
       </c>
     </row>
     <row r="45" spans="1:5" ht="16" thickBot="1">
@@ -1657,16 +1683,16 @@
         <v>44</v>
       </c>
       <c r="B45" s="10" t="s">
-        <v>94</v>
+        <v>27</v>
       </c>
       <c r="C45" s="10" t="s">
-        <v>95</v>
+        <v>28</v>
       </c>
       <c r="D45" s="11">
         <v>39582</v>
       </c>
       <c r="E45" s="10" t="s">
-        <v>96</v>
+        <v>29</v>
       </c>
     </row>
     <row r="46" spans="1:5" ht="16" thickBot="1">
@@ -1674,16 +1700,16 @@
         <v>45</v>
       </c>
       <c r="B46" s="10" t="s">
-        <v>98</v>
+        <v>31</v>
       </c>
       <c r="C46" s="10" t="s">
-        <v>99</v>
+        <v>32</v>
       </c>
       <c r="D46" s="11">
         <v>39589</v>
       </c>
       <c r="E46" s="10" t="s">
-        <v>97</v>
+        <v>30</v>
       </c>
     </row>
     <row r="47" spans="1:5" ht="16" thickBot="1">
@@ -1691,16 +1717,16 @@
         <v>46</v>
       </c>
       <c r="B47" s="10" t="s">
-        <v>100</v>
+        <v>33</v>
       </c>
       <c r="C47" s="10" t="s">
-        <v>99</v>
+        <v>32</v>
       </c>
       <c r="D47" s="11">
         <v>39596</v>
       </c>
       <c r="E47" s="10" t="s">
-        <v>97</v>
+        <v>30</v>
       </c>
     </row>
     <row r="48" spans="1:5" ht="16" thickBot="1">
@@ -1708,20 +1734,53 @@
         <v>47</v>
       </c>
       <c r="B48" s="10" t="s">
-        <v>101</v>
+        <v>34</v>
       </c>
       <c r="C48" s="10" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="D48" s="11">
         <v>39596</v>
       </c>
       <c r="E48" s="10" t="s">
-        <v>32</v>
+        <v>106</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" ht="16" thickBot="1">
+      <c r="A49" s="8">
+        <v>48</v>
+      </c>
+      <c r="B49" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="C49" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="D49" s="14">
+        <v>39612</v>
+      </c>
+      <c r="E49" s="13" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" ht="16" thickBot="1">
+      <c r="A50" s="8">
+        <v>49</v>
+      </c>
+      <c r="B50" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="C50" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="D50" s="14">
+        <v>39612</v>
+      </c>
+      <c r="E50" s="13" t="s">
+        <v>40</v>
       </c>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <sortState ref="A2:H13">
     <sortCondition ref="D3:D13"/>
     <sortCondition ref="E3:E13"/>
@@ -1729,6 +1788,7 @@
   </sortState>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
Committing changes made during the svn to git migration.
</commit_message>
<xml_diff>
--- a/project_management/caArray_caIntegrator_Action_Items.xlsx
+++ b/project_management/caArray_caIntegrator_Action_Items.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="22416"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="22810"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15800" tabRatio="500"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="146">
   <si>
     <t>Make the following changes to the caArray project plan:
 * Add a task to re-run the Section 508 compliance scan for 2.5.0 to ensure we are above 90%.
@@ -433,22 +433,97 @@
     <t>Upgrade caIntegrator Training tier.</t>
   </si>
   <si>
+    <t>Request more disk space on caArray PRODUCTION</t>
+  </si>
+  <si>
+    <t>Jacob Mensah</t>
+  </si>
+  <si>
+    <t>Cuong Nguyen</t>
+  </si>
+  <si>
+    <t>Test caArray database replication by putting a backup on the STAGE tier</t>
+  </si>
+  <si>
+    <t>Yeon Choi</t>
+  </si>
+  <si>
+    <t>Checklist for OSDI Kickoff</t>
+  </si>
+  <si>
+    <t>Include CSM/UPT upgrade and Section 508 compliance on project plan</t>
+  </si>
+  <si>
+    <t>Rewrite PMP in EPLC format</t>
+  </si>
+  <si>
+    <t>Shady Grove move orientation</t>
+  </si>
+  <si>
+    <t>Full Team</t>
+  </si>
+  <si>
+    <t>Discuss caArray Data Migration to File System</t>
+  </si>
+  <si>
+    <t>JJ Pan (with Juli Klemm and Yeon Choi)</t>
+  </si>
+  <si>
+    <t>Work with QA and Systems teams on estimates/project plan.</t>
+  </si>
+  <si>
+    <t>TRANSCEND Support (caIntegrator Jboss problems and caArray usage questions)</t>
+  </si>
+  <si>
+    <t>Abe Evans-EL and Rashmi Srinivasa</t>
+  </si>
+  <si>
+    <t>Contact previous authors and find out if they need any private branches retained in GitHub</t>
+  </si>
+  <si>
+    <t>Sree Nampally and Larry Brem</t>
+  </si>
+  <si>
+    <t>Look into changing names from caArray2/caIntegrator2 to caArray/caIntegrator</t>
+  </si>
+  <si>
+    <t>Winston Cheng and Abe Evans-EL</t>
+  </si>
+  <si>
+    <t>Put in a request to Clint's team to archive caintegrator-info.nci.nih.gov</t>
+  </si>
+  <si>
+    <t>Ulrike Wagner</t>
+  </si>
+  <si>
+    <t>Look into context-sensitive help links in caIntegrator</t>
+  </si>
+  <si>
+    <t>Shine Jacob and Abe Evans-EL</t>
+  </si>
+  <si>
+    <t>Contact Tabitha re: a possible walkthrough/demo of caIntegrator</t>
+  </si>
+  <si>
     <t>In Progress</t>
   </si>
   <si>
-    <t>Request more disk space on caArray PRODUCTION</t>
-  </si>
-  <si>
-    <t>Jacob Mensah</t>
-  </si>
-  <si>
-    <t>Cuong Nguyen</t>
-  </si>
-  <si>
-    <t>Test caArray database replication by putting a backup on the STAGE tier</t>
-  </si>
-  <si>
-    <t>Yeon Choi</t>
+    <t>Support from System team for OSDI</t>
+  </si>
+  <si>
+    <t>Options to make 100% 508 compliance for caIntegrator without code changes</t>
+  </si>
+  <si>
+    <t>Follow up with Kevin Burns on Agendia (Tina's) request for a caArray account. They already have guest credentials to the STAGE tier.</t>
+  </si>
+  <si>
+    <t>Update QA projections and Deployment schedule</t>
+  </si>
+  <si>
+    <t>Brian Hughes</t>
+  </si>
+  <si>
+    <t>Juli Klemm</t>
   </si>
 </sst>
 </file>
@@ -515,7 +590,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -575,36 +650,8 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="medium">
-        <color rgb="FF1F497D"/>
-      </left>
-      <right style="medium">
-        <color rgb="FF1F497D"/>
-      </right>
-      <top style="medium">
-        <color rgb="FF1F497D"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FF1F497D"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color rgb="FF1F497D"/>
-      </right>
-      <top style="medium">
-        <color rgb="FF1F497D"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FF1F497D"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="13">
+  <cellStyleXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -618,8 +665,34 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -663,26 +736,58 @@
     <xf numFmtId="14" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="13">
+  <cellStyles count="39">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1010,10 +1115,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E58"/>
+  <dimension ref="A1:E74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B34" workbookViewId="0">
-      <selection activeCell="B55" sqref="A55:XFD55"/>
+    <sheetView tabSelected="1" topLeftCell="A48" workbookViewId="0">
+      <selection activeCell="A73" sqref="A73:XFD73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
@@ -1935,7 +2040,7 @@
         <v>112</v>
       </c>
       <c r="C54" s="10" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D54" s="11">
         <v>39652</v>
@@ -1952,7 +2057,7 @@
         <v>113</v>
       </c>
       <c r="C55" s="10" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D55" s="11">
         <v>39652</v>
@@ -1962,20 +2067,20 @@
       </c>
     </row>
     <row r="56" spans="1:5" ht="16" thickBot="1">
-      <c r="A56" s="8">
+      <c r="A56" s="9">
         <v>55</v>
       </c>
-      <c r="B56" s="12" t="s">
+      <c r="B56" s="10" t="s">
         <v>114</v>
       </c>
-      <c r="C56" s="13" t="s">
-        <v>118</v>
-      </c>
-      <c r="D56" s="14">
+      <c r="C56" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="D56" s="11">
         <v>39652</v>
       </c>
-      <c r="E56" s="13" t="s">
-        <v>115</v>
+      <c r="E56" s="10" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="57" spans="1:5" ht="16" thickBot="1">
@@ -1983,7 +2088,7 @@
         <v>56</v>
       </c>
       <c r="B57" s="10" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C57" s="10" t="s">
         <v>38</v>
@@ -1996,20 +2101,288 @@
       </c>
     </row>
     <row r="58" spans="1:5" ht="16" thickBot="1">
-      <c r="A58" s="15">
-        <v>56</v>
-      </c>
-      <c r="B58" s="16" t="s">
+      <c r="A58" s="9">
+        <v>57</v>
+      </c>
+      <c r="B58" s="10" t="s">
+        <v>118</v>
+      </c>
+      <c r="C58" s="10" t="s">
         <v>119</v>
       </c>
-      <c r="C58" s="16" t="s">
+      <c r="D58" s="11">
+        <v>39722</v>
+      </c>
+      <c r="E58" s="10" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" ht="16" thickBot="1">
+      <c r="A59" s="9">
+        <v>58</v>
+      </c>
+      <c r="B59" s="10" t="s">
         <v>120</v>
       </c>
-      <c r="D58" s="14">
-        <v>39722</v>
-      </c>
-      <c r="E58" s="16" t="s">
-        <v>115</v>
+      <c r="C59" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="D59" s="11">
+        <v>39816</v>
+      </c>
+      <c r="E59" s="10" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" ht="16" thickBot="1">
+      <c r="A60" s="9">
+        <v>59</v>
+      </c>
+      <c r="B60" s="10" t="s">
+        <v>121</v>
+      </c>
+      <c r="C60" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="D60" s="11">
+        <v>39816</v>
+      </c>
+      <c r="E60" s="10" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" ht="16" thickBot="1">
+      <c r="A61" s="9">
+        <v>60</v>
+      </c>
+      <c r="B61" s="10" t="s">
+        <v>122</v>
+      </c>
+      <c r="C61" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="D61" s="11">
+        <v>39816</v>
+      </c>
+      <c r="E61" s="10" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" ht="16" thickBot="1">
+      <c r="A62" s="9">
+        <v>61</v>
+      </c>
+      <c r="B62" s="10" t="s">
+        <v>123</v>
+      </c>
+      <c r="C62" s="10" t="s">
+        <v>124</v>
+      </c>
+      <c r="D62" s="11">
+        <v>39821</v>
+      </c>
+      <c r="E62" s="10" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" ht="16" thickBot="1">
+      <c r="A63" s="9">
+        <v>62</v>
+      </c>
+      <c r="B63" s="10" t="s">
+        <v>125</v>
+      </c>
+      <c r="C63" s="10" t="s">
+        <v>126</v>
+      </c>
+      <c r="D63" s="11">
+        <v>39820</v>
+      </c>
+      <c r="E63" s="10" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" s="18" customFormat="1" ht="16" thickBot="1">
+      <c r="A64" s="15">
+        <v>63</v>
+      </c>
+      <c r="B64" s="16" t="s">
+        <v>127</v>
+      </c>
+      <c r="C64" s="16" t="s">
+        <v>44</v>
+      </c>
+      <c r="D64" s="17">
+        <v>39820</v>
+      </c>
+      <c r="E64" s="16" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" ht="31" thickBot="1">
+      <c r="A65" s="9">
+        <v>64</v>
+      </c>
+      <c r="B65" s="10" t="s">
+        <v>128</v>
+      </c>
+      <c r="C65" s="10" t="s">
+        <v>129</v>
+      </c>
+      <c r="D65" s="11">
+        <v>39820</v>
+      </c>
+      <c r="E65" s="10" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" ht="31" thickBot="1">
+      <c r="A66" s="9">
+        <v>65</v>
+      </c>
+      <c r="B66" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="C66" s="10" t="s">
+        <v>131</v>
+      </c>
+      <c r="D66" s="11">
+        <v>39827</v>
+      </c>
+      <c r="E66" s="10" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" ht="31" thickBot="1">
+      <c r="A67" s="9">
+        <v>66</v>
+      </c>
+      <c r="B67" s="10" t="s">
+        <v>132</v>
+      </c>
+      <c r="C67" s="10" t="s">
+        <v>133</v>
+      </c>
+      <c r="D67" s="11">
+        <v>39827</v>
+      </c>
+      <c r="E67" s="10" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" s="18" customFormat="1" ht="16" thickBot="1">
+      <c r="A68" s="15">
+        <v>67</v>
+      </c>
+      <c r="B68" s="16" t="s">
+        <v>134</v>
+      </c>
+      <c r="C68" s="16" t="s">
+        <v>135</v>
+      </c>
+      <c r="D68" s="17">
+        <v>39827</v>
+      </c>
+      <c r="E68" s="16" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" ht="16" thickBot="1">
+      <c r="A69" s="9">
+        <v>68</v>
+      </c>
+      <c r="B69" s="10" t="s">
+        <v>136</v>
+      </c>
+      <c r="C69" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="D69" s="11">
+        <v>39827</v>
+      </c>
+      <c r="E69" s="10" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" ht="16" thickBot="1">
+      <c r="A70" s="9">
+        <v>69</v>
+      </c>
+      <c r="B70" s="10" t="s">
+        <v>138</v>
+      </c>
+      <c r="C70" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D70" s="11">
+        <v>39827</v>
+      </c>
+      <c r="E70" s="10" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" s="18" customFormat="1" ht="16" thickBot="1">
+      <c r="A71" s="15">
+        <v>70</v>
+      </c>
+      <c r="B71" s="16" t="s">
+        <v>140</v>
+      </c>
+      <c r="C71" s="16" t="s">
+        <v>145</v>
+      </c>
+      <c r="D71" s="17"/>
+      <c r="E71" s="16" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" s="18" customFormat="1" ht="31" thickBot="1">
+      <c r="A72" s="15">
+        <v>71</v>
+      </c>
+      <c r="B72" s="16" t="s">
+        <v>141</v>
+      </c>
+      <c r="C72" s="16" t="s">
+        <v>137</v>
+      </c>
+      <c r="D72" s="17"/>
+      <c r="E72" s="16" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" ht="31" thickBot="1">
+      <c r="A73" s="9">
+        <v>72</v>
+      </c>
+      <c r="B73" s="10" t="s">
+        <v>142</v>
+      </c>
+      <c r="C73" s="10" t="s">
+        <v>144</v>
+      </c>
+      <c r="D73" s="11">
+        <v>39841</v>
+      </c>
+      <c r="E73" s="10" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" s="18" customFormat="1" ht="16" thickBot="1">
+      <c r="A74" s="15">
+        <v>73</v>
+      </c>
+      <c r="B74" s="16" t="s">
+        <v>143</v>
+      </c>
+      <c r="C74" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="D74" s="17">
+        <v>39848</v>
+      </c>
+      <c r="E74" s="16" t="s">
+        <v>139</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated project plan and action items. Meeting minutes from status meeting.
</commit_message>
<xml_diff>
--- a/project_management/caArray_caIntegrator_Action_Items.xlsx
+++ b/project_management/caArray_caIntegrator_Action_Items.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="22810"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="23117"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15800" tabRatio="500"/>
@@ -1117,8 +1117,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B12" workbookViewId="0">
-      <selection activeCell="B74" sqref="A74:XFD74"/>
+    <sheetView tabSelected="1" topLeftCell="B53" workbookViewId="0">
+      <selection activeCell="B64" sqref="A64:XFD64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
@@ -2202,21 +2202,21 @@
         <v>39</v>
       </c>
     </row>
-    <row r="64" spans="1:5" s="18" customFormat="1" ht="16" thickBot="1">
-      <c r="A64" s="15">
+    <row r="64" spans="1:5" ht="16" thickBot="1">
+      <c r="A64" s="9">
         <v>63</v>
       </c>
-      <c r="B64" s="16" t="s">
+      <c r="B64" s="10" t="s">
         <v>127</v>
       </c>
-      <c r="C64" s="16" t="s">
+      <c r="C64" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="D64" s="17">
+      <c r="D64" s="11">
         <v>39820</v>
       </c>
-      <c r="E64" s="16" t="s">
-        <v>139</v>
+      <c r="E64" s="10" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="65" spans="1:5" ht="31" thickBot="1">
@@ -2321,34 +2321,34 @@
         <v>39</v>
       </c>
     </row>
-    <row r="71" spans="1:5" s="18" customFormat="1" ht="16" thickBot="1">
-      <c r="A71" s="15">
+    <row r="71" spans="1:5" ht="16" thickBot="1">
+      <c r="A71" s="9">
         <v>70</v>
       </c>
-      <c r="B71" s="16" t="s">
+      <c r="B71" s="10" t="s">
         <v>140</v>
       </c>
-      <c r="C71" s="16" t="s">
+      <c r="C71" s="10" t="s">
         <v>145</v>
       </c>
-      <c r="D71" s="17"/>
-      <c r="E71" s="16" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="72" spans="1:5" s="18" customFormat="1" ht="31" thickBot="1">
-      <c r="A72" s="15">
+      <c r="D71" s="11"/>
+      <c r="E71" s="10" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" ht="31" thickBot="1">
+      <c r="A72" s="9">
         <v>71</v>
       </c>
-      <c r="B72" s="16" t="s">
+      <c r="B72" s="10" t="s">
         <v>141</v>
       </c>
-      <c r="C72" s="16" t="s">
+      <c r="C72" s="10" t="s">
         <v>137</v>
       </c>
-      <c r="D72" s="17"/>
-      <c r="E72" s="16" t="s">
-        <v>139</v>
+      <c r="D72" s="11"/>
+      <c r="E72" s="10" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="73" spans="1:5" ht="31" thickBot="1">

</xml_diff>

<commit_message>
Updates after the status meeting
</commit_message>
<xml_diff>
--- a/project_management/caArray_caIntegrator_Action_Items.xlsx
+++ b/project_management/caArray_caIntegrator_Action_Items.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="158">
   <si>
     <t>Make the following changes to the caArray project plan:
 * Add a task to re-run the Section 508 compliance scan for 2.5.0 to ensure we are above 90%.
@@ -542,6 +542,24 @@
   </si>
   <si>
     <t>Request gitHub integration with AntHill Pro on caArray PRODUCTION tier.</t>
+  </si>
+  <si>
+    <t>Get back to Brian Hughes about the mouse astrocytoma study in caIntegrator</t>
+  </si>
+  <si>
+    <t>In Progress</t>
+  </si>
+  <si>
+    <t>Work with Systems to resolve the UPT-caIntegrator issues Marina reported</t>
+  </si>
+  <si>
+    <t>Abe Evans-El</t>
+  </si>
+  <si>
+    <t>Assigned</t>
+  </si>
+  <si>
+    <t>Request gitHub integration with AntHill Pro on caIntegrator PRODUCTION tier.</t>
   </si>
 </sst>
 </file>
@@ -675,7 +693,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="49">
+  <cellStyleXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -725,8 +743,14 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -782,8 +806,20 @@
     <xf numFmtId="14" fontId="5" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="49">
+  <cellStyles count="55">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -808,6 +844,9 @@
     <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -832,6 +871,9 @@
     <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1159,10 +1201,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E78"/>
+  <dimension ref="A1:E81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B58" workbookViewId="0">
-      <selection activeCell="B79" sqref="A79:XFD79"/>
+    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="A81" sqref="A81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
@@ -2447,7 +2489,7 @@
       </c>
     </row>
     <row r="76" spans="1:5" s="16" customFormat="1" ht="16" thickBot="1">
-      <c r="A76" s="15">
+      <c r="A76" s="19">
         <v>75</v>
       </c>
       <c r="B76" s="17" t="s">
@@ -2464,7 +2506,7 @@
       </c>
     </row>
     <row r="77" spans="1:5" s="16" customFormat="1" ht="16" thickBot="1">
-      <c r="A77" s="15">
+      <c r="A77" s="19">
         <v>76</v>
       </c>
       <c r="B77" s="17" t="s">
@@ -2481,6 +2523,9 @@
       </c>
     </row>
     <row r="78" spans="1:5" ht="16" thickBot="1">
+      <c r="A78" s="20">
+        <v>77</v>
+      </c>
       <c r="B78" s="17" t="s">
         <v>151</v>
       </c>
@@ -2492,6 +2537,57 @@
       </c>
       <c r="E78" s="17" t="s">
         <v>39</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" ht="16" thickBot="1">
+      <c r="A79" s="15">
+        <v>78</v>
+      </c>
+      <c r="B79" s="21" t="s">
+        <v>152</v>
+      </c>
+      <c r="C79" s="21" t="s">
+        <v>81</v>
+      </c>
+      <c r="D79" s="22">
+        <v>39925</v>
+      </c>
+      <c r="E79" s="21" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" ht="16" thickBot="1">
+      <c r="A80" s="15">
+        <v>79</v>
+      </c>
+      <c r="B80" s="21" t="s">
+        <v>154</v>
+      </c>
+      <c r="C80" s="21" t="s">
+        <v>155</v>
+      </c>
+      <c r="D80" s="22">
+        <v>39925</v>
+      </c>
+      <c r="E80" s="21" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" ht="31" thickBot="1">
+      <c r="A81" s="15">
+        <v>80</v>
+      </c>
+      <c r="B81" s="21" t="s">
+        <v>157</v>
+      </c>
+      <c r="C81" s="21" t="s">
+        <v>155</v>
+      </c>
+      <c r="D81" s="22">
+        <v>39925</v>
+      </c>
+      <c r="E81" s="21" t="s">
+        <v>156</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Preparation for the 5/14/13 status meeting.
</commit_message>
<xml_diff>
--- a/project_management/caArray_caIntegrator_Action_Items.xlsx
+++ b/project_management/caArray_caIntegrator_Action_Items.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="20910"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="23206"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15800" tabRatio="500"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="160">
   <si>
     <t>Make the following changes to the caArray project plan:
 * Add a task to re-run the Section 508 compliance scan for 2.5.0 to ensure we are above 90%.
@@ -560,6 +560,12 @@
   </si>
   <si>
     <t>Request gitHub integration with AntHill Pro on caIntegrator PRODUCTION tier.</t>
+  </si>
+  <si>
+    <t>Confirm that all caArray tiers now have gitHub integration with AntHill Pro configured.</t>
+  </si>
+  <si>
+    <t>Hold meeting with Juli Klemm, Ulli Wagner, and JJ Pan to plan the caArray 2.5.3 release.</t>
   </si>
 </sst>
 </file>
@@ -693,8 +699,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="55">
+  <cellStyleXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -819,7 +827,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="55">
+  <cellStyles count="57">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -847,6 +855,7 @@
     <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -874,6 +883,7 @@
     <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1201,10 +1211,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E81"/>
+  <dimension ref="A1:E84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="A81" sqref="A81"/>
+    <sheetView tabSelected="1" topLeftCell="A65" workbookViewId="0">
+      <selection activeCell="C83" sqref="C83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
@@ -2540,37 +2550,37 @@
       </c>
     </row>
     <row r="79" spans="1:5" ht="16" thickBot="1">
-      <c r="A79" s="15">
+      <c r="A79" s="20">
         <v>78</v>
       </c>
-      <c r="B79" s="21" t="s">
+      <c r="B79" s="17" t="s">
         <v>152</v>
       </c>
-      <c r="C79" s="21" t="s">
+      <c r="C79" s="17" t="s">
         <v>81</v>
       </c>
-      <c r="D79" s="22">
+      <c r="D79" s="18">
         <v>39925</v>
       </c>
-      <c r="E79" s="21" t="s">
-        <v>153</v>
+      <c r="E79" s="17" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="80" spans="1:5" ht="16" thickBot="1">
-      <c r="A80" s="15">
+      <c r="A80" s="20">
         <v>79</v>
       </c>
-      <c r="B80" s="21" t="s">
+      <c r="B80" s="17" t="s">
         <v>154</v>
       </c>
-      <c r="C80" s="21" t="s">
+      <c r="C80" s="17" t="s">
         <v>155</v>
       </c>
-      <c r="D80" s="22">
+      <c r="D80" s="18">
         <v>39925</v>
       </c>
-      <c r="E80" s="21" t="s">
-        <v>156</v>
+      <c r="E80" s="17" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="81" spans="1:5" ht="31" thickBot="1">
@@ -2587,8 +2597,49 @@
         <v>39925</v>
       </c>
       <c r="E81" s="21" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" ht="31" thickBot="1">
+      <c r="A82" s="15">
+        <v>81</v>
+      </c>
+      <c r="B82" s="21" t="s">
+        <v>158</v>
+      </c>
+      <c r="C82" s="21" t="s">
+        <v>150</v>
+      </c>
+      <c r="D82" s="22">
+        <v>39939</v>
+      </c>
+      <c r="E82" s="21" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" ht="31" thickBot="1">
+      <c r="A83" s="15">
+        <v>82</v>
+      </c>
+      <c r="B83" s="21" t="s">
+        <v>159</v>
+      </c>
+      <c r="C83" s="21" t="s">
+        <v>150</v>
+      </c>
+      <c r="D83" s="22">
+        <v>39946</v>
+      </c>
+      <c r="E83" s="21" t="s">
         <v>156</v>
       </c>
+    </row>
+    <row r="84" spans="1:5" ht="16" thickBot="1">
+      <c r="A84" s="15"/>
+      <c r="B84" s="21"/>
+      <c r="C84" s="21"/>
+      <c r="D84" s="22"/>
+      <c r="E84" s="21"/>
     </row>
   </sheetData>
   <sortState ref="A2:H13">

</xml_diff>

<commit_message>
Updates for 5/14/13 status meeting
</commit_message>
<xml_diff>
--- a/project_management/caArray_caIntegrator_Action_Items.xlsx
+++ b/project_management/caArray_caIntegrator_Action_Items.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="161">
   <si>
     <t>Make the following changes to the caArray project plan:
 * Add a task to re-run the Section 508 compliance scan for 2.5.0 to ensure we are above 90%.
@@ -566,6 +566,9 @@
   </si>
   <si>
     <t>Hold meeting with Juli Klemm, Ulli Wagner, and JJ Pan to plan the caArray 2.5.3 release.</t>
+  </si>
+  <si>
+    <t>Run Section 508 scan on caIntegrator QA tier.</t>
   </si>
 </sst>
 </file>
@@ -1211,10 +1214,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E84"/>
+  <dimension ref="A1:E92"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A65" workbookViewId="0">
-      <selection activeCell="C83" sqref="C83"/>
+    <sheetView tabSelected="1" topLeftCell="B71" workbookViewId="0">
+      <selection activeCell="E85" sqref="E85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
@@ -2635,11 +2638,77 @@
       </c>
     </row>
     <row r="84" spans="1:5" ht="16" thickBot="1">
-      <c r="A84" s="15"/>
-      <c r="B84" s="21"/>
-      <c r="C84" s="21"/>
-      <c r="D84" s="22"/>
-      <c r="E84" s="21"/>
+      <c r="A84" s="15">
+        <v>83</v>
+      </c>
+      <c r="B84" s="21" t="s">
+        <v>160</v>
+      </c>
+      <c r="C84" s="21" t="s">
+        <v>150</v>
+      </c>
+      <c r="D84" s="22">
+        <v>39946</v>
+      </c>
+      <c r="E84" s="21" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" ht="16" thickBot="1">
+      <c r="A85" s="15"/>
+      <c r="B85" s="21"/>
+      <c r="C85" s="21"/>
+      <c r="D85" s="22"/>
+      <c r="E85" s="21"/>
+    </row>
+    <row r="86" spans="1:5" ht="16" thickBot="1">
+      <c r="A86" s="15"/>
+      <c r="B86" s="21"/>
+      <c r="C86" s="21"/>
+      <c r="D86" s="22"/>
+      <c r="E86" s="21"/>
+    </row>
+    <row r="87" spans="1:5" ht="16" thickBot="1">
+      <c r="A87" s="15"/>
+      <c r="B87" s="21"/>
+      <c r="C87" s="21"/>
+      <c r="D87" s="22"/>
+      <c r="E87" s="21"/>
+    </row>
+    <row r="88" spans="1:5" ht="16" thickBot="1">
+      <c r="A88" s="15"/>
+      <c r="B88" s="21"/>
+      <c r="C88" s="21"/>
+      <c r="D88" s="22"/>
+      <c r="E88" s="21"/>
+    </row>
+    <row r="89" spans="1:5" ht="16" thickBot="1">
+      <c r="A89" s="15"/>
+      <c r="B89" s="21"/>
+      <c r="C89" s="21"/>
+      <c r="D89" s="22"/>
+      <c r="E89" s="21"/>
+    </row>
+    <row r="90" spans="1:5" ht="16" thickBot="1">
+      <c r="A90" s="15"/>
+      <c r="B90" s="21"/>
+      <c r="C90" s="21"/>
+      <c r="D90" s="22"/>
+      <c r="E90" s="21"/>
+    </row>
+    <row r="91" spans="1:5" ht="16" thickBot="1">
+      <c r="A91" s="15"/>
+      <c r="B91" s="21"/>
+      <c r="C91" s="21"/>
+      <c r="D91" s="22"/>
+      <c r="E91" s="21"/>
+    </row>
+    <row r="92" spans="1:5" ht="16" thickBot="1">
+      <c r="A92" s="15"/>
+      <c r="B92" s="21"/>
+      <c r="C92" s="21"/>
+      <c r="D92" s="22"/>
+      <c r="E92" s="21"/>
     </row>
   </sheetData>
   <sortState ref="A2:H13">

</xml_diff>

<commit_message>
Updates after 5/14/13 status call
</commit_message>
<xml_diff>
--- a/project_management/caArray_caIntegrator_Action_Items.xlsx
+++ b/project_management/caArray_caIntegrator_Action_Items.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="23206"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15800" tabRatio="500"/>
+    <workbookView xWindow="280" yWindow="0" windowWidth="25600" windowHeight="15800" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Action_Items" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="164">
   <si>
     <t>Make the following changes to the caArray project plan:
 * Add a task to re-run the Section 508 compliance scan for 2.5.0 to ensure we are above 90%.
@@ -569,6 +569,15 @@
   </si>
   <si>
     <t>Run Section 508 scan on caIntegrator QA tier.</t>
+  </si>
+  <si>
+    <t>Follow up with Sarah Elkins on the status of updating AHP on caArray STAGE and TRAINING to use GitHub.</t>
+  </si>
+  <si>
+    <t>Contact Eva Shalley to find out if TRANSCEND plans to upgrade to the next release of caIntegrator.</t>
+  </si>
+  <si>
+    <t>Invite Laxmi Lolla to attend an upcoming status meeting to share her feedback and recommendations regarding usability and performance.</t>
   </si>
 </sst>
 </file>
@@ -1216,8 +1225,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E92"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B71" workbookViewId="0">
-      <selection activeCell="E85" sqref="E85"/>
+    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
+      <selection activeCell="B88" sqref="B88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
@@ -2654,57 +2663,97 @@
         <v>156</v>
       </c>
     </row>
-    <row r="85" spans="1:5" ht="16" thickBot="1">
-      <c r="A85" s="15"/>
-      <c r="B85" s="21"/>
-      <c r="C85" s="21"/>
-      <c r="D85" s="22"/>
-      <c r="E85" s="21"/>
-    </row>
-    <row r="86" spans="1:5" ht="16" thickBot="1">
-      <c r="A86" s="15"/>
-      <c r="B86" s="21"/>
-      <c r="C86" s="21"/>
-      <c r="D86" s="22"/>
-      <c r="E86" s="21"/>
-    </row>
-    <row r="87" spans="1:5" ht="16" thickBot="1">
-      <c r="A87" s="15"/>
-      <c r="B87" s="21"/>
-      <c r="C87" s="21"/>
-      <c r="D87" s="22"/>
-      <c r="E87" s="21"/>
+    <row r="85" spans="1:5" ht="31" thickBot="1">
+      <c r="A85" s="15">
+        <v>84</v>
+      </c>
+      <c r="B85" s="21" t="s">
+        <v>161</v>
+      </c>
+      <c r="C85" s="21" t="s">
+        <v>150</v>
+      </c>
+      <c r="D85" s="22">
+        <v>39946</v>
+      </c>
+      <c r="E85" s="21" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" ht="31" thickBot="1">
+      <c r="A86" s="15">
+        <v>85</v>
+      </c>
+      <c r="B86" s="21" t="s">
+        <v>162</v>
+      </c>
+      <c r="C86" s="21" t="s">
+        <v>150</v>
+      </c>
+      <c r="D86" s="22">
+        <v>39946</v>
+      </c>
+      <c r="E86" s="21" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" ht="31" thickBot="1">
+      <c r="A87" s="15">
+        <v>86</v>
+      </c>
+      <c r="B87" s="21" t="s">
+        <v>163</v>
+      </c>
+      <c r="C87" s="21" t="s">
+        <v>135</v>
+      </c>
+      <c r="D87" s="22">
+        <v>39946</v>
+      </c>
+      <c r="E87" s="21" t="s">
+        <v>156</v>
+      </c>
     </row>
     <row r="88" spans="1:5" ht="16" thickBot="1">
-      <c r="A88" s="15"/>
+      <c r="A88" s="15">
+        <v>87</v>
+      </c>
       <c r="B88" s="21"/>
       <c r="C88" s="21"/>
       <c r="D88" s="22"/>
       <c r="E88" s="21"/>
     </row>
     <row r="89" spans="1:5" ht="16" thickBot="1">
-      <c r="A89" s="15"/>
+      <c r="A89" s="15">
+        <v>88</v>
+      </c>
       <c r="B89" s="21"/>
       <c r="C89" s="21"/>
       <c r="D89" s="22"/>
       <c r="E89" s="21"/>
     </row>
     <row r="90" spans="1:5" ht="16" thickBot="1">
-      <c r="A90" s="15"/>
+      <c r="A90" s="15">
+        <v>89</v>
+      </c>
       <c r="B90" s="21"/>
       <c r="C90" s="21"/>
       <c r="D90" s="22"/>
       <c r="E90" s="21"/>
     </row>
     <row r="91" spans="1:5" ht="16" thickBot="1">
-      <c r="A91" s="15"/>
+      <c r="A91" s="15">
+        <v>90</v>
+      </c>
       <c r="B91" s="21"/>
       <c r="C91" s="21"/>
       <c r="D91" s="22"/>
       <c r="E91" s="21"/>
     </row>
     <row r="92" spans="1:5" ht="16" thickBot="1">
-      <c r="A92" s="15"/>
+      <c r="A92" s="15">
+        <v>91</v>
+      </c>
       <c r="B92" s="21"/>
       <c r="C92" s="21"/>
       <c r="D92" s="22"/>

</xml_diff>

<commit_message>
Prep for 5/21 status meeting.
</commit_message>
<xml_diff>
--- a/project_management/caArray_caIntegrator_Action_Items.xlsx
+++ b/project_management/caArray_caIntegrator_Action_Items.xlsx
@@ -577,7 +577,7 @@
     <t>Contact Eva Shalley to find out if TRANSCEND plans to upgrade to the next release of caIntegrator.</t>
   </si>
   <si>
-    <t>Invite Laxmi Lolla to attend an upcoming status meeting to share her feedback and recommendations regarding usability and performance.</t>
+    <t>Invite Laxmi Lolla or Ye Wu to attend an upcoming status meeting to share her feedback and recommendations regarding usability and performance.</t>
   </si>
 </sst>
 </file>
@@ -1225,8 +1225,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E92"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
-      <selection activeCell="B88" sqref="B88"/>
+    <sheetView tabSelected="1" topLeftCell="B79" workbookViewId="0">
+      <selection activeCell="E87" sqref="E87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
@@ -2677,7 +2677,7 @@
         <v>39946</v>
       </c>
       <c r="E85" s="21" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
     </row>
     <row r="86" spans="1:5" ht="31" thickBot="1">
@@ -2694,7 +2694,7 @@
         <v>39946</v>
       </c>
       <c r="E86" s="21" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
     </row>
     <row r="87" spans="1:5" ht="31" thickBot="1">
@@ -2711,7 +2711,7 @@
         <v>39946</v>
       </c>
       <c r="E87" s="21" t="s">
-        <v>156</v>
+        <v>39</v>
       </c>
     </row>
     <row r="88" spans="1:5" ht="16" thickBot="1">

</xml_diff>

<commit_message>
Updates after the 5/21 status call
</commit_message>
<xml_diff>
--- a/project_management/caArray_caIntegrator_Action_Items.xlsx
+++ b/project_management/caArray_caIntegrator_Action_Items.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="166">
   <si>
     <t>Make the following changes to the caArray project plan:
 * Add a task to re-run the Section 508 compliance scan for 2.5.0 to ensure we are above 90%.
@@ -578,6 +578,12 @@
   </si>
   <si>
     <t>Invite Laxmi Lolla or Ye Wu to attend an upcoming status meeting to share her feedback and recommendations regarding usability and performance.</t>
+  </si>
+  <si>
+    <t>Clean up the backlog of issues in Jira for caIntegrator.</t>
+  </si>
+  <si>
+    <t>Mervi Heiskanen, Shine Jacob, Mike Hunter</t>
   </si>
 </sst>
 </file>
@@ -1225,8 +1231,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E92"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B79" workbookViewId="0">
-      <selection activeCell="E87" sqref="E87"/>
+    <sheetView tabSelected="1" topLeftCell="C79" workbookViewId="0">
+      <selection activeCell="F88" sqref="F88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
@@ -2718,10 +2724,18 @@
       <c r="A88" s="15">
         <v>87</v>
       </c>
-      <c r="B88" s="21"/>
-      <c r="C88" s="21"/>
-      <c r="D88" s="22"/>
-      <c r="E88" s="21"/>
+      <c r="B88" s="21" t="s">
+        <v>164</v>
+      </c>
+      <c r="C88" s="21" t="s">
+        <v>165</v>
+      </c>
+      <c r="D88" s="22">
+        <v>39953</v>
+      </c>
+      <c r="E88" s="21" t="s">
+        <v>153</v>
+      </c>
     </row>
     <row r="89" spans="1:5" ht="16" thickBot="1">
       <c r="A89" s="15">

</xml_diff>

<commit_message>
Updates from 5/28/13 status meeting.
</commit_message>
<xml_diff>
--- a/project_management/caArray_caIntegrator_Action_Items.xlsx
+++ b/project_management/caArray_caIntegrator_Action_Items.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="23206"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="280" yWindow="0" windowWidth="25600" windowHeight="15800" tabRatio="500"/>
+    <workbookView xWindow="160" yWindow="0" windowWidth="25600" windowHeight="15800" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Action_Items" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="171">
   <si>
     <t>Make the following changes to the caArray project plan:
 * Add a task to re-run the Section 508 compliance scan for 2.5.0 to ensure we are above 90%.
@@ -583,7 +583,22 @@
     <t>Clean up the backlog of issues in Jira for caIntegrator.</t>
   </si>
   <si>
-    <t>Mervi Heiskanen, Shine Jacob, Mike Hunter</t>
+    <t>Schedule meeting with Tabitha to discuss performance and usability.</t>
+  </si>
+  <si>
+    <t>Provide links to the two MAT KC videos related to data submission.</t>
+  </si>
+  <si>
+    <t>Jill Hadfield</t>
+  </si>
+  <si>
+    <t>Review the MAT KC videos related to data submission (links provided by Jill).</t>
+  </si>
+  <si>
+    <t>Mervi Heiskanen, Shine Jacob</t>
+  </si>
+  <si>
+    <t>Complete - combined with 88</t>
   </si>
 </sst>
 </file>
@@ -1229,10 +1244,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E92"/>
+  <dimension ref="A1:E102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C79" workbookViewId="0">
-      <selection activeCell="F88" sqref="F88"/>
+    <sheetView tabSelected="1" topLeftCell="A75" workbookViewId="0">
+      <selection activeCell="B100" sqref="B100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
@@ -2666,103 +2681,127 @@
         <v>39946</v>
       </c>
       <c r="E84" s="21" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
     </row>
     <row r="85" spans="1:5" ht="31" thickBot="1">
-      <c r="A85" s="15">
+      <c r="A85" s="9">
         <v>84</v>
       </c>
-      <c r="B85" s="21" t="s">
+      <c r="B85" s="10" t="s">
         <v>161</v>
       </c>
-      <c r="C85" s="21" t="s">
+      <c r="C85" s="10" t="s">
         <v>150</v>
       </c>
-      <c r="D85" s="22">
+      <c r="D85" s="11">
         <v>39946</v>
       </c>
-      <c r="E85" s="21" t="s">
-        <v>153</v>
+      <c r="E85" s="10" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="86" spans="1:5" ht="31" thickBot="1">
-      <c r="A86" s="15">
+      <c r="A86" s="9">
         <v>85</v>
       </c>
-      <c r="B86" s="21" t="s">
+      <c r="B86" s="10" t="s">
         <v>162</v>
       </c>
-      <c r="C86" s="21" t="s">
+      <c r="C86" s="10" t="s">
         <v>150</v>
       </c>
-      <c r="D86" s="22">
+      <c r="D86" s="11">
         <v>39946</v>
       </c>
-      <c r="E86" s="21" t="s">
-        <v>153</v>
+      <c r="E86" s="10" t="s">
+        <v>170</v>
       </c>
     </row>
     <row r="87" spans="1:5" ht="31" thickBot="1">
-      <c r="A87" s="15">
+      <c r="A87" s="9">
         <v>86</v>
       </c>
-      <c r="B87" s="21" t="s">
+      <c r="B87" s="10" t="s">
         <v>163</v>
       </c>
-      <c r="C87" s="21" t="s">
+      <c r="C87" s="10" t="s">
         <v>135</v>
       </c>
-      <c r="D87" s="22">
+      <c r="D87" s="11">
         <v>39946</v>
       </c>
-      <c r="E87" s="21" t="s">
+      <c r="E87" s="10" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="88" spans="1:5" ht="16" thickBot="1">
-      <c r="A88" s="15">
+      <c r="A88" s="9">
         <v>87</v>
       </c>
-      <c r="B88" s="21" t="s">
+      <c r="B88" s="10" t="s">
         <v>164</v>
       </c>
-      <c r="C88" s="21" t="s">
-        <v>165</v>
-      </c>
-      <c r="D88" s="22">
+      <c r="C88" s="10" t="s">
+        <v>169</v>
+      </c>
+      <c r="D88" s="11">
         <v>39953</v>
       </c>
-      <c r="E88" s="21" t="s">
-        <v>153</v>
+      <c r="E88" s="10" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="89" spans="1:5" ht="16" thickBot="1">
       <c r="A89" s="15">
         <v>88</v>
       </c>
-      <c r="B89" s="21"/>
-      <c r="C89" s="21"/>
-      <c r="D89" s="22"/>
-      <c r="E89" s="21"/>
+      <c r="B89" s="21" t="s">
+        <v>165</v>
+      </c>
+      <c r="C89" s="21" t="s">
+        <v>150</v>
+      </c>
+      <c r="D89" s="22">
+        <v>39960</v>
+      </c>
+      <c r="E89" s="21" t="s">
+        <v>156</v>
+      </c>
     </row>
     <row r="90" spans="1:5" ht="16" thickBot="1">
       <c r="A90" s="15">
         <v>89</v>
       </c>
-      <c r="B90" s="21"/>
-      <c r="C90" s="21"/>
-      <c r="D90" s="22"/>
-      <c r="E90" s="21"/>
+      <c r="B90" s="21" t="s">
+        <v>166</v>
+      </c>
+      <c r="C90" s="21" t="s">
+        <v>167</v>
+      </c>
+      <c r="D90" s="22">
+        <v>39960</v>
+      </c>
+      <c r="E90" s="21" t="s">
+        <v>156</v>
+      </c>
     </row>
     <row r="91" spans="1:5" ht="16" thickBot="1">
       <c r="A91" s="15">
         <v>90</v>
       </c>
-      <c r="B91" s="21"/>
-      <c r="C91" s="21"/>
-      <c r="D91" s="22"/>
-      <c r="E91" s="21"/>
+      <c r="B91" s="21" t="s">
+        <v>168</v>
+      </c>
+      <c r="C91" s="21" t="s">
+        <v>150</v>
+      </c>
+      <c r="D91" s="22">
+        <v>39960</v>
+      </c>
+      <c r="E91" s="21" t="s">
+        <v>156</v>
+      </c>
     </row>
     <row r="92" spans="1:5" ht="16" thickBot="1">
       <c r="A92" s="15">
@@ -2772,6 +2811,96 @@
       <c r="C92" s="21"/>
       <c r="D92" s="22"/>
       <c r="E92" s="21"/>
+    </row>
+    <row r="93" spans="1:5" ht="16" thickBot="1">
+      <c r="A93" s="15">
+        <v>92</v>
+      </c>
+      <c r="B93" s="21"/>
+      <c r="C93" s="21"/>
+      <c r="D93" s="22"/>
+      <c r="E93" s="21"/>
+    </row>
+    <row r="94" spans="1:5" ht="16" thickBot="1">
+      <c r="A94" s="15">
+        <v>93</v>
+      </c>
+      <c r="B94" s="21"/>
+      <c r="C94" s="21"/>
+      <c r="D94" s="22"/>
+      <c r="E94" s="21"/>
+    </row>
+    <row r="95" spans="1:5" ht="16" thickBot="1">
+      <c r="A95" s="15">
+        <v>94</v>
+      </c>
+      <c r="B95" s="21"/>
+      <c r="C95" s="21"/>
+      <c r="D95" s="22"/>
+      <c r="E95" s="21"/>
+    </row>
+    <row r="96" spans="1:5" ht="16" thickBot="1">
+      <c r="A96" s="15">
+        <v>95</v>
+      </c>
+      <c r="B96" s="21"/>
+      <c r="C96" s="21"/>
+      <c r="D96" s="22"/>
+      <c r="E96" s="21"/>
+    </row>
+    <row r="97" spans="1:5" ht="16" thickBot="1">
+      <c r="A97" s="15">
+        <v>96</v>
+      </c>
+      <c r="B97" s="21"/>
+      <c r="C97" s="21"/>
+      <c r="D97" s="22"/>
+      <c r="E97" s="21"/>
+    </row>
+    <row r="98" spans="1:5" ht="16" thickBot="1">
+      <c r="A98" s="15">
+        <v>97</v>
+      </c>
+      <c r="B98" s="21"/>
+      <c r="C98" s="21"/>
+      <c r="D98" s="22"/>
+      <c r="E98" s="21"/>
+    </row>
+    <row r="99" spans="1:5" ht="16" thickBot="1">
+      <c r="A99" s="15">
+        <v>98</v>
+      </c>
+      <c r="B99" s="21"/>
+      <c r="C99" s="21"/>
+      <c r="D99" s="22"/>
+      <c r="E99" s="21"/>
+    </row>
+    <row r="100" spans="1:5" ht="16" thickBot="1">
+      <c r="A100" s="15">
+        <v>99</v>
+      </c>
+      <c r="B100" s="21"/>
+      <c r="C100" s="21"/>
+      <c r="D100" s="22"/>
+      <c r="E100" s="21"/>
+    </row>
+    <row r="101" spans="1:5" ht="16" thickBot="1">
+      <c r="A101" s="15">
+        <v>100</v>
+      </c>
+      <c r="B101" s="21"/>
+      <c r="C101" s="21"/>
+      <c r="D101" s="22"/>
+      <c r="E101" s="21"/>
+    </row>
+    <row r="102" spans="1:5" ht="16" thickBot="1">
+      <c r="A102" s="15">
+        <v>101</v>
+      </c>
+      <c r="B102" s="21"/>
+      <c r="C102" s="21"/>
+      <c r="D102" s="22"/>
+      <c r="E102" s="21"/>
     </row>
   </sheetData>
   <sortState ref="A2:H13">

</xml_diff>

<commit_message>
Prep for status meeting today
</commit_message>
<xml_diff>
--- a/project_management/caArray_caIntegrator_Action_Items.xlsx
+++ b/project_management/caArray_caIntegrator_Action_Items.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="172">
   <si>
     <t>Make the following changes to the caArray project plan:
 * Add a task to re-run the Section 508 compliance scan for 2.5.0 to ensure we are above 90%.
@@ -583,12 +583,6 @@
     <t>Clean up the backlog of issues in Jira for caIntegrator.</t>
   </si>
   <si>
-    <t>Schedule meeting with Tabitha to discuss performance and usability.</t>
-  </si>
-  <si>
-    <t>Provide links to the two MAT KC videos related to data submission.</t>
-  </si>
-  <si>
     <t>Jill Hadfield</t>
   </si>
   <si>
@@ -599,6 +593,15 @@
   </si>
   <si>
     <t>Complete - combined with 88</t>
+  </si>
+  <si>
+    <t>Schedule meeting with Eve and Tabitha to discuss performance and usability.</t>
+  </si>
+  <si>
+    <t>Provide Eve Shalley a summary of the changes in the next releases of caArray and caIntegrator</t>
+  </si>
+  <si>
+    <t>Provide links to the MAT KC videos related to data submission.</t>
   </si>
 </sst>
 </file>
@@ -1247,7 +1250,7 @@
   <dimension ref="A1:E102"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A75" workbookViewId="0">
-      <selection activeCell="B100" sqref="B100"/>
+      <selection activeCell="C90" sqref="C90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
@@ -2617,20 +2620,20 @@
       </c>
     </row>
     <row r="81" spans="1:5" ht="31" thickBot="1">
-      <c r="A81" s="15">
+      <c r="A81" s="9">
         <v>80</v>
       </c>
-      <c r="B81" s="21" t="s">
+      <c r="B81" s="10" t="s">
         <v>157</v>
       </c>
-      <c r="C81" s="21" t="s">
+      <c r="C81" s="10" t="s">
         <v>155</v>
       </c>
-      <c r="D81" s="22">
+      <c r="D81" s="11">
         <v>39925</v>
       </c>
-      <c r="E81" s="21" t="s">
-        <v>153</v>
+      <c r="E81" s="10" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="82" spans="1:5" ht="31" thickBot="1">
@@ -2715,7 +2718,7 @@
         <v>39946</v>
       </c>
       <c r="E86" s="10" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="87" spans="1:5" ht="31" thickBot="1">
@@ -2743,7 +2746,7 @@
         <v>164</v>
       </c>
       <c r="C88" s="10" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="D88" s="11">
         <v>39953</v>
@@ -2757,7 +2760,7 @@
         <v>88</v>
       </c>
       <c r="B89" s="21" t="s">
-        <v>165</v>
+        <v>169</v>
       </c>
       <c r="C89" s="21" t="s">
         <v>150</v>
@@ -2770,20 +2773,20 @@
       </c>
     </row>
     <row r="90" spans="1:5" ht="16" thickBot="1">
-      <c r="A90" s="15">
+      <c r="A90" s="9">
         <v>89</v>
       </c>
-      <c r="B90" s="21" t="s">
-        <v>166</v>
-      </c>
-      <c r="C90" s="21" t="s">
-        <v>167</v>
-      </c>
-      <c r="D90" s="22">
+      <c r="B90" s="10" t="s">
+        <v>171</v>
+      </c>
+      <c r="C90" s="10" t="s">
+        <v>165</v>
+      </c>
+      <c r="D90" s="11">
         <v>39960</v>
       </c>
-      <c r="E90" s="21" t="s">
-        <v>156</v>
+      <c r="E90" s="10" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="91" spans="1:5" ht="16" thickBot="1">
@@ -2791,7 +2794,7 @@
         <v>90</v>
       </c>
       <c r="B91" s="21" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C91" s="21" t="s">
         <v>150</v>
@@ -2800,17 +2803,25 @@
         <v>39960</v>
       </c>
       <c r="E91" s="21" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="92" spans="1:5" ht="16" thickBot="1">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" ht="31" thickBot="1">
       <c r="A92" s="15">
         <v>91</v>
       </c>
-      <c r="B92" s="21"/>
-      <c r="C92" s="21"/>
-      <c r="D92" s="22"/>
-      <c r="E92" s="21"/>
+      <c r="B92" s="21" t="s">
+        <v>170</v>
+      </c>
+      <c r="C92" s="21" t="s">
+        <v>150</v>
+      </c>
+      <c r="D92" s="22">
+        <v>39962</v>
+      </c>
+      <c r="E92" s="21" t="s">
+        <v>153</v>
+      </c>
     </row>
     <row r="93" spans="1:5" ht="16" thickBot="1">
       <c r="A93" s="15">

</xml_diff>

<commit_message>
Updates from yesteday's status meeting
</commit_message>
<xml_diff>
--- a/project_management/caArray_caIntegrator_Action_Items.xlsx
+++ b/project_management/caArray_caIntegrator_Action_Items.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="23206"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="160" yWindow="0" windowWidth="25600" windowHeight="15800" tabRatio="500"/>
+    <workbookView xWindow="3780" yWindow="0" windowWidth="25600" windowHeight="15800" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Action_Items" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="177">
   <si>
     <t>Make the following changes to the caArray project plan:
 * Add a task to re-run the Section 508 compliance scan for 2.5.0 to ensure we are above 90%.
@@ -602,6 +602,21 @@
   </si>
   <si>
     <t>Provide links to the MAT KC videos related to data submission.</t>
+  </si>
+  <si>
+    <t>Discuss the documentation update process</t>
+  </si>
+  <si>
+    <t>Mike Hunter and Jill Hadfield</t>
+  </si>
+  <si>
+    <t>Find the past FISMA documentation and confirm the tracker issues</t>
+  </si>
+  <si>
+    <t>Add a %FTE column to the project plans and populate it going forward</t>
+  </si>
+  <si>
+    <t>Mike Hunter and Shine Jacob</t>
   </si>
 </sst>
 </file>
@@ -1249,8 +1264,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A75" workbookViewId="0">
-      <selection activeCell="C90" sqref="C90"/>
+    <sheetView tabSelected="1" topLeftCell="B75" workbookViewId="0">
+      <selection activeCell="E96" sqref="E96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
@@ -2827,28 +2842,52 @@
       <c r="A93" s="15">
         <v>92</v>
       </c>
-      <c r="B93" s="21"/>
-      <c r="C93" s="21"/>
-      <c r="D93" s="22"/>
-      <c r="E93" s="21"/>
+      <c r="B93" s="21" t="s">
+        <v>172</v>
+      </c>
+      <c r="C93" s="21" t="s">
+        <v>173</v>
+      </c>
+      <c r="D93" s="22">
+        <v>39967</v>
+      </c>
+      <c r="E93" s="21" t="s">
+        <v>156</v>
+      </c>
     </row>
     <row r="94" spans="1:5" ht="16" thickBot="1">
       <c r="A94" s="15">
         <v>93</v>
       </c>
-      <c r="B94" s="21"/>
-      <c r="C94" s="21"/>
-      <c r="D94" s="22"/>
-      <c r="E94" s="21"/>
+      <c r="B94" s="21" t="s">
+        <v>174</v>
+      </c>
+      <c r="C94" s="21" t="s">
+        <v>150</v>
+      </c>
+      <c r="D94" s="22">
+        <v>39967</v>
+      </c>
+      <c r="E94" s="21" t="s">
+        <v>156</v>
+      </c>
     </row>
     <row r="95" spans="1:5" ht="16" thickBot="1">
       <c r="A95" s="15">
         <v>94</v>
       </c>
-      <c r="B95" s="21"/>
-      <c r="C95" s="21"/>
-      <c r="D95" s="22"/>
-      <c r="E95" s="21"/>
+      <c r="B95" s="21" t="s">
+        <v>175</v>
+      </c>
+      <c r="C95" s="21" t="s">
+        <v>176</v>
+      </c>
+      <c r="D95" s="22">
+        <v>39967</v>
+      </c>
+      <c r="E95" s="21" t="s">
+        <v>156</v>
+      </c>
     </row>
     <row r="96" spans="1:5" ht="16" thickBot="1">
       <c r="A96" s="15">

</xml_diff>

<commit_message>
Prep for tomorrow's status meeting
</commit_message>
<xml_diff>
--- a/project_management/caArray_caIntegrator_Action_Items.xlsx
+++ b/project_management/caArray_caIntegrator_Action_Items.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="23206"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="3780" yWindow="0" windowWidth="25600" windowHeight="15800" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Action_Items" sheetId="1" r:id="rId1"/>
@@ -345,278 +345,277 @@
     <t>Mervi Heiskanen</t>
   </si>
   <si>
+    <t>Complete</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Send the Agilent 415K ADF custom array design to Zhong.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Henry Schaefer</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Shine and Rashmi to provide latest product roadmaps to Zhong for the MAT-KC.</t>
+  </si>
+  <si>
+    <t>Talk to Sudha re: QA backup during Quy’s absence in the end of July.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Quy Phung and Rashmi Srinivasa</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Complete</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Complete</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Send TRANSCEND Use Cases document to JJ and Deb.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Rashmi Srinivasa</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Confirm with Jill regarding the documentation updates for caArray.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Review Test Plan for SSO and Non-SSO.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Rashmi Srinivasa</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Maureen Colbert</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Send triaged bug list to Juli, JJ, Deb and Larry and schedule a second Bug Triage meeting.</t>
+  </si>
+  <si>
+    <t>Send caIntegrator bug estimates to JJ and Mervi</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Shine</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Follow up with Systems team re: file storage for the caArray Production tier.</t>
+  </si>
+  <si>
+    <t>Submit tickets to get the Curation and Training tiers upgraded to AHP3 and the new tech stack.</t>
+  </si>
+  <si>
+    <t>Submit tickets to decommission the old caArray and caIntegrator tiers.</t>
+  </si>
+  <si>
+    <t>Upgrade caArray Curation tier.</t>
+  </si>
+  <si>
+    <t>Upgrade caArray Training tier.</t>
+  </si>
+  <si>
+    <t>Upgrade caIntegrator Training tier.</t>
+  </si>
+  <si>
+    <t>Request more disk space on caArray PRODUCTION</t>
+  </si>
+  <si>
+    <t>Jacob Mensah</t>
+  </si>
+  <si>
+    <t>Cuong Nguyen</t>
+  </si>
+  <si>
+    <t>Test caArray database replication by putting a backup on the STAGE tier</t>
+  </si>
+  <si>
+    <t>Yeon Choi</t>
+  </si>
+  <si>
+    <t>Checklist for OSDI Kickoff</t>
+  </si>
+  <si>
+    <t>Include CSM/UPT upgrade and Section 508 compliance on project plan</t>
+  </si>
+  <si>
+    <t>Rewrite PMP in EPLC format</t>
+  </si>
+  <si>
+    <t>Shady Grove move orientation</t>
+  </si>
+  <si>
+    <t>Full Team</t>
+  </si>
+  <si>
+    <t>Discuss caArray Data Migration to File System</t>
+  </si>
+  <si>
+    <t>JJ Pan (with Juli Klemm and Yeon Choi)</t>
+  </si>
+  <si>
+    <t>Work with QA and Systems teams on estimates/project plan.</t>
+  </si>
+  <si>
+    <t>TRANSCEND Support (caIntegrator Jboss problems and caArray usage questions)</t>
+  </si>
+  <si>
+    <t>Abe Evans-EL and Rashmi Srinivasa</t>
+  </si>
+  <si>
+    <t>Contact previous authors and find out if they need any private branches retained in GitHub</t>
+  </si>
+  <si>
+    <t>Sree Nampally and Larry Brem</t>
+  </si>
+  <si>
+    <t>Look into changing names from caArray2/caIntegrator2 to caArray/caIntegrator</t>
+  </si>
+  <si>
+    <t>Winston Cheng and Abe Evans-EL</t>
+  </si>
+  <si>
+    <t>Put in a request to Clint's team to archive caintegrator-info.nci.nih.gov</t>
+  </si>
+  <si>
+    <t>Ulrike Wagner</t>
+  </si>
+  <si>
+    <t>Look into context-sensitive help links in caIntegrator</t>
+  </si>
+  <si>
+    <t>Shine Jacob and Abe Evans-EL</t>
+  </si>
+  <si>
+    <t>Contact Tabitha re: a possible walkthrough/demo of caIntegrator</t>
+  </si>
+  <si>
+    <t>Support from System team for OSDI</t>
+  </si>
+  <si>
+    <t>Options to make 100% 508 compliance for caIntegrator without code changes</t>
+  </si>
+  <si>
+    <t>Follow up with Kevin Burns on Agendia (Tina's) request for a caArray account. They already have guest credentials to the STAGE tier.</t>
+  </si>
+  <si>
+    <t>Update QA projections and Deployment schedule</t>
+  </si>
+  <si>
+    <t>Brian Hughes</t>
+  </si>
+  <si>
+    <t>Juli Klemm</t>
+  </si>
+  <si>
+    <t>Marina and JJ</t>
+  </si>
+  <si>
+    <t>Follow up with Sudha and Sichen to get approval to deploy the latest caArray tag to STAGE in order to test the AntHill Pro setup for OSDI.</t>
+  </si>
+  <si>
+    <t>Request caIntegrator QA tier appscan.</t>
+  </si>
+  <si>
+    <t>Request caArray QA tier appscan.</t>
+  </si>
+  <si>
+    <t>Mike Hunter and Rashmi Srinivasa</t>
+  </si>
+  <si>
+    <t>Mike Hunter</t>
+  </si>
+  <si>
+    <t>Request gitHub integration with AntHill Pro on caArray PRODUCTION tier.</t>
+  </si>
+  <si>
+    <t>Get back to Brian Hughes about the mouse astrocytoma study in caIntegrator</t>
+  </si>
+  <si>
+    <t>In Progress</t>
+  </si>
+  <si>
+    <t>Work with Systems to resolve the UPT-caIntegrator issues Marina reported</t>
+  </si>
+  <si>
+    <t>Abe Evans-El</t>
+  </si>
+  <si>
+    <t>Assigned</t>
+  </si>
+  <si>
+    <t>Request gitHub integration with AntHill Pro on caIntegrator PRODUCTION tier.</t>
+  </si>
+  <si>
+    <t>Confirm that all caArray tiers now have gitHub integration with AntHill Pro configured.</t>
+  </si>
+  <si>
+    <t>Run Section 508 scan on caIntegrator QA tier.</t>
+  </si>
+  <si>
+    <t>Follow up with Sarah Elkins on the status of updating AHP on caArray STAGE and TRAINING to use GitHub.</t>
+  </si>
+  <si>
+    <t>Contact Eva Shalley to find out if TRANSCEND plans to upgrade to the next release of caIntegrator.</t>
+  </si>
+  <si>
+    <t>Invite Laxmi Lolla or Ye Wu to attend an upcoming status meeting to share her feedback and recommendations regarding usability and performance.</t>
+  </si>
+  <si>
+    <t>Clean up the backlog of issues in Jira for caIntegrator.</t>
+  </si>
+  <si>
+    <t>Jill Hadfield</t>
+  </si>
+  <si>
+    <t>Review the MAT KC videos related to data submission (links provided by Jill).</t>
+  </si>
+  <si>
+    <t>Mervi Heiskanen, Shine Jacob</t>
+  </si>
+  <si>
+    <t>Complete - combined with 88</t>
+  </si>
+  <si>
+    <t>Schedule meeting with Eve and Tabitha to discuss performance and usability.</t>
+  </si>
+  <si>
+    <t>Provide Eve Shalley a summary of the changes in the next releases of caArray and caIntegrator</t>
+  </si>
+  <si>
+    <t>Provide links to the MAT KC videos related to data submission.</t>
+  </si>
+  <si>
+    <t>Discuss the documentation update process</t>
+  </si>
+  <si>
+    <t>Mike Hunter and Jill Hadfield</t>
+  </si>
+  <si>
+    <t>Find the past FISMA documentation and confirm the tracker issues</t>
+  </si>
+  <si>
+    <t>Add a %FTE column to the project plans and populate it going forward</t>
+  </si>
+  <si>
+    <t>Mike Hunter and Shine Jacob</t>
+  </si>
+  <si>
     <t>On Hold (I-SPY2 data not yet available)</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Complete</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Send the Agilent 415K ADF custom array design to Zhong.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Henry Schaefer</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Shine and Rashmi to provide latest product roadmaps to Zhong for the MAT-KC.</t>
-  </si>
-  <si>
-    <t>Talk to Sudha re: QA backup during Quy’s absence in the end of July.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Quy Phung and Rashmi Srinivasa</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Complete</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Complete</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Send TRANSCEND Use Cases document to JJ and Deb.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Rashmi Srinivasa</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Confirm with Jill regarding the documentation updates for caArray.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Review Test Plan for SSO and Non-SSO.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Rashmi Srinivasa</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Maureen Colbert</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Send triaged bug list to Juli, JJ, Deb and Larry and schedule a second Bug Triage meeting.</t>
-  </si>
-  <si>
-    <t>Send caIntegrator bug estimates to JJ and Mervi</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Shine</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Follow up with Systems team re: file storage for the caArray Production tier.</t>
-  </si>
-  <si>
-    <t>Submit tickets to get the Curation and Training tiers upgraded to AHP3 and the new tech stack.</t>
-  </si>
-  <si>
-    <t>Submit tickets to decommission the old caArray and caIntegrator tiers.</t>
-  </si>
-  <si>
-    <t>Upgrade caArray Curation tier.</t>
-  </si>
-  <si>
-    <t>Upgrade caArray Training tier.</t>
-  </si>
-  <si>
-    <t>Upgrade caIntegrator Training tier.</t>
-  </si>
-  <si>
-    <t>Request more disk space on caArray PRODUCTION</t>
-  </si>
-  <si>
-    <t>Jacob Mensah</t>
-  </si>
-  <si>
-    <t>Cuong Nguyen</t>
-  </si>
-  <si>
-    <t>Test caArray database replication by putting a backup on the STAGE tier</t>
-  </si>
-  <si>
-    <t>Yeon Choi</t>
-  </si>
-  <si>
-    <t>Checklist for OSDI Kickoff</t>
-  </si>
-  <si>
-    <t>Include CSM/UPT upgrade and Section 508 compliance on project plan</t>
-  </si>
-  <si>
-    <t>Rewrite PMP in EPLC format</t>
-  </si>
-  <si>
-    <t>Shady Grove move orientation</t>
-  </si>
-  <si>
-    <t>Full Team</t>
-  </si>
-  <si>
-    <t>Discuss caArray Data Migration to File System</t>
-  </si>
-  <si>
-    <t>JJ Pan (with Juli Klemm and Yeon Choi)</t>
-  </si>
-  <si>
-    <t>Work with QA and Systems teams on estimates/project plan.</t>
-  </si>
-  <si>
-    <t>TRANSCEND Support (caIntegrator Jboss problems and caArray usage questions)</t>
-  </si>
-  <si>
-    <t>Abe Evans-EL and Rashmi Srinivasa</t>
-  </si>
-  <si>
-    <t>Contact previous authors and find out if they need any private branches retained in GitHub</t>
-  </si>
-  <si>
-    <t>Sree Nampally and Larry Brem</t>
-  </si>
-  <si>
-    <t>Look into changing names from caArray2/caIntegrator2 to caArray/caIntegrator</t>
-  </si>
-  <si>
-    <t>Winston Cheng and Abe Evans-EL</t>
-  </si>
-  <si>
-    <t>Put in a request to Clint's team to archive caintegrator-info.nci.nih.gov</t>
-  </si>
-  <si>
-    <t>Ulrike Wagner</t>
-  </si>
-  <si>
-    <t>Look into context-sensitive help links in caIntegrator</t>
-  </si>
-  <si>
-    <t>Shine Jacob and Abe Evans-EL</t>
-  </si>
-  <si>
-    <t>Contact Tabitha re: a possible walkthrough/demo of caIntegrator</t>
-  </si>
-  <si>
-    <t>Support from System team for OSDI</t>
-  </si>
-  <si>
-    <t>Options to make 100% 508 compliance for caIntegrator without code changes</t>
-  </si>
-  <si>
-    <t>Follow up with Kevin Burns on Agendia (Tina's) request for a caArray account. They already have guest credentials to the STAGE tier.</t>
-  </si>
-  <si>
-    <t>Update QA projections and Deployment schedule</t>
-  </si>
-  <si>
-    <t>Brian Hughes</t>
-  </si>
-  <si>
-    <t>Juli Klemm</t>
-  </si>
-  <si>
-    <t>Marina and JJ</t>
-  </si>
-  <si>
-    <t>Follow up with Sudha and Sichen to get approval to deploy the latest caArray tag to STAGE in order to test the AntHill Pro setup for OSDI.</t>
-  </si>
-  <si>
-    <t>Request caIntegrator QA tier appscan.</t>
-  </si>
-  <si>
-    <t>Request caArray QA tier appscan.</t>
-  </si>
-  <si>
-    <t>Mike Hunter and Rashmi Srinivasa</t>
-  </si>
-  <si>
-    <t>Mike Hunter</t>
-  </si>
-  <si>
-    <t>Request gitHub integration with AntHill Pro on caArray PRODUCTION tier.</t>
-  </si>
-  <si>
-    <t>Get back to Brian Hughes about the mouse astrocytoma study in caIntegrator</t>
-  </si>
-  <si>
-    <t>In Progress</t>
-  </si>
-  <si>
-    <t>Work with Systems to resolve the UPT-caIntegrator issues Marina reported</t>
-  </si>
-  <si>
-    <t>Abe Evans-El</t>
-  </si>
-  <si>
-    <t>Assigned</t>
-  </si>
-  <si>
-    <t>Request gitHub integration with AntHill Pro on caIntegrator PRODUCTION tier.</t>
-  </si>
-  <si>
-    <t>Confirm that all caArray tiers now have gitHub integration with AntHill Pro configured.</t>
-  </si>
-  <si>
-    <t>Hold meeting with Juli Klemm, Ulli Wagner, and JJ Pan to plan the caArray 2.5.3 release.</t>
-  </si>
-  <si>
-    <t>Run Section 508 scan on caIntegrator QA tier.</t>
-  </si>
-  <si>
-    <t>Follow up with Sarah Elkins on the status of updating AHP on caArray STAGE and TRAINING to use GitHub.</t>
-  </si>
-  <si>
-    <t>Contact Eva Shalley to find out if TRANSCEND plans to upgrade to the next release of caIntegrator.</t>
-  </si>
-  <si>
-    <t>Invite Laxmi Lolla or Ye Wu to attend an upcoming status meeting to share her feedback and recommendations regarding usability and performance.</t>
-  </si>
-  <si>
-    <t>Clean up the backlog of issues in Jira for caIntegrator.</t>
-  </si>
-  <si>
-    <t>Jill Hadfield</t>
-  </si>
-  <si>
-    <t>Review the MAT KC videos related to data submission (links provided by Jill).</t>
-  </si>
-  <si>
-    <t>Mervi Heiskanen, Shine Jacob</t>
-  </si>
-  <si>
-    <t>Complete - combined with 88</t>
-  </si>
-  <si>
-    <t>Schedule meeting with Eve and Tabitha to discuss performance and usability.</t>
-  </si>
-  <si>
-    <t>Provide Eve Shalley a summary of the changes in the next releases of caArray and caIntegrator</t>
-  </si>
-  <si>
-    <t>Provide links to the MAT KC videos related to data submission.</t>
-  </si>
-  <si>
-    <t>Discuss the documentation update process</t>
-  </si>
-  <si>
-    <t>Mike Hunter and Jill Hadfield</t>
-  </si>
-  <si>
-    <t>Find the past FISMA documentation and confirm the tracker issues</t>
-  </si>
-  <si>
-    <t>Add a %FTE column to the project plans and populate it going forward</t>
-  </si>
-  <si>
-    <t>Mike Hunter and Shine Jacob</t>
+  </si>
+  <si>
+    <t>Hold a meeting with Jacob Shine, Juli Klemm, Ulli Wagner, and JJ Pan to plan the caArray 2.5.2 release and the caIntegrator 1.4.2 release.</t>
   </si>
 </sst>
 </file>
@@ -1264,8 +1263,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B75" workbookViewId="0">
-      <selection activeCell="E96" sqref="E96"/>
+    <sheetView tabSelected="1" topLeftCell="B82" workbookViewId="0">
+      <selection activeCell="E83" sqref="E83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
@@ -1470,7 +1469,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C12" s="6" t="s">
         <v>10</v>
@@ -1643,7 +1642,7 @@
         <v>30</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D22" s="7">
         <v>39400</v>
@@ -1660,7 +1659,7 @@
         <v>85</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D23" s="7">
         <v>39400</v>
@@ -1751,7 +1750,7 @@
         <v>39470</v>
       </c>
       <c r="E28" s="13" t="s">
-        <v>91</v>
+        <v>175</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="91" thickBot="1">
@@ -1785,7 +1784,7 @@
         <v>39477</v>
       </c>
       <c r="E30" s="10" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="31" thickBot="1">
@@ -1802,7 +1801,7 @@
         <v>39477</v>
       </c>
       <c r="E31" s="10" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="16" thickBot="1">
@@ -1810,10 +1809,10 @@
         <v>31</v>
       </c>
       <c r="B32" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="C32" s="10" t="s">
         <v>93</v>
-      </c>
-      <c r="C32" s="10" t="s">
-        <v>94</v>
       </c>
       <c r="D32" s="11">
         <v>39491</v>
@@ -1827,7 +1826,7 @@
         <v>32</v>
       </c>
       <c r="B33" s="10" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C33" s="10" t="s">
         <v>38</v>
@@ -2006,7 +2005,7 @@
         <v>39575</v>
       </c>
       <c r="E43" s="10" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="44" spans="1:5" ht="16" thickBot="1">
@@ -2023,7 +2022,7 @@
         <v>39575</v>
       </c>
       <c r="E44" s="10" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="45" spans="1:5" ht="16" thickBot="1">
@@ -2031,16 +2030,16 @@
         <v>44</v>
       </c>
       <c r="B45" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="C45" s="10" t="s">
         <v>96</v>
-      </c>
-      <c r="C45" s="10" t="s">
-        <v>97</v>
       </c>
       <c r="D45" s="11">
         <v>39582</v>
       </c>
       <c r="E45" s="10" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="46" spans="1:5" ht="16" thickBot="1">
@@ -2048,16 +2047,16 @@
         <v>45</v>
       </c>
       <c r="B46" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="C46" s="10" t="s">
         <v>100</v>
-      </c>
-      <c r="C46" s="10" t="s">
-        <v>101</v>
       </c>
       <c r="D46" s="11">
         <v>39589</v>
       </c>
       <c r="E46" s="10" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="47" spans="1:5" ht="16" thickBot="1">
@@ -2065,16 +2064,16 @@
         <v>46</v>
       </c>
       <c r="B47" s="10" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C47" s="10" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D47" s="11">
         <v>39596</v>
       </c>
       <c r="E47" s="10" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="48" spans="1:5" ht="16" thickBot="1">
@@ -2082,7 +2081,7 @@
         <v>47</v>
       </c>
       <c r="B48" s="10" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C48" s="10" t="s">
         <v>66</v>
@@ -2099,10 +2098,10 @@
         <v>48</v>
       </c>
       <c r="B49" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="C49" s="10" t="s">
         <v>107</v>
-      </c>
-      <c r="C49" s="10" t="s">
-        <v>108</v>
       </c>
       <c r="D49" s="11">
         <v>39612</v>
@@ -2133,7 +2132,7 @@
         <v>50</v>
       </c>
       <c r="B51" s="10" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C51" s="10" t="s">
         <v>59</v>
@@ -2150,7 +2149,7 @@
         <v>51</v>
       </c>
       <c r="B52" s="10" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C52" s="10" t="s">
         <v>38</v>
@@ -2167,7 +2166,7 @@
         <v>52</v>
       </c>
       <c r="B53" s="10" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C53" s="10" t="s">
         <v>38</v>
@@ -2184,10 +2183,10 @@
         <v>53</v>
       </c>
       <c r="B54" s="10" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C54" s="10" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D54" s="11">
         <v>39652</v>
@@ -2201,10 +2200,10 @@
         <v>54</v>
       </c>
       <c r="B55" s="10" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C55" s="10" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D55" s="11">
         <v>39652</v>
@@ -2218,10 +2217,10 @@
         <v>55</v>
       </c>
       <c r="B56" s="10" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C56" s="10" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D56" s="11">
         <v>39652</v>
@@ -2235,7 +2234,7 @@
         <v>56</v>
       </c>
       <c r="B57" s="10" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C57" s="10" t="s">
         <v>38</v>
@@ -2252,10 +2251,10 @@
         <v>57</v>
       </c>
       <c r="B58" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="C58" s="10" t="s">
         <v>118</v>
-      </c>
-      <c r="C58" s="10" t="s">
-        <v>119</v>
       </c>
       <c r="D58" s="11">
         <v>39722</v>
@@ -2269,7 +2268,7 @@
         <v>58</v>
       </c>
       <c r="B59" s="10" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C59" s="10" t="s">
         <v>44</v>
@@ -2286,7 +2285,7 @@
         <v>59</v>
       </c>
       <c r="B60" s="10" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C60" s="10" t="s">
         <v>44</v>
@@ -2303,7 +2302,7 @@
         <v>60</v>
       </c>
       <c r="B61" s="10" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C61" s="10" t="s">
         <v>44</v>
@@ -2320,10 +2319,10 @@
         <v>61</v>
       </c>
       <c r="B62" s="10" t="s">
+        <v>122</v>
+      </c>
+      <c r="C62" s="10" t="s">
         <v>123</v>
-      </c>
-      <c r="C62" s="10" t="s">
-        <v>124</v>
       </c>
       <c r="D62" s="11">
         <v>39821</v>
@@ -2337,10 +2336,10 @@
         <v>62</v>
       </c>
       <c r="B63" s="10" t="s">
+        <v>124</v>
+      </c>
+      <c r="C63" s="10" t="s">
         <v>125</v>
-      </c>
-      <c r="C63" s="10" t="s">
-        <v>126</v>
       </c>
       <c r="D63" s="11">
         <v>39820</v>
@@ -2354,7 +2353,7 @@
         <v>63</v>
       </c>
       <c r="B64" s="10" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C64" s="10" t="s">
         <v>44</v>
@@ -2371,10 +2370,10 @@
         <v>64</v>
       </c>
       <c r="B65" s="10" t="s">
+        <v>127</v>
+      </c>
+      <c r="C65" s="10" t="s">
         <v>128</v>
-      </c>
-      <c r="C65" s="10" t="s">
-        <v>129</v>
       </c>
       <c r="D65" s="11">
         <v>39820</v>
@@ -2388,10 +2387,10 @@
         <v>65</v>
       </c>
       <c r="B66" s="10" t="s">
+        <v>129</v>
+      </c>
+      <c r="C66" s="10" t="s">
         <v>130</v>
-      </c>
-      <c r="C66" s="10" t="s">
-        <v>131</v>
       </c>
       <c r="D66" s="11">
         <v>39827</v>
@@ -2405,10 +2404,10 @@
         <v>66</v>
       </c>
       <c r="B67" s="10" t="s">
+        <v>131</v>
+      </c>
+      <c r="C67" s="10" t="s">
         <v>132</v>
-      </c>
-      <c r="C67" s="10" t="s">
-        <v>133</v>
       </c>
       <c r="D67" s="11">
         <v>39827</v>
@@ -2422,10 +2421,10 @@
         <v>67</v>
       </c>
       <c r="B68" s="10" t="s">
+        <v>133</v>
+      </c>
+      <c r="C68" s="10" t="s">
         <v>134</v>
-      </c>
-      <c r="C68" s="10" t="s">
-        <v>135</v>
       </c>
       <c r="D68" s="11">
         <v>39827</v>
@@ -2439,10 +2438,10 @@
         <v>68</v>
       </c>
       <c r="B69" s="10" t="s">
+        <v>135</v>
+      </c>
+      <c r="C69" s="10" t="s">
         <v>136</v>
-      </c>
-      <c r="C69" s="10" t="s">
-        <v>137</v>
       </c>
       <c r="D69" s="11">
         <v>39827</v>
@@ -2456,7 +2455,7 @@
         <v>69</v>
       </c>
       <c r="B70" s="10" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C70" s="10" t="s">
         <v>38</v>
@@ -2473,10 +2472,10 @@
         <v>70</v>
       </c>
       <c r="B71" s="10" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C71" s="10" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D71" s="11"/>
       <c r="E71" s="10" t="s">
@@ -2488,10 +2487,10 @@
         <v>71</v>
       </c>
       <c r="B72" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C72" s="10" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D72" s="11"/>
       <c r="E72" s="10" t="s">
@@ -2503,10 +2502,10 @@
         <v>72</v>
       </c>
       <c r="B73" s="10" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C73" s="10" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D73" s="11">
         <v>39841</v>
@@ -2520,7 +2519,7 @@
         <v>73</v>
       </c>
       <c r="B74" s="10" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C74" s="10" t="s">
         <v>38</v>
@@ -2537,10 +2536,10 @@
         <v>74</v>
       </c>
       <c r="B75" s="10" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C75" s="10" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D75" s="11">
         <v>39890</v>
@@ -2554,7 +2553,7 @@
         <v>75</v>
       </c>
       <c r="B76" s="17" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C76" s="17" t="s">
         <v>81</v>
@@ -2571,10 +2570,10 @@
         <v>76</v>
       </c>
       <c r="B77" s="17" t="s">
+        <v>147</v>
+      </c>
+      <c r="C77" s="17" t="s">
         <v>148</v>
-      </c>
-      <c r="C77" s="17" t="s">
-        <v>149</v>
       </c>
       <c r="D77" s="18">
         <v>39904</v>
@@ -2588,10 +2587,10 @@
         <v>77</v>
       </c>
       <c r="B78" s="17" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C78" s="17" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D78" s="18">
         <v>39911</v>
@@ -2605,7 +2604,7 @@
         <v>78</v>
       </c>
       <c r="B79" s="17" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C79" s="17" t="s">
         <v>81</v>
@@ -2622,10 +2621,10 @@
         <v>79</v>
       </c>
       <c r="B80" s="17" t="s">
+        <v>153</v>
+      </c>
+      <c r="C80" s="17" t="s">
         <v>154</v>
-      </c>
-      <c r="C80" s="17" t="s">
-        <v>155</v>
       </c>
       <c r="D80" s="18">
         <v>39925</v>
@@ -2639,10 +2638,10 @@
         <v>80</v>
       </c>
       <c r="B81" s="10" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C81" s="10" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D81" s="11">
         <v>39925</v>
@@ -2652,20 +2651,20 @@
       </c>
     </row>
     <row r="82" spans="1:5" ht="31" thickBot="1">
-      <c r="A82" s="15">
+      <c r="A82" s="9">
         <v>81</v>
       </c>
-      <c r="B82" s="21" t="s">
-        <v>158</v>
-      </c>
-      <c r="C82" s="21" t="s">
-        <v>150</v>
-      </c>
-      <c r="D82" s="22">
+      <c r="B82" s="10" t="s">
+        <v>157</v>
+      </c>
+      <c r="C82" s="10" t="s">
+        <v>149</v>
+      </c>
+      <c r="D82" s="11">
         <v>39939</v>
       </c>
-      <c r="E82" s="21" t="s">
-        <v>153</v>
+      <c r="E82" s="10" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="83" spans="1:5" ht="31" thickBot="1">
@@ -2673,16 +2672,16 @@
         <v>82</v>
       </c>
       <c r="B83" s="21" t="s">
-        <v>159</v>
+        <v>176</v>
       </c>
       <c r="C83" s="21" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D83" s="22">
         <v>39946</v>
       </c>
       <c r="E83" s="21" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
     </row>
     <row r="84" spans="1:5" ht="16" thickBot="1">
@@ -2690,16 +2689,16 @@
         <v>83</v>
       </c>
       <c r="B84" s="21" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C84" s="21" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D84" s="22">
         <v>39946</v>
       </c>
       <c r="E84" s="21" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="85" spans="1:5" ht="31" thickBot="1">
@@ -2707,10 +2706,10 @@
         <v>84</v>
       </c>
       <c r="B85" s="10" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="C85" s="10" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D85" s="11">
         <v>39946</v>
@@ -2724,16 +2723,16 @@
         <v>85</v>
       </c>
       <c r="B86" s="10" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="C86" s="10" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D86" s="11">
         <v>39946</v>
       </c>
       <c r="E86" s="10" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="87" spans="1:5" ht="31" thickBot="1">
@@ -2741,10 +2740,10 @@
         <v>86</v>
       </c>
       <c r="B87" s="10" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C87" s="10" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D87" s="11">
         <v>39946</v>
@@ -2758,10 +2757,10 @@
         <v>87</v>
       </c>
       <c r="B88" s="10" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C88" s="10" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D88" s="11">
         <v>39953</v>
@@ -2775,16 +2774,16 @@
         <v>88</v>
       </c>
       <c r="B89" s="21" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C89" s="21" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D89" s="22">
         <v>39960</v>
       </c>
       <c r="E89" s="21" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
     </row>
     <row r="90" spans="1:5" ht="16" thickBot="1">
@@ -2792,10 +2791,10 @@
         <v>89</v>
       </c>
       <c r="B90" s="10" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="C90" s="10" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="D90" s="11">
         <v>39960</v>
@@ -2809,33 +2808,33 @@
         <v>90</v>
       </c>
       <c r="B91" s="21" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C91" s="21" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D91" s="22">
         <v>39960</v>
       </c>
       <c r="E91" s="21" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="92" spans="1:5" ht="31" thickBot="1">
-      <c r="A92" s="15">
+      <c r="A92" s="9">
         <v>91</v>
       </c>
-      <c r="B92" s="21" t="s">
-        <v>170</v>
-      </c>
-      <c r="C92" s="21" t="s">
-        <v>150</v>
-      </c>
-      <c r="D92" s="22">
+      <c r="B92" s="10" t="s">
+        <v>168</v>
+      </c>
+      <c r="C92" s="10" t="s">
+        <v>149</v>
+      </c>
+      <c r="D92" s="11">
         <v>39962</v>
       </c>
-      <c r="E92" s="21" t="s">
-        <v>153</v>
+      <c r="E92" s="10" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="93" spans="1:5" ht="16" thickBot="1">
@@ -2843,16 +2842,16 @@
         <v>92</v>
       </c>
       <c r="B93" s="21" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="C93" s="21" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D93" s="22">
         <v>39967</v>
       </c>
       <c r="E93" s="21" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="94" spans="1:5" ht="16" thickBot="1">
@@ -2860,16 +2859,16 @@
         <v>93</v>
       </c>
       <c r="B94" s="21" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="C94" s="21" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D94" s="22">
         <v>39967</v>
       </c>
       <c r="E94" s="21" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
     </row>
     <row r="95" spans="1:5" ht="16" thickBot="1">
@@ -2877,16 +2876,16 @@
         <v>94</v>
       </c>
       <c r="B95" s="21" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C95" s="21" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="D95" s="22">
         <v>39967</v>
       </c>
       <c r="E95" s="21" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
     </row>
     <row r="96" spans="1:5" ht="16" thickBot="1">

</xml_diff>

<commit_message>
Prep for status meeting tomorrow
</commit_message>
<xml_diff>
--- a/project_management/caArray_caIntegrator_Action_Items.xlsx
+++ b/project_management/caArray_caIntegrator_Action_Items.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="23206"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="10960" yWindow="20" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="240" yWindow="240" windowWidth="26100" windowHeight="17240" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Action_Items" sheetId="1" r:id="rId1"/>
@@ -606,9 +606,6 @@
     <t>Find the past FISMA documentation and confirm the tracker issues</t>
   </si>
   <si>
-    <t>Add a %FTE column to the project plans and populate it going forward</t>
-  </si>
-  <si>
     <t>Mike Hunter and Shine Jacob</t>
   </si>
   <si>
@@ -628,6 +625,9 @@
   </si>
   <si>
     <t>Schedule a meeting with Craig Hayn from the Verifying Group to confirm our plan for addressing the FISMA items meets the spirit of the POAM.</t>
+  </si>
+  <si>
+    <t>Add a %FTE ("Work") column to the project plans and populate it going forward</t>
   </si>
 </sst>
 </file>
@@ -1263,8 +1263,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B77" workbookViewId="0">
-      <selection activeCell="E100" sqref="E100"/>
+    <sheetView tabSelected="1" topLeftCell="A77" workbookViewId="0">
+      <selection activeCell="A97" sqref="A97:E99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
@@ -2672,7 +2672,7 @@
         <v>82</v>
       </c>
       <c r="B83" s="17" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C83" s="17" t="s">
         <v>149</v>
@@ -2855,37 +2855,37 @@
       </c>
     </row>
     <row r="94" spans="1:5" ht="16" thickBot="1">
-      <c r="A94" s="11">
+      <c r="A94" s="8">
         <v>93</v>
       </c>
-      <c r="B94" s="17" t="s">
+      <c r="B94" s="9" t="s">
         <v>172</v>
       </c>
-      <c r="C94" s="17" t="s">
+      <c r="C94" s="9" t="s">
         <v>149</v>
       </c>
-      <c r="D94" s="18">
+      <c r="D94" s="10">
         <v>39967</v>
       </c>
-      <c r="E94" s="17" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="95" spans="1:5" ht="16" thickBot="1">
-      <c r="A95" s="11">
+      <c r="E94" s="9" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" ht="31" thickBot="1">
+      <c r="A95" s="8">
         <v>94</v>
       </c>
-      <c r="B95" s="17" t="s">
+      <c r="B95" s="9" t="s">
+        <v>180</v>
+      </c>
+      <c r="C95" s="9" t="s">
         <v>173</v>
       </c>
-      <c r="C95" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="D95" s="18">
+      <c r="D95" s="10">
         <v>39967</v>
       </c>
-      <c r="E95" s="17" t="s">
-        <v>152</v>
+      <c r="E95" s="9" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="96" spans="1:5" ht="31" thickBot="1">
@@ -2893,67 +2893,67 @@
         <v>95</v>
       </c>
       <c r="B96" s="17" t="s">
+        <v>175</v>
+      </c>
+      <c r="C96" s="17" t="s">
         <v>176</v>
-      </c>
-      <c r="C96" s="17" t="s">
-        <v>177</v>
       </c>
       <c r="D96" s="18">
         <v>39974</v>
       </c>
       <c r="E96" s="17" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
     </row>
     <row r="97" spans="1:5" ht="31" thickBot="1">
-      <c r="A97" s="11">
+      <c r="A97" s="8">
         <v>96</v>
       </c>
-      <c r="B97" s="17" t="s">
+      <c r="B97" s="9" t="s">
+        <v>177</v>
+      </c>
+      <c r="C97" s="9" t="s">
+        <v>149</v>
+      </c>
+      <c r="D97" s="10">
+        <v>39974</v>
+      </c>
+      <c r="E97" s="9" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" ht="31" thickBot="1">
+      <c r="A98" s="8">
+        <v>97</v>
+      </c>
+      <c r="B98" s="9" t="s">
         <v>178</v>
       </c>
-      <c r="C97" s="17" t="s">
+      <c r="C98" s="9" t="s">
         <v>149</v>
       </c>
-      <c r="D97" s="18">
+      <c r="D98" s="10">
         <v>39974</v>
       </c>
-      <c r="E97" s="17" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="98" spans="1:5" ht="31" thickBot="1">
-      <c r="A98" s="11">
-        <v>97</v>
-      </c>
-      <c r="B98" s="17" t="s">
+      <c r="E98" s="9" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" ht="31" thickBot="1">
+      <c r="A99" s="8">
+        <v>98</v>
+      </c>
+      <c r="B99" s="9" t="s">
         <v>179</v>
       </c>
-      <c r="C98" s="17" t="s">
-        <v>149</v>
-      </c>
-      <c r="D98" s="18">
+      <c r="C99" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="D99" s="10">
         <v>39974</v>
       </c>
-      <c r="E98" s="17" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="99" spans="1:5" ht="31" thickBot="1">
-      <c r="A99" s="11">
-        <v>98</v>
-      </c>
-      <c r="B99" s="17" t="s">
-        <v>180</v>
-      </c>
-      <c r="C99" s="17" t="s">
-        <v>59</v>
-      </c>
-      <c r="D99" s="18">
-        <v>39974</v>
-      </c>
-      <c r="E99" s="17" t="s">
-        <v>155</v>
+      <c r="E99" s="9" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="100" spans="1:5" ht="16" thickBot="1">

</xml_diff>

<commit_message>
Updates from the 6/18 status meeting.
</commit_message>
<xml_diff>
--- a/project_management/caArray_caIntegrator_Action_Items.xlsx
+++ b/project_management/caArray_caIntegrator_Action_Items.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="23206"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="240" windowWidth="26100" windowHeight="17240" tabRatio="500"/>
+    <workbookView xWindow="1860" yWindow="0" windowWidth="26100" windowHeight="17240" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Action_Items" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="184">
   <si>
     <t>Make the following changes to the caArray project plan:
 * Add a task to re-run the Section 508 compliance scan for 2.5.0 to ensure we are above 90%.
@@ -628,6 +628,15 @@
   </si>
   <si>
     <t>Add a %FTE ("Work") column to the project plans and populate it going forward</t>
+  </si>
+  <si>
+    <t>Find out when UPT 5.0 will be officially released and required on the tech stack.</t>
+  </si>
+  <si>
+    <t>Create/update the test plan for testing the restore of caArray data from tape backup.</t>
+  </si>
+  <si>
+    <t>Mike Hunter, Marina Omelchenko, Winston Cheng</t>
   </si>
 </sst>
 </file>
@@ -1261,10 +1270,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E102"/>
+  <dimension ref="A1:E122"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A77" workbookViewId="0">
-      <selection activeCell="A97" sqref="A97:E99"/>
+    <sheetView tabSelected="1" topLeftCell="A98" workbookViewId="0">
+      <selection activeCell="E102" sqref="E102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
@@ -2956,23 +2965,39 @@
         <v>39</v>
       </c>
     </row>
-    <row r="100" spans="1:5" ht="16" thickBot="1">
+    <row r="100" spans="1:5" ht="31" thickBot="1">
       <c r="A100" s="11">
         <v>99</v>
       </c>
-      <c r="B100" s="17"/>
-      <c r="C100" s="17"/>
-      <c r="D100" s="18"/>
-      <c r="E100" s="17"/>
-    </row>
-    <row r="101" spans="1:5" ht="16" thickBot="1">
+      <c r="B100" s="17" t="s">
+        <v>181</v>
+      </c>
+      <c r="C100" s="17" t="s">
+        <v>59</v>
+      </c>
+      <c r="D100" s="18">
+        <v>39981</v>
+      </c>
+      <c r="E100" s="17" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5" ht="31" thickBot="1">
       <c r="A101" s="11">
         <v>100</v>
       </c>
-      <c r="B101" s="17"/>
-      <c r="C101" s="17"/>
-      <c r="D101" s="18"/>
-      <c r="E101" s="17"/>
+      <c r="B101" s="17" t="s">
+        <v>182</v>
+      </c>
+      <c r="C101" s="17" t="s">
+        <v>183</v>
+      </c>
+      <c r="D101" s="18">
+        <v>39981</v>
+      </c>
+      <c r="E101" s="17" t="s">
+        <v>155</v>
+      </c>
     </row>
     <row r="102" spans="1:5" ht="16" thickBot="1">
       <c r="A102" s="11">
@@ -2982,6 +3007,186 @@
       <c r="C102" s="17"/>
       <c r="D102" s="18"/>
       <c r="E102" s="17"/>
+    </row>
+    <row r="103" spans="1:5" ht="16" thickBot="1">
+      <c r="A103" s="11">
+        <v>102</v>
+      </c>
+      <c r="B103" s="17"/>
+      <c r="C103" s="17"/>
+      <c r="D103" s="18"/>
+      <c r="E103" s="17"/>
+    </row>
+    <row r="104" spans="1:5" ht="16" thickBot="1">
+      <c r="A104" s="11">
+        <v>103</v>
+      </c>
+      <c r="B104" s="17"/>
+      <c r="C104" s="17"/>
+      <c r="D104" s="18"/>
+      <c r="E104" s="17"/>
+    </row>
+    <row r="105" spans="1:5" ht="16" thickBot="1">
+      <c r="A105" s="11">
+        <v>104</v>
+      </c>
+      <c r="B105" s="17"/>
+      <c r="C105" s="17"/>
+      <c r="D105" s="18"/>
+      <c r="E105" s="17"/>
+    </row>
+    <row r="106" spans="1:5" ht="16" thickBot="1">
+      <c r="A106" s="11">
+        <v>105</v>
+      </c>
+      <c r="B106" s="17"/>
+      <c r="C106" s="17"/>
+      <c r="D106" s="18"/>
+      <c r="E106" s="17"/>
+    </row>
+    <row r="107" spans="1:5" ht="16" thickBot="1">
+      <c r="A107" s="11">
+        <v>106</v>
+      </c>
+      <c r="B107" s="17"/>
+      <c r="C107" s="17"/>
+      <c r="D107" s="18"/>
+      <c r="E107" s="17"/>
+    </row>
+    <row r="108" spans="1:5" ht="16" thickBot="1">
+      <c r="A108" s="11">
+        <v>107</v>
+      </c>
+      <c r="B108" s="17"/>
+      <c r="C108" s="17"/>
+      <c r="D108" s="18"/>
+      <c r="E108" s="17"/>
+    </row>
+    <row r="109" spans="1:5" ht="16" thickBot="1">
+      <c r="A109" s="11">
+        <v>108</v>
+      </c>
+      <c r="B109" s="17"/>
+      <c r="C109" s="17"/>
+      <c r="D109" s="18"/>
+      <c r="E109" s="17"/>
+    </row>
+    <row r="110" spans="1:5" ht="16" thickBot="1">
+      <c r="A110" s="11">
+        <v>109</v>
+      </c>
+      <c r="B110" s="17"/>
+      <c r="C110" s="17"/>
+      <c r="D110" s="18"/>
+      <c r="E110" s="17"/>
+    </row>
+    <row r="111" spans="1:5" ht="16" thickBot="1">
+      <c r="A111" s="11">
+        <v>110</v>
+      </c>
+      <c r="B111" s="17"/>
+      <c r="C111" s="17"/>
+      <c r="D111" s="18"/>
+      <c r="E111" s="17"/>
+    </row>
+    <row r="112" spans="1:5" ht="16" thickBot="1">
+      <c r="A112" s="11">
+        <v>111</v>
+      </c>
+      <c r="B112" s="17"/>
+      <c r="C112" s="17"/>
+      <c r="D112" s="18"/>
+      <c r="E112" s="17"/>
+    </row>
+    <row r="113" spans="1:5" ht="16" thickBot="1">
+      <c r="A113" s="11">
+        <v>112</v>
+      </c>
+      <c r="B113" s="17"/>
+      <c r="C113" s="17"/>
+      <c r="D113" s="18"/>
+      <c r="E113" s="17"/>
+    </row>
+    <row r="114" spans="1:5" ht="16" thickBot="1">
+      <c r="A114" s="11">
+        <v>113</v>
+      </c>
+      <c r="B114" s="17"/>
+      <c r="C114" s="17"/>
+      <c r="D114" s="18"/>
+      <c r="E114" s="17"/>
+    </row>
+    <row r="115" spans="1:5" ht="16" thickBot="1">
+      <c r="A115" s="11">
+        <v>114</v>
+      </c>
+      <c r="B115" s="17"/>
+      <c r="C115" s="17"/>
+      <c r="D115" s="18"/>
+      <c r="E115" s="17"/>
+    </row>
+    <row r="116" spans="1:5" ht="16" thickBot="1">
+      <c r="A116" s="11">
+        <v>115</v>
+      </c>
+      <c r="B116" s="17"/>
+      <c r="C116" s="17"/>
+      <c r="D116" s="18"/>
+      <c r="E116" s="17"/>
+    </row>
+    <row r="117" spans="1:5" ht="16" thickBot="1">
+      <c r="A117" s="11">
+        <v>116</v>
+      </c>
+      <c r="B117" s="17"/>
+      <c r="C117" s="17"/>
+      <c r="D117" s="18"/>
+      <c r="E117" s="17"/>
+    </row>
+    <row r="118" spans="1:5" ht="16" thickBot="1">
+      <c r="A118" s="11">
+        <v>117</v>
+      </c>
+      <c r="B118" s="17"/>
+      <c r="C118" s="17"/>
+      <c r="D118" s="18"/>
+      <c r="E118" s="17"/>
+    </row>
+    <row r="119" spans="1:5" ht="16" thickBot="1">
+      <c r="A119" s="11">
+        <v>118</v>
+      </c>
+      <c r="B119" s="17"/>
+      <c r="C119" s="17"/>
+      <c r="D119" s="18"/>
+      <c r="E119" s="17"/>
+    </row>
+    <row r="120" spans="1:5" ht="16" thickBot="1">
+      <c r="A120" s="11">
+        <v>119</v>
+      </c>
+      <c r="B120" s="17"/>
+      <c r="C120" s="17"/>
+      <c r="D120" s="18"/>
+      <c r="E120" s="17"/>
+    </row>
+    <row r="121" spans="1:5" ht="16" thickBot="1">
+      <c r="A121" s="11">
+        <v>120</v>
+      </c>
+      <c r="B121" s="17"/>
+      <c r="C121" s="17"/>
+      <c r="D121" s="18"/>
+      <c r="E121" s="17"/>
+    </row>
+    <row r="122" spans="1:5" ht="16" thickBot="1">
+      <c r="A122" s="11">
+        <v>121</v>
+      </c>
+      <c r="B122" s="17"/>
+      <c r="C122" s="17"/>
+      <c r="D122" s="18"/>
+      <c r="E122" s="17"/>
     </row>
   </sheetData>
   <sortState ref="A2:H13">

</xml_diff>

<commit_message>
Updates after status meeting.
</commit_message>
<xml_diff>
--- a/project_management/caArray_caIntegrator_Action_Items.xlsx
+++ b/project_management/caArray_caIntegrator_Action_Items.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="23206"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="23515"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1860" yWindow="0" windowWidth="26100" windowHeight="17240" tabRatio="500"/>
+    <workbookView xWindow="3860" yWindow="1900" windowWidth="26100" windowHeight="17240" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Action_Items" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="190">
   <si>
     <t>Make the following changes to the caArray project plan:
 * Add a task to re-run the Section 508 compliance scan for 2.5.0 to ensure we are above 90%.
@@ -637,6 +637,24 @@
   </si>
   <si>
     <t>Mike Hunter, Marina Omelchenko, Winston Cheng</t>
+  </si>
+  <si>
+    <t>Send target release target dates to Ulli to communicate to Engineering</t>
+  </si>
+  <si>
+    <t>Post the caIntegrator screencasts to a private wiki (need the files)</t>
+  </si>
+  <si>
+    <t>In August, invite AIM team and IVIM to discuss upgrade path for caIntegrator.</t>
+  </si>
+  <si>
+    <t>Shine Jacob, Abe Evans-EL, Ulrike Wagner</t>
+  </si>
+  <si>
+    <t>Invite NBIA team to discuss upgrade path for caIntegrator.</t>
+  </si>
+  <si>
+    <t>Abe Evans-El and Mike Hunter</t>
   </si>
 </sst>
 </file>
@@ -770,8 +788,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="57">
+  <cellStyleXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -886,7 +906,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="57">
+  <cellStyles count="59">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -915,6 +935,7 @@
     <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -943,6 +964,7 @@
     <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1272,8 +1294,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E122"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A98" workbookViewId="0">
-      <selection activeCell="E102" sqref="E102"/>
+    <sheetView tabSelected="1" topLeftCell="C86" workbookViewId="0">
+      <selection activeCell="F105" sqref="F105"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
@@ -2694,20 +2716,20 @@
       </c>
     </row>
     <row r="84" spans="1:5" ht="16" thickBot="1">
-      <c r="A84" s="11">
+      <c r="A84" s="8">
         <v>83</v>
       </c>
-      <c r="B84" s="17" t="s">
+      <c r="B84" s="9" t="s">
         <v>158</v>
       </c>
-      <c r="C84" s="17" t="s">
+      <c r="C84" s="9" t="s">
         <v>149</v>
       </c>
-      <c r="D84" s="18">
+      <c r="D84" s="10">
         <v>39946</v>
       </c>
-      <c r="E84" s="17" t="s">
-        <v>152</v>
+      <c r="E84" s="9" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="85" spans="1:5" ht="31" thickBot="1">
@@ -2813,20 +2835,20 @@
       </c>
     </row>
     <row r="91" spans="1:5" ht="16" thickBot="1">
-      <c r="A91" s="11">
+      <c r="A91" s="8">
         <v>90</v>
       </c>
-      <c r="B91" s="17" t="s">
+      <c r="B91" s="9" t="s">
         <v>164</v>
       </c>
-      <c r="C91" s="17" t="s">
+      <c r="C91" s="9" t="s">
         <v>149</v>
       </c>
-      <c r="D91" s="18">
+      <c r="D91" s="10">
         <v>39960</v>
       </c>
-      <c r="E91" s="17" t="s">
-        <v>152</v>
+      <c r="E91" s="9" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="92" spans="1:5" ht="31" thickBot="1">
@@ -2996,44 +3018,76 @@
         <v>39981</v>
       </c>
       <c r="E101" s="17" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
     </row>
     <row r="102" spans="1:5" ht="16" thickBot="1">
-      <c r="A102" s="11">
+      <c r="A102" s="8">
         <v>101</v>
       </c>
-      <c r="B102" s="17"/>
-      <c r="C102" s="17"/>
-      <c r="D102" s="18"/>
-      <c r="E102" s="17"/>
+      <c r="B102" s="9" t="s">
+        <v>184</v>
+      </c>
+      <c r="C102" s="9" t="s">
+        <v>149</v>
+      </c>
+      <c r="D102" s="10">
+        <v>39988</v>
+      </c>
+      <c r="E102" s="9" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="103" spans="1:5" ht="16" thickBot="1">
       <c r="A103" s="11">
         <v>102</v>
       </c>
-      <c r="B103" s="17"/>
-      <c r="C103" s="17"/>
-      <c r="D103" s="18"/>
-      <c r="E103" s="17"/>
+      <c r="B103" s="17" t="s">
+        <v>185</v>
+      </c>
+      <c r="C103" s="17" t="s">
+        <v>187</v>
+      </c>
+      <c r="D103" s="18">
+        <v>39988</v>
+      </c>
+      <c r="E103" s="17" t="s">
+        <v>152</v>
+      </c>
     </row>
     <row r="104" spans="1:5" ht="16" thickBot="1">
       <c r="A104" s="11">
         <v>103</v>
       </c>
-      <c r="B104" s="17"/>
-      <c r="C104" s="17"/>
-      <c r="D104" s="18"/>
-      <c r="E104" s="17"/>
+      <c r="B104" s="17" t="s">
+        <v>186</v>
+      </c>
+      <c r="C104" s="17" t="s">
+        <v>134</v>
+      </c>
+      <c r="D104" s="18">
+        <v>39988</v>
+      </c>
+      <c r="E104" s="17" t="s">
+        <v>155</v>
+      </c>
     </row>
     <row r="105" spans="1:5" ht="16" thickBot="1">
       <c r="A105" s="11">
         <v>104</v>
       </c>
-      <c r="B105" s="17"/>
-      <c r="C105" s="17"/>
-      <c r="D105" s="18"/>
-      <c r="E105" s="17"/>
+      <c r="B105" s="17" t="s">
+        <v>188</v>
+      </c>
+      <c r="C105" s="17" t="s">
+        <v>189</v>
+      </c>
+      <c r="D105" s="18">
+        <v>39988</v>
+      </c>
+      <c r="E105" s="17" t="s">
+        <v>155</v>
+      </c>
     </row>
     <row r="106" spans="1:5" ht="16" thickBot="1">
       <c r="A106" s="11">

</xml_diff>

<commit_message>
Prep for status meeting
</commit_message>
<xml_diff>
--- a/project_management/caArray_caIntegrator_Action_Items.xlsx
+++ b/project_management/caArray_caIntegrator_Action_Items.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="23515"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="3860" yWindow="1900" windowWidth="26100" windowHeight="17240" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Action_Items" sheetId="1" r:id="rId1"/>
@@ -1294,8 +1294,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E122"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C86" workbookViewId="0">
-      <selection activeCell="F105" sqref="F105"/>
+    <sheetView tabSelected="1" topLeftCell="A84" workbookViewId="0">
+      <selection activeCell="A103" sqref="A103:E103"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
@@ -2699,20 +2699,20 @@
       </c>
     </row>
     <row r="83" spans="1:5" ht="31" thickBot="1">
-      <c r="A83" s="11">
+      <c r="A83" s="8">
         <v>82</v>
       </c>
-      <c r="B83" s="17" t="s">
+      <c r="B83" s="9" t="s">
         <v>174</v>
       </c>
-      <c r="C83" s="17" t="s">
+      <c r="C83" s="9" t="s">
         <v>149</v>
       </c>
-      <c r="D83" s="18">
+      <c r="D83" s="10">
         <v>39946</v>
       </c>
-      <c r="E83" s="17" t="s">
-        <v>152</v>
+      <c r="E83" s="9" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="84" spans="1:5" ht="16" thickBot="1">
@@ -2869,20 +2869,20 @@
       </c>
     </row>
     <row r="93" spans="1:5" ht="16" thickBot="1">
-      <c r="A93" s="11">
+      <c r="A93" s="8">
         <v>92</v>
       </c>
-      <c r="B93" s="17" t="s">
+      <c r="B93" s="9" t="s">
         <v>170</v>
       </c>
-      <c r="C93" s="17" t="s">
+      <c r="C93" s="9" t="s">
         <v>171</v>
       </c>
-      <c r="D93" s="18">
+      <c r="D93" s="10">
         <v>39967</v>
       </c>
-      <c r="E93" s="17" t="s">
-        <v>155</v>
+      <c r="E93" s="9" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="94" spans="1:5" ht="16" thickBot="1">
@@ -3039,20 +3039,20 @@
       </c>
     </row>
     <row r="103" spans="1:5" ht="16" thickBot="1">
-      <c r="A103" s="11">
+      <c r="A103" s="8">
         <v>102</v>
       </c>
-      <c r="B103" s="17" t="s">
+      <c r="B103" s="9" t="s">
         <v>185</v>
       </c>
-      <c r="C103" s="17" t="s">
+      <c r="C103" s="9" t="s">
         <v>187</v>
       </c>
-      <c r="D103" s="18">
+      <c r="D103" s="10">
         <v>39988</v>
       </c>
-      <c r="E103" s="17" t="s">
-        <v>152</v>
+      <c r="E103" s="9" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="104" spans="1:5" ht="16" thickBot="1">

</xml_diff>

<commit_message>
Action items from the status meeting.
</commit_message>
<xml_diff>
--- a/project_management/caArray_caIntegrator_Action_Items.xlsx
+++ b/project_management/caArray_caIntegrator_Action_Items.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="23515"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="3840" yWindow="760" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Action_Items" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="194">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="341" uniqueCount="201">
   <si>
     <t>Make the following changes to the caArray project plan:
 * Add a task to re-run the Section 508 compliance scan for 2.5.0 to ensure we are above 90%.
@@ -667,6 +667,27 @@
   </si>
   <si>
     <t>Follow up on the versioning guidance for caIntegrator (1.5 vs 1.4.2).</t>
+  </si>
+  <si>
+    <t>Provide the verbiage for making an experiment public and get it approved by Legal.</t>
+  </si>
+  <si>
+    <t>Provide Juli the nature of the verbiage for making an experiment public.</t>
+  </si>
+  <si>
+    <t>Respond to JJ's email about audit log review procedure.</t>
+  </si>
+  <si>
+    <t>Review caArray audit log capabilities in the 7/30 status meeting.</t>
+  </si>
+  <si>
+    <t>Mike Hunter and Winston Cheng</t>
+  </si>
+  <si>
+    <t>Review caIntegrator performance improvements in the 7/23 status meeting.</t>
+  </si>
+  <si>
+    <t>Mike Hunter and Abe Evans-El</t>
   </si>
 </sst>
 </file>
@@ -1314,8 +1335,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E122"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A95" workbookViewId="0">
-      <selection activeCell="B112" sqref="B112"/>
+    <sheetView tabSelected="1" topLeftCell="B92" workbookViewId="0">
+      <selection activeCell="E108" sqref="E108"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
@@ -3140,7 +3161,7 @@
         <v>40002</v>
       </c>
       <c r="E107" s="17" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
     </row>
     <row r="108" spans="1:5" ht="16" thickBot="1">
@@ -3164,46 +3185,86 @@
       <c r="A109" s="11">
         <v>108</v>
       </c>
-      <c r="B109" s="17"/>
-      <c r="C109" s="17"/>
-      <c r="D109" s="18"/>
-      <c r="E109" s="17"/>
-    </row>
-    <row r="110" spans="1:5" ht="16" thickBot="1">
+      <c r="B109" s="17" t="s">
+        <v>195</v>
+      </c>
+      <c r="C109" s="17" t="s">
+        <v>149</v>
+      </c>
+      <c r="D109" s="18">
+        <v>40009</v>
+      </c>
+      <c r="E109" s="17" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5" ht="31" thickBot="1">
       <c r="A110" s="11">
         <v>109</v>
       </c>
-      <c r="B110" s="17"/>
-      <c r="C110" s="17"/>
-      <c r="D110" s="18"/>
-      <c r="E110" s="17"/>
+      <c r="B110" s="17" t="s">
+        <v>194</v>
+      </c>
+      <c r="C110" s="17" t="s">
+        <v>143</v>
+      </c>
+      <c r="D110" s="18">
+        <v>40009</v>
+      </c>
+      <c r="E110" s="17" t="s">
+        <v>155</v>
+      </c>
     </row>
     <row r="111" spans="1:5" ht="16" thickBot="1">
       <c r="A111" s="11">
         <v>110</v>
       </c>
-      <c r="B111" s="17"/>
-      <c r="C111" s="17"/>
-      <c r="D111" s="18"/>
-      <c r="E111" s="17"/>
+      <c r="B111" s="17" t="s">
+        <v>196</v>
+      </c>
+      <c r="C111" s="17" t="s">
+        <v>149</v>
+      </c>
+      <c r="D111" s="18">
+        <v>40009</v>
+      </c>
+      <c r="E111" s="17" t="s">
+        <v>155</v>
+      </c>
     </row>
     <row r="112" spans="1:5" ht="16" thickBot="1">
       <c r="A112" s="11">
         <v>111</v>
       </c>
-      <c r="B112" s="17"/>
-      <c r="C112" s="17"/>
-      <c r="D112" s="18"/>
-      <c r="E112" s="17"/>
+      <c r="B112" s="17" t="s">
+        <v>197</v>
+      </c>
+      <c r="C112" s="17" t="s">
+        <v>198</v>
+      </c>
+      <c r="D112" s="18">
+        <v>40009</v>
+      </c>
+      <c r="E112" s="17" t="s">
+        <v>155</v>
+      </c>
     </row>
     <row r="113" spans="1:5" ht="16" thickBot="1">
       <c r="A113" s="11">
         <v>112</v>
       </c>
-      <c r="B113" s="17"/>
-      <c r="C113" s="17"/>
-      <c r="D113" s="18"/>
-      <c r="E113" s="17"/>
+      <c r="B113" s="17" t="s">
+        <v>199</v>
+      </c>
+      <c r="C113" s="17" t="s">
+        <v>200</v>
+      </c>
+      <c r="D113" s="18">
+        <v>40009</v>
+      </c>
+      <c r="E113" s="17" t="s">
+        <v>155</v>
+      </c>
     </row>
     <row r="114" spans="1:5" ht="16" thickBot="1">
       <c r="A114" s="11">

</xml_diff>

<commit_message>
Updates from the status meeting
</commit_message>
<xml_diff>
--- a/project_management/caArray_caIntegrator_Action_Items.xlsx
+++ b/project_management/caArray_caIntegrator_Action_Items.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="341" uniqueCount="201">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="205">
   <si>
     <t>Make the following changes to the caArray project plan:
 * Add a task to re-run the Section 508 compliance scan for 2.5.0 to ensure we are above 90%.
@@ -688,6 +688,18 @@
   </si>
   <si>
     <t>Mike Hunter and Abe Evans-El</t>
+  </si>
+  <si>
+    <t>Review the project plans for caArray and caIntegrator to determine if there are things to do to streamline getting both applications back into Production before September</t>
+  </si>
+  <si>
+    <t>Decide which of the three options proposed for making it easy to review audit log entries each month to implement</t>
+  </si>
+  <si>
+    <t>JJ Pan and Juli Klemm</t>
+  </si>
+  <si>
+    <t>After Abe addresses the performance drop for Agilent Data Sets, share Abe's performance page from the wiki with Eve Shalley</t>
   </si>
 </sst>
 </file>
@@ -1335,8 +1347,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E122"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A111" sqref="A111:E111"/>
+    <sheetView tabSelected="1" topLeftCell="B96" workbookViewId="0">
+      <selection activeCell="E117" sqref="E117"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
@@ -3250,48 +3262,72 @@
       </c>
     </row>
     <row r="113" spans="1:5" ht="16" thickBot="1">
-      <c r="A113" s="11">
+      <c r="A113" s="8">
         <v>112</v>
       </c>
-      <c r="B113" s="17" t="s">
+      <c r="B113" s="9" t="s">
         <v>199</v>
       </c>
-      <c r="C113" s="17" t="s">
+      <c r="C113" s="9" t="s">
         <v>200</v>
       </c>
-      <c r="D113" s="18">
+      <c r="D113" s="10">
         <v>40009</v>
       </c>
-      <c r="E113" s="17" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="114" spans="1:5" ht="16" thickBot="1">
+      <c r="E113" s="9" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5" ht="46" thickBot="1">
       <c r="A114" s="11">
         <v>113</v>
       </c>
-      <c r="B114" s="17"/>
-      <c r="C114" s="17"/>
-      <c r="D114" s="18"/>
-      <c r="E114" s="17"/>
-    </row>
-    <row r="115" spans="1:5" ht="16" thickBot="1">
+      <c r="B114" s="17" t="s">
+        <v>201</v>
+      </c>
+      <c r="C114" s="17" t="s">
+        <v>59</v>
+      </c>
+      <c r="D114" s="18">
+        <v>40016</v>
+      </c>
+      <c r="E114" s="17" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="115" spans="1:5" ht="31" thickBot="1">
       <c r="A115" s="11">
         <v>114</v>
       </c>
-      <c r="B115" s="17"/>
-      <c r="C115" s="17"/>
-      <c r="D115" s="18"/>
-      <c r="E115" s="17"/>
-    </row>
-    <row r="116" spans="1:5" ht="16" thickBot="1">
+      <c r="B115" s="17" t="s">
+        <v>202</v>
+      </c>
+      <c r="C115" s="17" t="s">
+        <v>203</v>
+      </c>
+      <c r="D115" s="18">
+        <v>40016</v>
+      </c>
+      <c r="E115" s="17" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="116" spans="1:5" ht="31" thickBot="1">
       <c r="A116" s="11">
         <v>115</v>
       </c>
-      <c r="B116" s="17"/>
-      <c r="C116" s="17"/>
-      <c r="D116" s="18"/>
-      <c r="E116" s="17"/>
+      <c r="B116" s="17" t="s">
+        <v>204</v>
+      </c>
+      <c r="C116" s="17" t="s">
+        <v>149</v>
+      </c>
+      <c r="D116" s="18">
+        <v>40016</v>
+      </c>
+      <c r="E116" s="17" t="s">
+        <v>155</v>
+      </c>
     </row>
     <row r="117" spans="1:5" ht="16" thickBot="1">
       <c r="A117" s="11">

</xml_diff>

<commit_message>
Updates from the status meeting and sprint planning
</commit_message>
<xml_diff>
--- a/project_management/caArray_caIntegrator_Action_Items.xlsx
+++ b/project_management/caArray_caIntegrator_Action_Items.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="205">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="359" uniqueCount="209">
   <si>
     <t>Make the following changes to the caArray project plan:
 * Add a task to re-run the Section 508 compliance scan for 2.5.0 to ensure we are above 90%.
@@ -700,6 +700,18 @@
   </si>
   <si>
     <t>After Abe addresses the performance drop for Agilent Data Sets, share Abe's performance page from the wiki with Eve Shalley</t>
+  </si>
+  <si>
+    <t>Send Craig Fee the estimated dates for bringing caArray and caIntegrator back on line.</t>
+  </si>
+  <si>
+    <t>Follow up with Ann Wiley to find out what she needs from us to update the product landing page.</t>
+  </si>
+  <si>
+    <t>Meet to refine the audit log requirements. (Thursday: after 2:00)</t>
+  </si>
+  <si>
+    <t>Ulli Wagner, Mike Hunter, JJ Pan, Juli Klemm, Winston Cheng</t>
   </si>
 </sst>
 </file>
@@ -1347,8 +1359,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E122"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A95" workbookViewId="0">
-      <selection activeCell="A114" sqref="A114:E115"/>
+    <sheetView tabSelected="1" topLeftCell="A106" workbookViewId="0">
+      <selection activeCell="A117" sqref="A117:E117"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
@@ -3329,32 +3341,56 @@
         <v>155</v>
       </c>
     </row>
-    <row r="117" spans="1:5" ht="16" thickBot="1">
-      <c r="A117" s="11">
+    <row r="117" spans="1:5" ht="31" thickBot="1">
+      <c r="A117" s="8">
         <v>116</v>
       </c>
-      <c r="B117" s="17"/>
-      <c r="C117" s="17"/>
-      <c r="D117" s="18"/>
-      <c r="E117" s="17"/>
-    </row>
-    <row r="118" spans="1:5" ht="16" thickBot="1">
+      <c r="B117" s="9" t="s">
+        <v>205</v>
+      </c>
+      <c r="C117" s="9" t="s">
+        <v>149</v>
+      </c>
+      <c r="D117" s="10">
+        <v>40023</v>
+      </c>
+      <c r="E117" s="9" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="118" spans="1:5" ht="31" thickBot="1">
       <c r="A118" s="11">
         <v>117</v>
       </c>
-      <c r="B118" s="17"/>
-      <c r="C118" s="17"/>
-      <c r="D118" s="18"/>
-      <c r="E118" s="17"/>
+      <c r="B118" s="17" t="s">
+        <v>206</v>
+      </c>
+      <c r="C118" s="17" t="s">
+        <v>149</v>
+      </c>
+      <c r="D118" s="18">
+        <v>40023</v>
+      </c>
+      <c r="E118" s="17" t="s">
+        <v>155</v>
+      </c>
     </row>
     <row r="119" spans="1:5" ht="16" thickBot="1">
       <c r="A119" s="11">
         <v>118</v>
       </c>
-      <c r="B119" s="17"/>
-      <c r="C119" s="17"/>
-      <c r="D119" s="18"/>
-      <c r="E119" s="17"/>
+      <c r="B119" s="17" t="s">
+        <v>207</v>
+      </c>
+      <c r="C119" s="17" t="s">
+        <v>208</v>
+      </c>
+      <c r="D119" s="18">
+        <v>40023</v>
+      </c>
+      <c r="E119" s="17" t="s">
+        <v>155</v>
+      </c>
     </row>
     <row r="120" spans="1:5" ht="16" thickBot="1">
       <c r="A120" s="11">

</xml_diff>

<commit_message>
Updates for the weekly status meeting
</commit_message>
<xml_diff>
--- a/project_management/caArray_caIntegrator_Action_Items.xlsx
+++ b/project_management/caArray_caIntegrator_Action_Items.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="23515"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="23812"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="359" uniqueCount="209">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="398" uniqueCount="225">
   <si>
     <t>Make the following changes to the caArray project plan:
 * Add a task to re-run the Section 508 compliance scan for 2.5.0 to ensure we are above 90%.
@@ -712,6 +712,54 @@
   </si>
   <si>
     <t>Ulli Wagner, Mike Hunter, JJ Pan, Juli Klemm, Winston Cheng</t>
+  </si>
+  <si>
+    <t>Review feedback from TRANSCEND:  Address the changes (documentation, new features, improvements, bugs)</t>
+  </si>
+  <si>
+    <t>Review feedback from TRANSCEND: Address the performance and time-out issues - collect sample test files</t>
+  </si>
+  <si>
+    <t>Installation Guide Updates: Work with Jill and Dev Team to make sure that the installation guide is updated</t>
+  </si>
+  <si>
+    <t>Let Jill know what kind of links we use for the install documentation</t>
+  </si>
+  <si>
+    <t>Obsolete</t>
+  </si>
+  <si>
+    <t>Start providing a quick daily status email for caArray and caIntegrator until 2.5.1 and 1.4.1 go to Production</t>
+  </si>
+  <si>
+    <t>Identify the minimal requirements for the test plans for caArray 2.5.1 and caIntegrator 1.4.1 to get into QA.</t>
+  </si>
+  <si>
+    <t>Marina Omelchenko, Sudha, Preston Wood</t>
+  </si>
+  <si>
+    <t>Email the current status of the caArray POAM issues to JJ to ensure we're on track for all outstanding issues.</t>
+  </si>
+  <si>
+    <t>Send the SQL audit log script to Systems and JJ for a monthly cron job.</t>
+  </si>
+  <si>
+    <t>Winston Cheng</t>
+  </si>
+  <si>
+    <t>Determine the optimal records to keep as public for the caIntegrator appscan on STAGE.</t>
+  </si>
+  <si>
+    <t>Provide language and instructions to Jill for handling the 2.5.0 installation instructions.</t>
+  </si>
+  <si>
+    <t>Change Management Request #59 (Java 1.7) upgrade. Review and Respond.</t>
+  </si>
+  <si>
+    <t>Grid dependencies for caArray and caIntegrator. Review and Respond once Ulli has the official request.</t>
+  </si>
+  <si>
+    <t>Status update on the caArray QA tier. Jacob will forward  Shine, his latest communication with Winston.</t>
   </si>
 </sst>
 </file>
@@ -845,8 +893,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="63">
+  <cellStyleXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -967,7 +1019,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="63">
+  <cellStyles count="67">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -999,6 +1051,8 @@
     <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1030,6 +1084,8 @@
     <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1357,10 +1413,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E122"/>
+  <dimension ref="A1:E151"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A106" workbookViewId="0">
-      <selection activeCell="A117" sqref="A117:E117"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A128" sqref="A128:E132"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
@@ -3257,20 +3313,20 @@
       </c>
     </row>
     <row r="112" spans="1:5" ht="16" thickBot="1">
-      <c r="A112" s="11">
+      <c r="A112" s="8">
         <v>111</v>
       </c>
-      <c r="B112" s="17" t="s">
+      <c r="B112" s="9" t="s">
         <v>197</v>
       </c>
-      <c r="C112" s="17" t="s">
+      <c r="C112" s="9" t="s">
         <v>198</v>
       </c>
-      <c r="D112" s="18">
+      <c r="D112" s="10">
         <v>40009</v>
       </c>
-      <c r="E112" s="17" t="s">
-        <v>155</v>
+      <c r="E112" s="9" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="113" spans="1:5" ht="16" thickBot="1">
@@ -3325,20 +3381,20 @@
       </c>
     </row>
     <row r="116" spans="1:5" ht="31" thickBot="1">
-      <c r="A116" s="11">
+      <c r="A116" s="8">
         <v>115</v>
       </c>
-      <c r="B116" s="17" t="s">
+      <c r="B116" s="9" t="s">
         <v>204</v>
       </c>
-      <c r="C116" s="17" t="s">
+      <c r="C116" s="9" t="s">
         <v>149</v>
       </c>
-      <c r="D116" s="18">
+      <c r="D116" s="10">
         <v>40016</v>
       </c>
-      <c r="E116" s="17" t="s">
-        <v>155</v>
+      <c r="E116" s="9" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="117" spans="1:5" ht="31" thickBot="1">
@@ -3359,65 +3415,430 @@
       </c>
     </row>
     <row r="118" spans="1:5" ht="31" thickBot="1">
-      <c r="A118" s="11">
+      <c r="A118" s="8">
         <v>117</v>
       </c>
-      <c r="B118" s="17" t="s">
+      <c r="B118" s="9" t="s">
         <v>206</v>
       </c>
-      <c r="C118" s="17" t="s">
+      <c r="C118" s="9" t="s">
         <v>149</v>
       </c>
-      <c r="D118" s="18">
+      <c r="D118" s="10">
         <v>40023</v>
       </c>
-      <c r="E118" s="17" t="s">
-        <v>155</v>
+      <c r="E118" s="9" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="119" spans="1:5" ht="16" thickBot="1">
-      <c r="A119" s="11">
+      <c r="A119" s="8">
         <v>118</v>
       </c>
-      <c r="B119" s="17" t="s">
+      <c r="B119" s="9" t="s">
         <v>207</v>
       </c>
-      <c r="C119" s="17" t="s">
+      <c r="C119" s="9" t="s">
         <v>208</v>
       </c>
-      <c r="D119" s="18">
+      <c r="D119" s="10">
         <v>40023</v>
       </c>
-      <c r="E119" s="17" t="s">
-        <v>155</v>
+      <c r="E119" s="9" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="120" spans="1:5" ht="16" thickBot="1">
-      <c r="A120" s="11">
+      <c r="A120" s="8">
         <v>119</v>
       </c>
-      <c r="B120" s="17"/>
-      <c r="C120" s="17"/>
-      <c r="D120" s="18"/>
-      <c r="E120" s="17"/>
-    </row>
-    <row r="121" spans="1:5" ht="16" thickBot="1">
-      <c r="A121" s="11">
+      <c r="B120" s="9" t="s">
+        <v>222</v>
+      </c>
+      <c r="C120" s="9" t="s">
+        <v>173</v>
+      </c>
+      <c r="D120" s="10">
+        <v>40023</v>
+      </c>
+      <c r="E120" s="9" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="121" spans="1:5" ht="31" thickBot="1">
+      <c r="A121" s="8">
         <v>120</v>
       </c>
-      <c r="B121" s="17"/>
-      <c r="C121" s="17"/>
-      <c r="D121" s="18"/>
-      <c r="E121" s="17"/>
-    </row>
-    <row r="122" spans="1:5" ht="16" thickBot="1">
-      <c r="A122" s="11">
+      <c r="B121" s="9" t="s">
+        <v>223</v>
+      </c>
+      <c r="C121" s="9" t="s">
+        <v>173</v>
+      </c>
+      <c r="D121" s="10">
+        <v>40030</v>
+      </c>
+      <c r="E121" s="9" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="122" spans="1:5" ht="31" thickBot="1">
+      <c r="A122" s="8">
         <v>121</v>
       </c>
-      <c r="B122" s="17"/>
-      <c r="C122" s="17"/>
-      <c r="D122" s="18"/>
-      <c r="E122" s="17"/>
+      <c r="B122" s="9" t="s">
+        <v>224</v>
+      </c>
+      <c r="C122" s="9" t="s">
+        <v>173</v>
+      </c>
+      <c r="D122" s="10">
+        <v>40030</v>
+      </c>
+      <c r="E122" s="9" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="123" spans="1:5" ht="31" thickBot="1">
+      <c r="A123" s="11">
+        <v>122</v>
+      </c>
+      <c r="B123" s="17" t="s">
+        <v>209</v>
+      </c>
+      <c r="C123" s="17" t="s">
+        <v>173</v>
+      </c>
+      <c r="D123" s="18">
+        <v>40037</v>
+      </c>
+      <c r="E123" s="17" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="124" spans="1:5" ht="31" thickBot="1">
+      <c r="A124" s="11">
+        <v>123</v>
+      </c>
+      <c r="B124" s="17" t="s">
+        <v>210</v>
+      </c>
+      <c r="C124" s="17" t="s">
+        <v>173</v>
+      </c>
+      <c r="D124" s="18">
+        <v>40037</v>
+      </c>
+      <c r="E124" s="17" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="125" spans="1:5" ht="31" thickBot="1">
+      <c r="A125" s="8">
+        <v>124</v>
+      </c>
+      <c r="B125" s="9" t="s">
+        <v>211</v>
+      </c>
+      <c r="C125" s="9" t="s">
+        <v>173</v>
+      </c>
+      <c r="D125" s="10">
+        <v>40037</v>
+      </c>
+      <c r="E125" s="9" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="126" spans="1:5" ht="16" thickBot="1">
+      <c r="A126" s="8">
+        <v>125</v>
+      </c>
+      <c r="B126" s="9" t="s">
+        <v>212</v>
+      </c>
+      <c r="C126" s="9" t="s">
+        <v>149</v>
+      </c>
+      <c r="D126" s="10">
+        <v>40044</v>
+      </c>
+      <c r="E126" s="9" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="127" spans="1:5" ht="31" thickBot="1">
+      <c r="A127" s="11">
+        <v>126</v>
+      </c>
+      <c r="B127" s="17" t="s">
+        <v>214</v>
+      </c>
+      <c r="C127" s="17" t="s">
+        <v>173</v>
+      </c>
+      <c r="D127" s="18">
+        <v>40044</v>
+      </c>
+      <c r="E127" s="17" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="128" spans="1:5" ht="31" thickBot="1">
+      <c r="A128" s="8">
+        <v>127</v>
+      </c>
+      <c r="B128" s="9" t="s">
+        <v>215</v>
+      </c>
+      <c r="C128" s="9" t="s">
+        <v>216</v>
+      </c>
+      <c r="D128" s="10">
+        <v>40058</v>
+      </c>
+      <c r="E128" s="9" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="129" spans="1:5" ht="31" thickBot="1">
+      <c r="A129" s="8">
+        <v>128</v>
+      </c>
+      <c r="B129" s="9" t="s">
+        <v>217</v>
+      </c>
+      <c r="C129" s="9" t="s">
+        <v>149</v>
+      </c>
+      <c r="D129" s="10">
+        <v>40058</v>
+      </c>
+      <c r="E129" s="9" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="130" spans="1:5" ht="16" thickBot="1">
+      <c r="A130" s="8">
+        <v>129</v>
+      </c>
+      <c r="B130" s="9" t="s">
+        <v>218</v>
+      </c>
+      <c r="C130" s="9" t="s">
+        <v>219</v>
+      </c>
+      <c r="D130" s="10">
+        <v>40065</v>
+      </c>
+      <c r="E130" s="9" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="131" spans="1:5" ht="31" thickBot="1">
+      <c r="A131" s="8">
+        <v>130</v>
+      </c>
+      <c r="B131" s="9" t="s">
+        <v>220</v>
+      </c>
+      <c r="C131" s="9" t="s">
+        <v>200</v>
+      </c>
+      <c r="D131" s="10">
+        <v>40065</v>
+      </c>
+      <c r="E131" s="9" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="132" spans="1:5" ht="31" thickBot="1">
+      <c r="A132" s="8">
+        <v>131</v>
+      </c>
+      <c r="B132" s="9" t="s">
+        <v>221</v>
+      </c>
+      <c r="C132" s="9" t="s">
+        <v>143</v>
+      </c>
+      <c r="D132" s="10">
+        <v>40072</v>
+      </c>
+      <c r="E132" s="9" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="133" spans="1:5" ht="16" thickBot="1">
+      <c r="A133" s="11">
+        <v>132</v>
+      </c>
+      <c r="B133" s="17"/>
+      <c r="C133" s="17"/>
+      <c r="D133" s="18"/>
+      <c r="E133" s="17"/>
+    </row>
+    <row r="134" spans="1:5" ht="16" thickBot="1">
+      <c r="A134" s="11">
+        <v>133</v>
+      </c>
+      <c r="B134" s="17"/>
+      <c r="C134" s="17"/>
+      <c r="D134" s="18"/>
+      <c r="E134" s="17"/>
+    </row>
+    <row r="135" spans="1:5" ht="16" thickBot="1">
+      <c r="A135" s="11">
+        <v>134</v>
+      </c>
+      <c r="B135" s="17"/>
+      <c r="C135" s="17"/>
+      <c r="D135" s="18"/>
+      <c r="E135" s="17"/>
+    </row>
+    <row r="136" spans="1:5" ht="16" thickBot="1">
+      <c r="A136" s="11">
+        <v>135</v>
+      </c>
+      <c r="B136" s="17"/>
+      <c r="C136" s="17"/>
+      <c r="D136" s="18"/>
+      <c r="E136" s="17"/>
+    </row>
+    <row r="137" spans="1:5" ht="16" thickBot="1">
+      <c r="A137" s="11">
+        <v>136</v>
+      </c>
+      <c r="B137" s="17"/>
+      <c r="C137" s="17"/>
+      <c r="D137" s="18"/>
+      <c r="E137" s="17"/>
+    </row>
+    <row r="138" spans="1:5" ht="16" thickBot="1">
+      <c r="A138" s="11">
+        <v>137</v>
+      </c>
+      <c r="B138" s="17"/>
+      <c r="C138" s="17"/>
+      <c r="D138" s="18"/>
+      <c r="E138" s="17"/>
+    </row>
+    <row r="139" spans="1:5" ht="16" thickBot="1">
+      <c r="A139" s="11">
+        <v>138</v>
+      </c>
+      <c r="B139" s="17"/>
+      <c r="C139" s="17"/>
+      <c r="D139" s="18"/>
+      <c r="E139" s="17"/>
+    </row>
+    <row r="140" spans="1:5" ht="16" thickBot="1">
+      <c r="A140" s="11">
+        <v>139</v>
+      </c>
+      <c r="B140" s="17"/>
+      <c r="C140" s="17"/>
+      <c r="D140" s="18"/>
+      <c r="E140" s="17"/>
+    </row>
+    <row r="141" spans="1:5" ht="16" thickBot="1">
+      <c r="A141" s="11">
+        <v>140</v>
+      </c>
+      <c r="B141" s="17"/>
+      <c r="C141" s="17"/>
+      <c r="D141" s="18"/>
+      <c r="E141" s="17"/>
+    </row>
+    <row r="142" spans="1:5" ht="16" thickBot="1">
+      <c r="A142" s="11">
+        <v>141</v>
+      </c>
+      <c r="B142" s="17"/>
+      <c r="C142" s="17"/>
+      <c r="D142" s="18"/>
+      <c r="E142" s="17"/>
+    </row>
+    <row r="143" spans="1:5" ht="16" thickBot="1">
+      <c r="A143" s="11">
+        <v>142</v>
+      </c>
+      <c r="B143" s="17"/>
+      <c r="C143" s="17"/>
+      <c r="D143" s="18"/>
+      <c r="E143" s="17"/>
+    </row>
+    <row r="144" spans="1:5" ht="16" thickBot="1">
+      <c r="A144" s="11">
+        <v>143</v>
+      </c>
+      <c r="B144" s="17"/>
+      <c r="C144" s="17"/>
+      <c r="D144" s="18"/>
+      <c r="E144" s="17"/>
+    </row>
+    <row r="145" spans="1:5" ht="16" thickBot="1">
+      <c r="A145" s="11">
+        <v>144</v>
+      </c>
+      <c r="B145" s="17"/>
+      <c r="C145" s="17"/>
+      <c r="D145" s="18"/>
+      <c r="E145" s="17"/>
+    </row>
+    <row r="146" spans="1:5" ht="16" thickBot="1">
+      <c r="A146" s="11">
+        <v>145</v>
+      </c>
+      <c r="B146" s="17"/>
+      <c r="C146" s="17"/>
+      <c r="D146" s="18"/>
+      <c r="E146" s="17"/>
+    </row>
+    <row r="147" spans="1:5" ht="16" thickBot="1">
+      <c r="A147" s="11">
+        <v>146</v>
+      </c>
+      <c r="B147" s="17"/>
+      <c r="C147" s="17"/>
+      <c r="D147" s="18"/>
+      <c r="E147" s="17"/>
+    </row>
+    <row r="148" spans="1:5" ht="16" thickBot="1">
+      <c r="A148" s="11">
+        <v>147</v>
+      </c>
+      <c r="B148" s="17"/>
+      <c r="C148" s="17"/>
+      <c r="D148" s="18"/>
+      <c r="E148" s="17"/>
+    </row>
+    <row r="149" spans="1:5" ht="16" thickBot="1">
+      <c r="A149" s="11">
+        <v>148</v>
+      </c>
+      <c r="B149" s="17"/>
+      <c r="C149" s="17"/>
+      <c r="D149" s="18"/>
+      <c r="E149" s="17"/>
+    </row>
+    <row r="150" spans="1:5" ht="16" thickBot="1">
+      <c r="A150" s="11">
+        <v>149</v>
+      </c>
+      <c r="B150" s="17"/>
+      <c r="C150" s="17"/>
+      <c r="D150" s="18"/>
+      <c r="E150" s="17"/>
+    </row>
+    <row r="151" spans="1:5" ht="16" thickBot="1">
+      <c r="A151" s="11">
+        <v>150</v>
+      </c>
+      <c r="B151" s="17"/>
+      <c r="C151" s="17"/>
+      <c r="D151" s="18"/>
+      <c r="E151" s="17"/>
     </row>
   </sheetData>
   <sortState ref="A2:H13">

</xml_diff>

<commit_message>
updated with recent data
</commit_message>
<xml_diff>
--- a/project_management/caArray_caIntegrator_Action_Items.xlsx
+++ b/project_management/caArray_caIntegrator_Action_Items.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="23812"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="23913"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28680" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Action_Items" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="398" uniqueCount="225">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="401" uniqueCount="227">
   <si>
     <t>Make the following changes to the caArray project plan:
 * Add a task to re-run the Section 508 compliance scan for 2.5.0 to ensure we are above 90%.
@@ -552,9 +552,6 @@
     <t>Abe Evans-El</t>
   </si>
   <si>
-    <t>Assigned</t>
-  </si>
-  <si>
     <t>Request gitHub integration with AntHill Pro on caIntegrator PRODUCTION tier.</t>
   </si>
   <si>
@@ -760,13 +757,22 @@
   </si>
   <si>
     <t>Status update on the caArray QA tier. Jacob will forward  Shine, his latest communication with Winston.</t>
+  </si>
+  <si>
+    <t>Complete (Not required)</t>
+  </si>
+  <si>
+    <t>Check in with Sudha to find out why the peer review for caIntegrator's Test Plan took longer than a week</t>
+  </si>
+  <si>
+    <t>Preston Wood</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Verdana"/>
@@ -804,6 +810,12 @@
       <sz val="10"/>
       <color theme="11"/>
       <name val="Verdana"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF333333"/>
+      <name val="Cambria"/>
+      <scheme val="major"/>
     </font>
   </fonts>
   <fills count="5">
@@ -962,7 +974,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1017,6 +1029,9 @@
     </xf>
     <xf numFmtId="14" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="67">
@@ -1416,13 +1431,14 @@
   <dimension ref="A1:E151"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A128" sqref="A128:E132"/>
+      <pane ySplit="1" topLeftCell="A120" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C137" sqref="C137"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="7" style="1" customWidth="1"/>
-    <col min="2" max="2" width="57.85546875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="62.140625" style="1" customWidth="1"/>
     <col min="3" max="3" width="47.140625" style="1" customWidth="1"/>
     <col min="4" max="4" width="15.42578125" style="1" customWidth="1"/>
     <col min="5" max="5" width="51.42578125" style="1" customWidth="1"/>
@@ -1480,7 +1496,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="31" thickBot="1">
+    <row r="4" spans="1:5" ht="16" thickBot="1">
       <c r="A4" s="5">
         <v>3</v>
       </c>
@@ -1616,7 +1632,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="31" thickBot="1">
+    <row r="12" spans="1:5" ht="16" thickBot="1">
       <c r="A12" s="5">
         <v>11</v>
       </c>
@@ -2041,7 +2057,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="37" spans="1:5" ht="31" thickBot="1">
+    <row r="37" spans="1:5" ht="16" thickBot="1">
       <c r="A37" s="8">
         <v>36</v>
       </c>
@@ -2126,7 +2142,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="42" spans="1:5" ht="31" thickBot="1">
+    <row r="42" spans="1:5" ht="16" thickBot="1">
       <c r="A42" s="8">
         <v>41</v>
       </c>
@@ -2517,7 +2533,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="65" spans="1:5" ht="31" thickBot="1">
+    <row r="65" spans="1:5" ht="16" thickBot="1">
       <c r="A65" s="8">
         <v>64</v>
       </c>
@@ -2551,7 +2567,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="67" spans="1:5" ht="31" thickBot="1">
+    <row r="67" spans="1:5" ht="16" thickBot="1">
       <c r="A67" s="8">
         <v>66</v>
       </c>
@@ -2634,7 +2650,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="72" spans="1:5" ht="31" thickBot="1">
+    <row r="72" spans="1:5" ht="16" thickBot="1">
       <c r="A72" s="8">
         <v>71</v>
       </c>
@@ -2785,12 +2801,12 @@
         <v>39</v>
       </c>
     </row>
-    <row r="81" spans="1:5" ht="31" thickBot="1">
+    <row r="81" spans="1:5" ht="16" thickBot="1">
       <c r="A81" s="8">
         <v>80</v>
       </c>
       <c r="B81" s="9" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C81" s="9" t="s">
         <v>154</v>
@@ -2807,7 +2823,7 @@
         <v>81</v>
       </c>
       <c r="B82" s="9" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C82" s="9" t="s">
         <v>149</v>
@@ -2824,7 +2840,7 @@
         <v>82</v>
       </c>
       <c r="B83" s="9" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C83" s="9" t="s">
         <v>149</v>
@@ -2841,7 +2857,7 @@
         <v>83</v>
       </c>
       <c r="B84" s="9" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C84" s="9" t="s">
         <v>149</v>
@@ -2858,7 +2874,7 @@
         <v>84</v>
       </c>
       <c r="B85" s="9" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C85" s="9" t="s">
         <v>149</v>
@@ -2875,7 +2891,7 @@
         <v>85</v>
       </c>
       <c r="B86" s="9" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C86" s="9" t="s">
         <v>149</v>
@@ -2884,7 +2900,7 @@
         <v>39946</v>
       </c>
       <c r="E86" s="9" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="87" spans="1:5" ht="31" thickBot="1">
@@ -2892,7 +2908,7 @@
         <v>86</v>
       </c>
       <c r="B87" s="9" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C87" s="9" t="s">
         <v>134</v>
@@ -2909,10 +2925,10 @@
         <v>87</v>
       </c>
       <c r="B88" s="9" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C88" s="9" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D88" s="10">
         <v>39953</v>
@@ -2926,7 +2942,7 @@
         <v>88</v>
       </c>
       <c r="B89" s="9" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C89" s="9" t="s">
         <v>149</v>
@@ -2943,10 +2959,10 @@
         <v>89</v>
       </c>
       <c r="B90" s="9" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C90" s="9" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D90" s="10">
         <v>39960</v>
@@ -2960,7 +2976,7 @@
         <v>90</v>
       </c>
       <c r="B91" s="9" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C91" s="9" t="s">
         <v>149</v>
@@ -2977,7 +2993,7 @@
         <v>91</v>
       </c>
       <c r="B92" s="9" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C92" s="9" t="s">
         <v>149</v>
@@ -2994,10 +3010,10 @@
         <v>92</v>
       </c>
       <c r="B93" s="9" t="s">
+        <v>169</v>
+      </c>
+      <c r="C93" s="9" t="s">
         <v>170</v>
-      </c>
-      <c r="C93" s="9" t="s">
-        <v>171</v>
       </c>
       <c r="D93" s="10">
         <v>39967</v>
@@ -3011,7 +3027,7 @@
         <v>93</v>
       </c>
       <c r="B94" s="9" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C94" s="9" t="s">
         <v>149</v>
@@ -3023,15 +3039,15 @@
         <v>39</v>
       </c>
     </row>
-    <row r="95" spans="1:5" ht="31" thickBot="1">
+    <row r="95" spans="1:5" ht="16" thickBot="1">
       <c r="A95" s="8">
         <v>94</v>
       </c>
       <c r="B95" s="9" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C95" s="9" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D95" s="10">
         <v>39967</v>
@@ -3045,10 +3061,10 @@
         <v>95</v>
       </c>
       <c r="B96" s="9" t="s">
+        <v>174</v>
+      </c>
+      <c r="C96" s="9" t="s">
         <v>175</v>
-      </c>
-      <c r="C96" s="9" t="s">
-        <v>176</v>
       </c>
       <c r="D96" s="10">
         <v>39974</v>
@@ -3062,7 +3078,7 @@
         <v>96</v>
       </c>
       <c r="B97" s="9" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C97" s="9" t="s">
         <v>149</v>
@@ -3079,7 +3095,7 @@
         <v>97</v>
       </c>
       <c r="B98" s="9" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C98" s="9" t="s">
         <v>149</v>
@@ -3096,7 +3112,7 @@
         <v>98</v>
       </c>
       <c r="B99" s="9" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C99" s="9" t="s">
         <v>59</v>
@@ -3108,21 +3124,21 @@
         <v>39</v>
       </c>
     </row>
-    <row r="100" spans="1:5" ht="31" thickBot="1">
-      <c r="A100" s="11">
+    <row r="100" spans="1:5" ht="16" thickBot="1">
+      <c r="A100" s="15">
         <v>99</v>
       </c>
-      <c r="B100" s="17" t="s">
-        <v>181</v>
-      </c>
-      <c r="C100" s="17" t="s">
+      <c r="B100" s="13" t="s">
+        <v>180</v>
+      </c>
+      <c r="C100" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="D100" s="18">
+      <c r="D100" s="14">
         <v>39981</v>
       </c>
-      <c r="E100" s="17" t="s">
-        <v>155</v>
+      <c r="E100" s="13" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="101" spans="1:5" ht="31" thickBot="1">
@@ -3130,10 +3146,10 @@
         <v>100</v>
       </c>
       <c r="B101" s="9" t="s">
+        <v>181</v>
+      </c>
+      <c r="C101" s="9" t="s">
         <v>182</v>
-      </c>
-      <c r="C101" s="9" t="s">
-        <v>183</v>
       </c>
       <c r="D101" s="10">
         <v>39981</v>
@@ -3147,7 +3163,7 @@
         <v>101</v>
       </c>
       <c r="B102" s="9" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C102" s="9" t="s">
         <v>149</v>
@@ -3164,10 +3180,10 @@
         <v>102</v>
       </c>
       <c r="B103" s="9" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C103" s="9" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D103" s="10">
         <v>39988</v>
@@ -3177,37 +3193,37 @@
       </c>
     </row>
     <row r="104" spans="1:5" ht="16" thickBot="1">
-      <c r="A104" s="11">
+      <c r="A104" s="15">
         <v>103</v>
       </c>
-      <c r="B104" s="17" t="s">
-        <v>186</v>
-      </c>
-      <c r="C104" s="17" t="s">
+      <c r="B104" s="13" t="s">
+        <v>185</v>
+      </c>
+      <c r="C104" s="13" t="s">
         <v>134</v>
       </c>
-      <c r="D104" s="18">
+      <c r="D104" s="14">
         <v>39988</v>
       </c>
-      <c r="E104" s="17" t="s">
-        <v>155</v>
+      <c r="E104" s="13" t="s">
+        <v>224</v>
       </c>
     </row>
     <row r="105" spans="1:5" ht="16" thickBot="1">
-      <c r="A105" s="11">
+      <c r="A105" s="15">
         <v>104</v>
       </c>
-      <c r="B105" s="17" t="s">
+      <c r="B105" s="13" t="s">
+        <v>187</v>
+      </c>
+      <c r="C105" s="13" t="s">
         <v>188</v>
       </c>
-      <c r="C105" s="17" t="s">
-        <v>189</v>
-      </c>
-      <c r="D105" s="18">
+      <c r="D105" s="14">
         <v>39988</v>
       </c>
-      <c r="E105" s="17" t="s">
-        <v>155</v>
+      <c r="E105" s="13" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="106" spans="1:5" ht="31" thickBot="1">
@@ -3215,7 +3231,7 @@
         <v>105</v>
       </c>
       <c r="B106" s="9" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C106" s="9" t="s">
         <v>149</v>
@@ -3232,10 +3248,10 @@
         <v>106</v>
       </c>
       <c r="B107" s="9" t="s">
+        <v>190</v>
+      </c>
+      <c r="C107" s="9" t="s">
         <v>191</v>
-      </c>
-      <c r="C107" s="9" t="s">
-        <v>192</v>
       </c>
       <c r="D107" s="10">
         <v>40002</v>
@@ -3249,7 +3265,7 @@
         <v>107</v>
       </c>
       <c r="B108" s="9" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C108" s="9" t="s">
         <v>59</v>
@@ -3266,7 +3282,7 @@
         <v>108</v>
       </c>
       <c r="B109" s="9" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C109" s="9" t="s">
         <v>149</v>
@@ -3278,21 +3294,21 @@
         <v>39</v>
       </c>
     </row>
-    <row r="110" spans="1:5" ht="31" thickBot="1">
-      <c r="A110" s="11">
+    <row r="110" spans="1:5" ht="16" thickBot="1">
+      <c r="A110" s="15">
         <v>109</v>
       </c>
-      <c r="B110" s="17" t="s">
-        <v>194</v>
-      </c>
-      <c r="C110" s="17" t="s">
+      <c r="B110" s="13" t="s">
+        <v>193</v>
+      </c>
+      <c r="C110" s="13" t="s">
         <v>143</v>
       </c>
-      <c r="D110" s="18">
+      <c r="D110" s="14">
         <v>40009</v>
       </c>
-      <c r="E110" s="17" t="s">
-        <v>152</v>
+      <c r="E110" s="13" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="111" spans="1:5" ht="16" thickBot="1">
@@ -3300,7 +3316,7 @@
         <v>110</v>
       </c>
       <c r="B111" s="9" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C111" s="9" t="s">
         <v>149</v>
@@ -3317,10 +3333,10 @@
         <v>111</v>
       </c>
       <c r="B112" s="9" t="s">
+        <v>196</v>
+      </c>
+      <c r="C112" s="9" t="s">
         <v>197</v>
-      </c>
-      <c r="C112" s="9" t="s">
-        <v>198</v>
       </c>
       <c r="D112" s="10">
         <v>40009</v>
@@ -3334,10 +3350,10 @@
         <v>112</v>
       </c>
       <c r="B113" s="9" t="s">
+        <v>198</v>
+      </c>
+      <c r="C113" s="9" t="s">
         <v>199</v>
-      </c>
-      <c r="C113" s="9" t="s">
-        <v>200</v>
       </c>
       <c r="D113" s="10">
         <v>40009</v>
@@ -3351,7 +3367,7 @@
         <v>113</v>
       </c>
       <c r="B114" s="9" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C114" s="9" t="s">
         <v>59</v>
@@ -3368,10 +3384,10 @@
         <v>114</v>
       </c>
       <c r="B115" s="9" t="s">
+        <v>201</v>
+      </c>
+      <c r="C115" s="9" t="s">
         <v>202</v>
-      </c>
-      <c r="C115" s="9" t="s">
-        <v>203</v>
       </c>
       <c r="D115" s="10">
         <v>40016</v>
@@ -3385,7 +3401,7 @@
         <v>115</v>
       </c>
       <c r="B116" s="9" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C116" s="9" t="s">
         <v>149</v>
@@ -3402,7 +3418,7 @@
         <v>116</v>
       </c>
       <c r="B117" s="9" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C117" s="9" t="s">
         <v>149</v>
@@ -3419,7 +3435,7 @@
         <v>117</v>
       </c>
       <c r="B118" s="9" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C118" s="9" t="s">
         <v>149</v>
@@ -3436,10 +3452,10 @@
         <v>118</v>
       </c>
       <c r="B119" s="9" t="s">
+        <v>206</v>
+      </c>
+      <c r="C119" s="9" t="s">
         <v>207</v>
-      </c>
-      <c r="C119" s="9" t="s">
-        <v>208</v>
       </c>
       <c r="D119" s="10">
         <v>40023</v>
@@ -3453,10 +3469,10 @@
         <v>119</v>
       </c>
       <c r="B120" s="9" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C120" s="9" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D120" s="10">
         <v>40023</v>
@@ -3470,10 +3486,10 @@
         <v>120</v>
       </c>
       <c r="B121" s="9" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C121" s="9" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D121" s="10">
         <v>40030</v>
@@ -3487,10 +3503,10 @@
         <v>121</v>
       </c>
       <c r="B122" s="9" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C122" s="9" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D122" s="10">
         <v>40030</v>
@@ -3504,10 +3520,10 @@
         <v>122</v>
       </c>
       <c r="B123" s="17" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C123" s="17" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D123" s="18">
         <v>40037</v>
@@ -3521,10 +3537,10 @@
         <v>123</v>
       </c>
       <c r="B124" s="17" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C124" s="17" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D124" s="18">
         <v>40037</v>
@@ -3538,10 +3554,10 @@
         <v>124</v>
       </c>
       <c r="B125" s="9" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C125" s="9" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D125" s="10">
         <v>40037</v>
@@ -3555,7 +3571,7 @@
         <v>125</v>
       </c>
       <c r="B126" s="9" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C126" s="9" t="s">
         <v>149</v>
@@ -3564,24 +3580,24 @@
         <v>40044</v>
       </c>
       <c r="E126" s="9" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="127" spans="1:5" ht="31" thickBot="1">
+      <c r="A127" s="15">
+        <v>126</v>
+      </c>
+      <c r="B127" s="13" t="s">
         <v>213</v>
       </c>
-    </row>
-    <row r="127" spans="1:5" ht="31" thickBot="1">
-      <c r="A127" s="11">
-        <v>126</v>
-      </c>
-      <c r="B127" s="17" t="s">
-        <v>214</v>
-      </c>
-      <c r="C127" s="17" t="s">
-        <v>173</v>
-      </c>
-      <c r="D127" s="18">
+      <c r="C127" s="13" t="s">
+        <v>172</v>
+      </c>
+      <c r="D127" s="14">
         <v>40044</v>
       </c>
-      <c r="E127" s="17" t="s">
-        <v>152</v>
+      <c r="E127" s="13" t="s">
+        <v>212</v>
       </c>
     </row>
     <row r="128" spans="1:5" ht="31" thickBot="1">
@@ -3589,10 +3605,10 @@
         <v>127</v>
       </c>
       <c r="B128" s="9" t="s">
+        <v>214</v>
+      </c>
+      <c r="C128" s="9" t="s">
         <v>215</v>
-      </c>
-      <c r="C128" s="9" t="s">
-        <v>216</v>
       </c>
       <c r="D128" s="10">
         <v>40058</v>
@@ -3606,7 +3622,7 @@
         <v>128</v>
       </c>
       <c r="B129" s="9" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C129" s="9" t="s">
         <v>149</v>
@@ -3615,7 +3631,7 @@
         <v>40058</v>
       </c>
       <c r="E129" s="9" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="130" spans="1:5" ht="16" thickBot="1">
@@ -3623,10 +3639,10 @@
         <v>129</v>
       </c>
       <c r="B130" s="9" t="s">
+        <v>217</v>
+      </c>
+      <c r="C130" s="9" t="s">
         <v>218</v>
-      </c>
-      <c r="C130" s="9" t="s">
-        <v>219</v>
       </c>
       <c r="D130" s="10">
         <v>40065</v>
@@ -3640,16 +3656,16 @@
         <v>130</v>
       </c>
       <c r="B131" s="9" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C131" s="9" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D131" s="10">
         <v>40065</v>
       </c>
       <c r="E131" s="9" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="132" spans="1:5" ht="31" thickBot="1">
@@ -3657,7 +3673,7 @@
         <v>131</v>
       </c>
       <c r="B132" s="9" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C132" s="9" t="s">
         <v>143</v>
@@ -3669,14 +3685,22 @@
         <v>39</v>
       </c>
     </row>
-    <row r="133" spans="1:5" ht="16" thickBot="1">
+    <row r="133" spans="1:5" ht="31" thickBot="1">
       <c r="A133" s="11">
         <v>132</v>
       </c>
-      <c r="B133" s="17"/>
-      <c r="C133" s="17"/>
-      <c r="D133" s="18"/>
-      <c r="E133" s="17"/>
+      <c r="B133" s="19" t="s">
+        <v>225</v>
+      </c>
+      <c r="C133" s="17" t="s">
+        <v>226</v>
+      </c>
+      <c r="D133" s="18">
+        <v>40128</v>
+      </c>
+      <c r="E133" s="17" t="s">
+        <v>152</v>
+      </c>
     </row>
     <row r="134" spans="1:5" ht="16" thickBot="1">
       <c r="A134" s="11">

</xml_diff>

<commit_message>
marked 2 actions items as complete
</commit_message>
<xml_diff>
--- a/project_management/caArray_caIntegrator_Action_Items.xlsx
+++ b/project_management/caArray_caIntegrator_Action_Items.xlsx
@@ -1431,8 +1431,8 @@
   <dimension ref="A1:E151"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A120" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C137" sqref="C137"/>
+      <pane ySplit="1" topLeftCell="A127" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B129" sqref="B129"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
@@ -3516,37 +3516,37 @@
       </c>
     </row>
     <row r="123" spans="1:5" ht="31" thickBot="1">
-      <c r="A123" s="11">
+      <c r="A123" s="15">
         <v>122</v>
       </c>
-      <c r="B123" s="17" t="s">
+      <c r="B123" s="13" t="s">
         <v>208</v>
       </c>
-      <c r="C123" s="17" t="s">
+      <c r="C123" s="13" t="s">
         <v>172</v>
       </c>
-      <c r="D123" s="18">
+      <c r="D123" s="14">
         <v>40037</v>
       </c>
-      <c r="E123" s="17" t="s">
-        <v>152</v>
+      <c r="E123" s="13" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="124" spans="1:5" ht="31" thickBot="1">
-      <c r="A124" s="11">
+      <c r="A124" s="15">
         <v>123</v>
       </c>
-      <c r="B124" s="17" t="s">
+      <c r="B124" s="13" t="s">
         <v>209</v>
       </c>
-      <c r="C124" s="17" t="s">
+      <c r="C124" s="13" t="s">
         <v>172</v>
       </c>
-      <c r="D124" s="18">
+      <c r="D124" s="14">
         <v>40037</v>
       </c>
-      <c r="E124" s="17" t="s">
-        <v>152</v>
+      <c r="E124" s="13" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="125" spans="1:5" ht="31" thickBot="1">

</xml_diff>